<commit_message>
added dsg adn desc and captured full data state
</commit_message>
<xml_diff>
--- a/docs/invoice.xlsx
+++ b/docs/invoice.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot;-&quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="31">
     <font>
       <name val="Arial"/>
       <color indexed="8"/>
@@ -80,12 +80,6 @@
     </font>
     <font>
       <name val="Roboto"/>
-      <b val="1"/>
-      <color indexed="13"/>
-      <sz val="9"/>
-    </font>
-    <font>
-      <name val="Roboto"/>
       <color indexed="8"/>
       <sz val="9"/>
     </font>
@@ -110,12 +104,6 @@
       <name val="Roboto"/>
       <b val="1"/>
       <color indexed="8"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Roboto"/>
-      <b val="1"/>
-      <color indexed="8"/>
       <sz val="9"/>
     </font>
     <font>
@@ -128,8 +116,89 @@
       <color theme="2" tint="0.7999816888943144"/>
       <sz val="10"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color indexed="8"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <charset val="1"/>
+      <b val="1"/>
+      <color rgb="FF1F3864"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <charset val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <charset val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <b val="1"/>
+      <color indexed="13"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color indexed="8"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Helvetica"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color indexed="8"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Helvetica"/>
+      <family val="2"/>
+      <color indexed="8"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Helvetica"/>
+      <family val="2"/>
+      <color indexed="8"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <color indexed="17"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <b val="1"/>
+      <color rgb="FF1F3864"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <b val="1"/>
+      <color indexed="15"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -160,8 +229,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -240,28 +315,6 @@
       <top style="thin">
         <color indexed="16"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -309,7 +362,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -317,36 +370,76 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="16"/>
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color theme="3"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
+      <top/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color theme="3"/>
       </left>
       <right/>
       <top/>
@@ -356,22 +449,223 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="medium">
+        <color theme="3"/>
+      </top>
+      <bottom style="medium">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color theme="3"/>
       </bottom>
       <diagonal/>
     </border>
@@ -379,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -410,27 +704,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -449,99 +725,46 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="11" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="11" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="4" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="12" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="11" fillId="5" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -554,45 +777,216 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="11" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="22" fillId="5" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="22" fillId="5" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="30" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="32"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1719,46 +2113,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="50" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="87" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="4.33203125" customWidth="1" style="70" min="1" max="1"/>
-    <col width="35.1640625" customWidth="1" style="70" min="2" max="2"/>
-    <col width="35.6640625" customWidth="1" style="70" min="3" max="3"/>
-    <col width="34" customWidth="1" style="70" min="4" max="4"/>
-    <col width="14.83203125" customWidth="1" style="70" min="5" max="6"/>
-    <col width="14.33203125" customWidth="1" style="70" min="7" max="7"/>
-    <col width="14.83203125" customWidth="1" style="70" min="8" max="9"/>
-    <col width="9.1640625" customWidth="1" style="70" min="10" max="10"/>
-    <col width="7.5" customWidth="1" style="70" min="11" max="11"/>
-    <col width="8.83203125" customWidth="1" style="70" min="12" max="12"/>
-    <col width="14.33203125" customWidth="1" style="70" min="13" max="13"/>
-    <col width="4" customWidth="1" style="70" min="14" max="14"/>
-    <col width="17.33203125" customWidth="1" style="70" min="15" max="16"/>
+    <col width="4.33203125" customWidth="1" style="107" min="1" max="1"/>
+    <col width="11.6640625" customWidth="1" style="107" min="2" max="2"/>
+    <col width="28.6640625" customWidth="1" style="107" min="3" max="3"/>
+    <col width="34" customWidth="1" style="107" min="4" max="4"/>
+    <col width="14.83203125" customWidth="1" style="107" min="5" max="5"/>
+    <col width="9" customWidth="1" style="107" min="6" max="6"/>
+    <col width="10.1640625" customWidth="1" style="107" min="7" max="7"/>
+    <col width="9.1640625" customWidth="1" style="107" min="8" max="8"/>
+    <col width="8.83203125" customWidth="1" style="107" min="9" max="9"/>
+    <col width="6.6640625" customWidth="1" style="107" min="10" max="10"/>
+    <col width="7.6640625" customWidth="1" style="107" min="11" max="11"/>
+    <col width="8.83203125" customWidth="1" style="107" min="12" max="12"/>
+    <col width="13.5" customWidth="1" style="107" min="13" max="13"/>
+    <col width="3.5" customWidth="1" style="107" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="70">
+    <row r="1" ht="14.25" customHeight="1" s="107">
       <c r="A1" s="1" t="n"/>
-      <c r="B1" s="60" t="n"/>
-      <c r="C1" s="61" t="n"/>
-      <c r="D1" s="61" t="n"/>
-      <c r="E1" s="61" t="n"/>
-      <c r="F1" s="61" t="n"/>
-      <c r="G1" s="61" t="n"/>
-      <c r="H1" s="61" t="n"/>
-      <c r="I1" s="61" t="n"/>
-      <c r="J1" s="61" t="n"/>
-      <c r="K1" s="61" t="n"/>
-      <c r="L1" s="61" t="n"/>
-      <c r="M1" s="62" t="n"/>
-      <c r="N1" s="63" t="n"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1" s="70">
+      <c r="B1" s="33" t="n"/>
+      <c r="C1" s="34" t="n"/>
+      <c r="D1" s="34" t="n"/>
+      <c r="E1" s="34" t="n"/>
+      <c r="F1" s="34" t="n"/>
+      <c r="G1" s="34" t="n"/>
+      <c r="H1" s="34" t="n"/>
+      <c r="I1" s="34" t="n"/>
+      <c r="J1" s="34" t="n"/>
+      <c r="K1" s="34" t="n"/>
+      <c r="L1" s="34" t="n"/>
+      <c r="M1" s="35" t="n"/>
+      <c r="N1" s="36" t="n"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1" s="107">
       <c r="A2" s="2" t="n"/>
       <c r="B2" s="3" t="n"/>
       <c r="C2" s="4" t="n"/>
@@ -1774,813 +2169,869 @@
       <c r="M2" s="5" t="n"/>
       <c r="N2" s="6" t="n"/>
     </row>
-    <row r="3" ht="109" customHeight="1" s="70">
+    <row r="3" ht="73" customHeight="1" s="107" thickBot="1">
       <c r="A3" s="7" t="n"/>
-      <c r="B3" s="67" t="inlineStr">
+      <c r="B3" s="104" t="inlineStr">
         <is>
           <t>Manufacturer Packaging Slip</t>
         </is>
       </c>
-      <c r="C3" s="8" t="n"/>
-      <c r="D3" s="8" t="n"/>
-      <c r="E3" s="9" t="n"/>
-      <c r="F3" s="9" t="n"/>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="9" t="n"/>
-      <c r="I3" s="9" t="n"/>
-      <c r="J3" s="9" t="n"/>
       <c r="K3" s="9" t="n"/>
       <c r="L3" s="9" t="n"/>
-      <c r="M3" s="10" t="inlineStr">
-        <is>
-          <t>&lt;Your Log</t>
-        </is>
+      <c r="M3" s="10" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="N3" s="11" t="n"/>
     </row>
-    <row r="4" ht="18" customHeight="1" s="70">
+    <row r="4" ht="18" customHeight="1" s="107">
       <c r="A4" s="7" t="n"/>
-      <c r="B4" s="12" t="inlineStr">
-        <is>
-          <t>Account</t>
-        </is>
-      </c>
-      <c r="C4" s="13" t="n"/>
-      <c r="D4" s="66" t="n"/>
-      <c r="E4" s="8" t="n"/>
-      <c r="F4" s="8" t="n"/>
-      <c r="G4" s="8" t="n"/>
-      <c r="H4" s="8" t="n"/>
-      <c r="I4" s="8" t="n"/>
-      <c r="J4" s="8" t="n"/>
-      <c r="K4" s="8" t="n"/>
-      <c r="L4" s="8" t="n"/>
-      <c r="M4" s="14" t="inlineStr">
-        <is>
-          <t>Quick Returns</t>
-        </is>
-      </c>
-      <c r="N4" s="15" t="n"/>
-    </row>
-    <row r="5" ht="18" customHeight="1" s="70">
+      <c r="B4" s="70" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="D4" s="113" t="n"/>
+      <c r="E4" s="114" t="n"/>
+      <c r="F4" s="114" t="n"/>
+      <c r="G4" s="114" t="n"/>
+      <c r="H4" s="115" t="n"/>
+      <c r="I4" s="82" t="n"/>
+      <c r="J4" s="82" t="n"/>
+      <c r="K4" s="82" t="n"/>
+      <c r="L4" s="116" t="inlineStr">
+        <is>
+          <t>INVOICE NO:</t>
+        </is>
+      </c>
+      <c r="M4" s="117" t="n"/>
+      <c r="N4" s="12" t="n"/>
+    </row>
+    <row r="5" ht="18" customHeight="1" s="107" thickBot="1">
       <c r="A5" s="7" t="n"/>
-      <c r="B5" s="16" t="inlineStr">
+      <c r="B5" s="71" t="inlineStr">
+        <is>
+          <t>01/12/2024</t>
+        </is>
+      </c>
+      <c r="D5" s="118" t="n"/>
+      <c r="E5" s="119" t="n"/>
+      <c r="F5" s="119" t="n"/>
+      <c r="G5" s="119" t="n"/>
+      <c r="H5" s="120" t="n"/>
+      <c r="I5" s="82" t="n"/>
+      <c r="J5" s="82" t="n"/>
+      <c r="K5" s="82" t="n"/>
+      <c r="L5" s="121" t="n"/>
+      <c r="M5" s="122" t="n"/>
+      <c r="N5" s="15" t="n"/>
+    </row>
+    <row r="6" ht="18" customHeight="1" s="107">
+      <c r="A6" s="7" t="n"/>
+      <c r="D6" s="83" t="n"/>
+      <c r="E6" s="106" t="n"/>
+      <c r="N6" s="16" t="n"/>
+    </row>
+    <row r="7" ht="22.5" customHeight="1" s="107">
+      <c r="A7" s="7" t="n"/>
+      <c r="D7" s="83" t="n"/>
+      <c r="E7" s="111" t="n"/>
+      <c r="N7" s="17" t="n"/>
+    </row>
+    <row r="8" ht="26.25" customHeight="1" s="107">
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="105" t="inlineStr">
+        <is>
+          <t>Account:</t>
+        </is>
+      </c>
+      <c r="C8" s="123" t="n"/>
+      <c r="D8" s="105" t="inlineStr">
+        <is>
+          <t>Wholesaler:</t>
+        </is>
+      </c>
+      <c r="E8" s="80" t="inlineStr">
+        <is>
+          <t>Issue Credit to:</t>
+        </is>
+      </c>
+      <c r="F8" s="123" t="n"/>
+      <c r="G8" s="123" t="n"/>
+      <c r="H8" s="100" t="n"/>
+      <c r="L8" s="66" t="n"/>
+      <c r="M8" s="66" t="n"/>
+      <c r="N8" s="18" t="n"/>
+    </row>
+    <row r="9" ht="8" customHeight="1" s="107">
+      <c r="A9" s="7" t="n"/>
+      <c r="B9" s="82" t="n"/>
+      <c r="D9" s="39" t="n"/>
+      <c r="E9" s="82" t="n"/>
+      <c r="H9" s="39" t="n"/>
+      <c r="I9" s="39" t="n"/>
+      <c r="J9" s="39" t="n"/>
+      <c r="K9" s="39" t="n"/>
+      <c r="L9" s="82" t="n"/>
+      <c r="M9" s="82" t="n"/>
+      <c r="N9" s="19" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1" s="107">
+      <c r="A10" s="52" t="n"/>
+      <c r="B10" s="99" t="inlineStr">
+        <is>
+          <t>Proud Pharmaceuticals</t>
+        </is>
+      </c>
+      <c r="D10" s="99" t="inlineStr">
         <is>
           <t>Cardinal Health</t>
         </is>
       </c>
-      <c r="C5" s="17" t="n"/>
-      <c r="D5" s="20" t="n"/>
-      <c r="E5" s="8" t="n"/>
-      <c r="F5" s="8" t="n"/>
-      <c r="G5" s="8" t="n"/>
-      <c r="H5" s="8" t="n"/>
-      <c r="I5" s="8" t="n"/>
-      <c r="J5" s="8" t="n"/>
-      <c r="K5" s="8" t="n"/>
-      <c r="L5" s="8" t="n"/>
-      <c r="M5" s="18" t="inlineStr">
-        <is>
-          <t>DATE</t>
-        </is>
-      </c>
-      <c r="N5" s="15" t="n"/>
-    </row>
-    <row r="6" ht="18" customHeight="1" s="70">
-      <c r="A6" s="7" t="n"/>
-      <c r="B6" s="19" t="inlineStr">
+      <c r="E10" s="83" t="inlineStr">
+        <is>
+          <t>Proud Pharmaceuticals</t>
+        </is>
+      </c>
+      <c r="H10" s="101" t="n"/>
+      <c r="L10" s="83" t="n"/>
+      <c r="M10" s="83" t="n"/>
+      <c r="N10" s="20" t="n"/>
+    </row>
+    <row r="11" ht="18" customHeight="1" s="107">
+      <c r="A11" s="52" t="n"/>
+      <c r="B11" s="99" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="D11" s="99" t="inlineStr">
         <is>
           <t>Acd</t>
         </is>
       </c>
-      <c r="C6" s="20" t="n"/>
-      <c r="D6" s="20" t="n"/>
-      <c r="E6" s="8" t="n"/>
-      <c r="F6" s="8" t="n"/>
-      <c r="G6" s="8" t="n"/>
-      <c r="H6" s="8" t="n"/>
-      <c r="I6" s="8" t="n"/>
-      <c r="J6" s="8" t="n"/>
-      <c r="K6" s="8" t="n"/>
-      <c r="L6" s="8" t="n"/>
-      <c r="M6" s="18" t="inlineStr">
-        <is>
-          <t>INVOICE NO.</t>
-        </is>
-      </c>
-      <c r="N6" s="21" t="n"/>
-    </row>
-    <row r="7" ht="18" customHeight="1" s="70">
-      <c r="A7" s="7" t="n"/>
-      <c r="B7" s="19" t="inlineStr">
+      <c r="E11" s="83" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="H11" s="102" t="n"/>
+      <c r="L11" s="83" t="n"/>
+      <c r="M11" s="83" t="n"/>
+      <c r="N11" s="20" t="n"/>
+    </row>
+    <row r="12" ht="18" customHeight="1" s="107">
+      <c r="A12" s="52" t="n"/>
+      <c r="B12" s="99" t="inlineStr">
+        <is>
+          <t>5960 East Shelby Drive, Suite 100</t>
+        </is>
+      </c>
+      <c r="D12" s="99" t="inlineStr">
         <is>
           <t>7000 Cardinal Place</t>
         </is>
       </c>
-      <c r="C7" s="20" t="n"/>
-      <c r="D7" s="20" t="n"/>
-      <c r="E7" s="69" t="n"/>
-      <c r="N7" s="22" t="n"/>
-    </row>
-    <row r="8" ht="22.5" customHeight="1" s="70">
-      <c r="A8" s="7" t="n"/>
-      <c r="B8" s="19" t="inlineStr">
+      <c r="E12" s="83" t="inlineStr">
+        <is>
+          <t>5960 East Shelby Drive, Suite 100</t>
+        </is>
+      </c>
+      <c r="H12" s="102" t="n"/>
+      <c r="L12" s="83" t="n"/>
+      <c r="M12" s="83" t="n"/>
+      <c r="N12" s="20" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="107">
+      <c r="A13" s="52" t="n"/>
+      <c r="B13" s="99" t="inlineStr">
+        <is>
+          <t>(800) 727-6331</t>
+        </is>
+      </c>
+      <c r="D13" s="99" t="inlineStr">
         <is>
           <t>(800) 926-3161</t>
         </is>
       </c>
-      <c r="C8" s="20" t="n"/>
-      <c r="D8" s="20" t="n"/>
-      <c r="E8" s="75" t="n"/>
-      <c r="N8" s="23" t="n"/>
-    </row>
-    <row r="9" ht="26.25" customHeight="1" s="70">
-      <c r="A9" s="7" t="n"/>
-      <c r="B9" s="12" t="inlineStr">
-        <is>
-          <t>BILL TO</t>
-        </is>
-      </c>
-      <c r="C9" s="12" t="inlineStr">
-        <is>
-          <t>SHIP TO</t>
-        </is>
-      </c>
-      <c r="D9" s="12" t="n"/>
-      <c r="E9" s="13" t="n"/>
-      <c r="F9" s="13" t="n"/>
-      <c r="G9" s="13" t="n"/>
-      <c r="H9" s="13" t="n"/>
-      <c r="I9" s="13" t="n"/>
-      <c r="J9" s="13" t="n"/>
-      <c r="K9" s="13" t="n"/>
-      <c r="L9" s="13" t="n"/>
-      <c r="M9" s="13" t="n"/>
-      <c r="N9" s="24" t="n"/>
-    </row>
-    <row r="10" ht="8" customHeight="1" s="70">
-      <c r="A10" s="7" t="n"/>
-      <c r="B10" s="25" t="n"/>
-      <c r="C10" s="25" t="n"/>
-      <c r="D10" s="25" t="n"/>
-      <c r="E10" s="25" t="n"/>
-      <c r="F10" s="25" t="n"/>
-      <c r="G10" s="25" t="n"/>
-      <c r="H10" s="25" t="n"/>
-      <c r="I10" s="25" t="n"/>
-      <c r="J10" s="25" t="n"/>
-      <c r="K10" s="25" t="n"/>
-      <c r="L10" s="25" t="n"/>
-      <c r="M10" s="25" t="n"/>
-      <c r="N10" s="26" t="n"/>
-    </row>
-    <row r="11" ht="18" customHeight="1" s="70">
-      <c r="A11" s="7" t="n"/>
-      <c r="B11" s="19" t="inlineStr">
-        <is>
-          <t>Proud Pharmaceuticals</t>
-        </is>
-      </c>
-      <c r="C11" s="19" t="inlineStr">
-        <is>
-          <t>Proud Pharmaceuticals</t>
-        </is>
-      </c>
-      <c r="D11" s="19" t="n"/>
-      <c r="E11" s="20" t="n"/>
-      <c r="F11" s="20" t="n"/>
-      <c r="G11" s="20" t="n"/>
-      <c r="H11" s="20" t="n"/>
-      <c r="I11" s="20" t="n"/>
-      <c r="J11" s="20" t="n"/>
-      <c r="K11" s="20" t="n"/>
-      <c r="L11" s="20" t="n"/>
-      <c r="M11" s="20" t="n"/>
-      <c r="N11" s="27" t="n"/>
-    </row>
-    <row r="12" ht="18" customHeight="1" s="70">
-      <c r="A12" s="7" t="n"/>
-      <c r="B12" s="19" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="C12" s="19" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="D12" s="19" t="n"/>
-      <c r="E12" s="20" t="n"/>
-      <c r="F12" s="20" t="n"/>
-      <c r="G12" s="20" t="n"/>
-      <c r="H12" s="20" t="n"/>
-      <c r="I12" s="20" t="n"/>
-      <c r="J12" s="20" t="n"/>
-      <c r="K12" s="20" t="n"/>
-      <c r="L12" s="20" t="n"/>
-      <c r="M12" s="20" t="n"/>
-      <c r="N12" s="27" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="70">
-      <c r="A13" s="7" t="n"/>
-      <c r="B13" s="19" t="inlineStr">
-        <is>
-          <t>5960 East Shelby Drive, Suite 100</t>
-        </is>
-      </c>
-      <c r="C13" s="19" t="inlineStr">
-        <is>
-          <t>5960 East Shelby Drive, Suite 100</t>
-        </is>
-      </c>
-      <c r="D13" s="19" t="n"/>
-      <c r="E13" s="20" t="n"/>
-      <c r="F13" s="20" t="n"/>
-      <c r="G13" s="20" t="n"/>
-      <c r="H13" s="20" t="n"/>
-      <c r="I13" s="20" t="n"/>
-      <c r="J13" s="20" t="n"/>
-      <c r="K13" s="20" t="n"/>
-      <c r="L13" s="20" t="n"/>
-      <c r="M13" s="20" t="n"/>
-      <c r="N13" s="27" t="n"/>
-    </row>
-    <row r="14" ht="18" customHeight="1" s="70">
-      <c r="A14" s="7" t="n"/>
-      <c r="B14" s="19" t="inlineStr">
+      <c r="E13" s="83" t="inlineStr">
         <is>
           <t>(800) 727-6331</t>
         </is>
       </c>
-      <c r="C14" s="19" t="inlineStr">
-        <is>
-          <t>(800) 727-6331</t>
-        </is>
-      </c>
-      <c r="D14" s="19" t="n"/>
-      <c r="E14" s="20" t="n"/>
-      <c r="F14" s="20" t="n"/>
-      <c r="G14" s="20" t="n"/>
-      <c r="H14" s="20" t="n"/>
-      <c r="I14" s="20" t="n"/>
-      <c r="J14" s="20" t="n"/>
-      <c r="K14" s="20" t="n"/>
-      <c r="L14" s="20" t="n"/>
-      <c r="M14" s="20" t="n"/>
-      <c r="N14" s="27" t="n"/>
-    </row>
-    <row r="15" ht="18" customHeight="1" s="70">
-      <c r="A15" s="7" t="n"/>
-      <c r="B15" s="19" t="inlineStr">
+      <c r="H13" s="102" t="n"/>
+      <c r="L13" s="83" t="n"/>
+      <c r="M13" s="83" t="n"/>
+      <c r="N13" s="20" t="n"/>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="107">
+      <c r="A14" s="52" t="n"/>
+      <c r="B14" s="99" t="inlineStr">
         <is>
           <t>chris.dewitt@parmedpharm.com</t>
         </is>
       </c>
-      <c r="C15" s="20" t="inlineStr">
+      <c r="D14" s="83" t="n"/>
+      <c r="E14" s="83" t="inlineStr">
         <is>
           <t>chris.dewitt@parmedpharm.com</t>
         </is>
       </c>
-      <c r="D15" s="20" t="n"/>
-      <c r="E15" s="20" t="n"/>
-      <c r="F15" s="20" t="n"/>
-      <c r="G15" s="20" t="n"/>
-      <c r="H15" s="20" t="n"/>
-      <c r="I15" s="20" t="n"/>
-      <c r="J15" s="20" t="n"/>
-      <c r="K15" s="20" t="n"/>
-      <c r="L15" s="20" t="n"/>
-      <c r="M15" s="20" t="n"/>
-      <c r="N15" s="27" t="n"/>
-    </row>
-    <row r="16" ht="18" customHeight="1" s="70">
-      <c r="A16" s="7" t="n"/>
-      <c r="B16" s="20" t="n"/>
-      <c r="C16" s="72" t="n"/>
-      <c r="N16" s="21" t="n"/>
-    </row>
-    <row r="17" ht="8" customHeight="1" s="70">
-      <c r="A17" s="7" t="n"/>
-      <c r="B17" s="8" t="n"/>
-      <c r="C17" s="8" t="n"/>
-      <c r="D17" s="8" t="n"/>
-      <c r="E17" s="8" t="n"/>
-      <c r="F17" s="8" t="n"/>
-      <c r="G17" s="8" t="n"/>
-      <c r="H17" s="8" t="n"/>
-      <c r="I17" s="8" t="n"/>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="26" t="n"/>
-    </row>
-    <row r="18" ht="18" customHeight="1" s="70">
-      <c r="A18" s="7" t="n"/>
-      <c r="B18" s="59" t="inlineStr">
+      <c r="H14" s="103" t="n"/>
+      <c r="L14" s="83" t="n"/>
+      <c r="M14" s="83" t="n"/>
+      <c r="N14" s="20" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="107">
+      <c r="A15" s="52" t="n"/>
+      <c r="B15" s="83" t="n"/>
+      <c r="C15" s="108" t="n"/>
+      <c r="N15" s="15" t="n"/>
+    </row>
+    <row r="16" ht="8" customHeight="1" s="107">
+      <c r="A16" s="52" t="n"/>
+      <c r="B16" s="82" t="n"/>
+      <c r="C16" s="82" t="n"/>
+      <c r="D16" s="82" t="n"/>
+      <c r="E16" s="82" t="n"/>
+      <c r="F16" s="82" t="n"/>
+      <c r="G16" s="82" t="n"/>
+      <c r="H16" s="82" t="n"/>
+      <c r="I16" s="82" t="n"/>
+      <c r="J16" s="82" t="n"/>
+      <c r="K16" s="82" t="n"/>
+      <c r="L16" s="82" t="n"/>
+      <c r="M16" s="82" t="n"/>
+      <c r="N16" s="19" t="n"/>
+    </row>
+    <row r="17" ht="25" customHeight="1" s="107">
+      <c r="A17" s="52" t="n"/>
+      <c r="B17" s="42" t="inlineStr">
         <is>
           <t>NDC/UPC</t>
         </is>
       </c>
-      <c r="C18" s="59" t="inlineStr">
+      <c r="C17" s="42" t="inlineStr">
         <is>
           <t>Manufacturer</t>
         </is>
       </c>
-      <c r="D18" s="59" t="inlineStr">
+      <c r="D17" s="42" t="inlineStr">
         <is>
           <t>Product name</t>
         </is>
       </c>
-      <c r="E18" s="59" t="inlineStr">
+      <c r="E17" s="42" t="inlineStr">
         <is>
           <t>Strength</t>
         </is>
       </c>
-      <c r="F18" s="59" t="inlineStr">
+      <c r="F17" s="42" t="inlineStr">
         <is>
           <t>DSG</t>
         </is>
       </c>
-      <c r="G18" s="59" t="inlineStr">
+      <c r="G17" s="42" t="inlineStr">
         <is>
           <t>Lot</t>
         </is>
       </c>
-      <c r="H18" s="59" t="inlineStr">
+      <c r="H17" s="42" t="inlineStr">
         <is>
           <t>Exp</t>
         </is>
       </c>
-      <c r="I18" s="59" t="inlineStr">
+      <c r="I17" s="42" t="inlineStr">
         <is>
           <t>Pkg Size</t>
         </is>
       </c>
-      <c r="J18" s="59" t="inlineStr">
+      <c r="J17" s="42" t="inlineStr">
         <is>
           <t>Full Qty</t>
         </is>
       </c>
-      <c r="K18" s="59" t="inlineStr">
+      <c r="K17" s="59" t="inlineStr">
         <is>
           <t>Partial Qty</t>
         </is>
       </c>
-      <c r="L18" s="59" t="inlineStr">
+      <c r="L17" s="42" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="M18" s="59" t="inlineStr">
+      <c r="M17" s="42" t="inlineStr">
         <is>
           <t>Est Value</t>
         </is>
       </c>
-      <c r="N18" s="15" t="n"/>
-    </row>
-    <row r="19" ht="18" customHeight="1" s="70">
-      <c r="A19" s="28" t="n"/>
-      <c r="B19" s="64" t="inlineStr">
-        <is>
-          <t>6818024906</t>
-        </is>
-      </c>
-      <c r="C19" s="29" t="inlineStr">
-        <is>
-          <t>Lupin Pharmaceuticals, Inc.</t>
-        </is>
-      </c>
-      <c r="D19" s="29" t="inlineStr">
-        <is>
-          <t>memantine hydrochloride</t>
-        </is>
-      </c>
-      <c r="E19" s="30" t="inlineStr">
-        <is>
-          <t>28 mg/1</t>
-        </is>
-      </c>
-      <c r="F19" s="30" t="n"/>
-      <c r="G19" s="30" t="inlineStr">
-        <is>
-          <t>H102306</t>
-        </is>
-      </c>
-      <c r="H19" s="30" t="inlineStr">
-        <is>
-          <t>09/23/30</t>
-        </is>
-      </c>
-      <c r="I19" s="30" t="n"/>
-      <c r="J19" s="30" t="n">
+      <c r="N17" s="12" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1" s="107">
+      <c r="A18" s="53" t="n"/>
+      <c r="B18" s="43" t="inlineStr">
+        <is>
+          <t>5511153205</t>
+        </is>
+      </c>
+      <c r="C18" s="44" t="inlineStr">
+        <is>
+          <t>Dr. Reddy's Laboratories Ltd</t>
+        </is>
+      </c>
+      <c r="D18" s="44" t="inlineStr">
+        <is>
+          <t>Divalproex sodium</t>
+        </is>
+      </c>
+      <c r="E18" s="45" t="inlineStr">
+        <is>
+          <t>125 mg/1</t>
+        </is>
+      </c>
+      <c r="F18" s="45" t="inlineStr">
+        <is>
+          <t>CAPSULE</t>
+        </is>
+      </c>
+      <c r="G18" s="45" t="inlineStr">
+        <is>
+          <t>C2115420</t>
+        </is>
+      </c>
+      <c r="H18" s="45" t="inlineStr">
+        <is>
+          <t>10/23/31</t>
+        </is>
+      </c>
+      <c r="I18" s="45" t="inlineStr">
+        <is>
+          <t>500 CT</t>
+        </is>
+      </c>
+      <c r="J18" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="K19" s="30" t="n"/>
-      <c r="L19" s="30" t="n"/>
-      <c r="M19" s="30" t="n"/>
-      <c r="N19" s="31" t="n"/>
-    </row>
-    <row r="20" ht="18" customHeight="1" s="70">
-      <c r="A20" s="28" t="n"/>
-      <c r="B20" s="65" t="n"/>
-      <c r="C20" s="32" t="n"/>
-      <c r="D20" s="32" t="n"/>
-      <c r="E20" s="33" t="n"/>
-      <c r="F20" s="33" t="n"/>
-      <c r="G20" s="33" t="n"/>
-      <c r="H20" s="33" t="n"/>
-      <c r="I20" s="33" t="n"/>
-      <c r="J20" s="33" t="n"/>
-      <c r="K20" s="33" t="n"/>
-      <c r="L20" s="33" t="n"/>
-      <c r="M20" s="33" t="n"/>
-      <c r="N20" s="31" t="n"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" s="70">
-      <c r="A21" s="28" t="n"/>
-      <c r="B21" s="64" t="n"/>
-      <c r="C21" s="29" t="n"/>
-      <c r="D21" s="29" t="n"/>
-      <c r="E21" s="30" t="n"/>
-      <c r="F21" s="30" t="n"/>
-      <c r="G21" s="30" t="n"/>
-      <c r="H21" s="30" t="n"/>
-      <c r="I21" s="30" t="n"/>
-      <c r="J21" s="30" t="n"/>
-      <c r="K21" s="30" t="n"/>
-      <c r="L21" s="30" t="n"/>
-      <c r="M21" s="30" t="n"/>
-      <c r="N21" s="31" t="n"/>
-    </row>
-    <row r="22" ht="18" customHeight="1" s="70">
-      <c r="A22" s="28" t="n"/>
-      <c r="B22" s="65" t="n"/>
-      <c r="C22" s="32" t="n"/>
-      <c r="D22" s="32" t="n"/>
-      <c r="E22" s="33" t="n"/>
-      <c r="F22" s="33" t="n"/>
-      <c r="G22" s="33" t="n"/>
-      <c r="H22" s="33" t="n"/>
-      <c r="I22" s="33" t="n"/>
-      <c r="J22" s="33" t="n"/>
-      <c r="K22" s="33" t="n"/>
-      <c r="L22" s="33" t="n"/>
-      <c r="M22" s="33" t="n"/>
-      <c r="N22" s="31" t="n"/>
-    </row>
-    <row r="23" ht="18" customHeight="1" s="70">
-      <c r="A23" s="28" t="n"/>
-      <c r="B23" s="64" t="n"/>
-      <c r="C23" s="29" t="n"/>
-      <c r="D23" s="29" t="n"/>
-      <c r="E23" s="30" t="n"/>
-      <c r="F23" s="30" t="n"/>
-      <c r="G23" s="30" t="n"/>
-      <c r="H23" s="30" t="n"/>
-      <c r="I23" s="30" t="n"/>
-      <c r="J23" s="30" t="n"/>
-      <c r="K23" s="30" t="n"/>
-      <c r="L23" s="30" t="n"/>
-      <c r="M23" s="30" t="n"/>
-      <c r="N23" s="31" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="70">
-      <c r="A24" s="28" t="n"/>
-      <c r="B24" s="65" t="n"/>
-      <c r="C24" s="32" t="n"/>
-      <c r="D24" s="32" t="n"/>
-      <c r="E24" s="33" t="n"/>
-      <c r="F24" s="33" t="n"/>
-      <c r="G24" s="33" t="n"/>
-      <c r="H24" s="33" t="n"/>
-      <c r="I24" s="33" t="n"/>
-      <c r="J24" s="33" t="n"/>
-      <c r="K24" s="33" t="n"/>
-      <c r="L24" s="33" t="n"/>
-      <c r="M24" s="33" t="n"/>
-      <c r="N24" s="31" t="n"/>
-    </row>
-    <row r="25" ht="18" customHeight="1" s="70">
-      <c r="A25" s="28" t="n"/>
-      <c r="B25" s="64" t="n"/>
-      <c r="C25" s="29" t="n"/>
-      <c r="D25" s="29" t="n"/>
-      <c r="E25" s="30" t="n"/>
-      <c r="F25" s="30" t="n"/>
-      <c r="G25" s="30" t="n"/>
-      <c r="H25" s="30" t="n"/>
-      <c r="I25" s="30" t="n"/>
-      <c r="J25" s="30" t="n"/>
-      <c r="K25" s="30" t="n"/>
-      <c r="L25" s="30" t="n"/>
-      <c r="M25" s="30" t="n"/>
-      <c r="N25" s="31" t="n"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" s="70">
-      <c r="A26" s="28" t="n"/>
-      <c r="B26" s="65" t="n"/>
-      <c r="C26" s="32" t="n"/>
-      <c r="D26" s="32" t="n"/>
-      <c r="E26" s="33" t="n"/>
-      <c r="F26" s="33" t="n"/>
-      <c r="G26" s="33" t="n"/>
-      <c r="H26" s="33" t="n"/>
-      <c r="I26" s="33" t="n"/>
-      <c r="J26" s="33" t="n"/>
-      <c r="K26" s="33" t="n"/>
-      <c r="L26" s="33" t="n"/>
-      <c r="M26" s="33" t="n"/>
-      <c r="N26" s="31" t="n"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" s="70">
-      <c r="A27" s="28" t="n"/>
-      <c r="B27" s="64" t="n"/>
-      <c r="C27" s="29" t="n"/>
-      <c r="D27" s="29" t="n"/>
-      <c r="E27" s="30" t="n"/>
-      <c r="F27" s="30" t="n"/>
-      <c r="G27" s="30" t="n"/>
-      <c r="H27" s="30" t="n"/>
-      <c r="I27" s="30" t="n"/>
-      <c r="J27" s="30" t="n"/>
-      <c r="K27" s="30" t="n"/>
-      <c r="L27" s="30" t="n"/>
-      <c r="M27" s="30" t="n"/>
-      <c r="N27" s="31" t="n"/>
-    </row>
-    <row r="28" ht="18" customHeight="1" s="70">
-      <c r="A28" s="28" t="n"/>
-      <c r="B28" s="65" t="n"/>
-      <c r="C28" s="32" t="n"/>
-      <c r="D28" s="32" t="n"/>
-      <c r="E28" s="33" t="n"/>
-      <c r="F28" s="33" t="n"/>
-      <c r="G28" s="33" t="n"/>
-      <c r="H28" s="33" t="n"/>
-      <c r="I28" s="33" t="n"/>
-      <c r="J28" s="33" t="n"/>
-      <c r="K28" s="33" t="n"/>
-      <c r="L28" s="33" t="n"/>
-      <c r="M28" s="33" t="n"/>
-      <c r="N28" s="31" t="n"/>
-    </row>
-    <row r="29" ht="18" customHeight="1" s="70">
-      <c r="A29" s="28" t="n"/>
-      <c r="B29" s="64" t="n"/>
-      <c r="C29" s="29" t="n"/>
-      <c r="D29" s="29" t="n"/>
-      <c r="E29" s="30" t="n"/>
-      <c r="F29" s="30" t="n"/>
-      <c r="G29" s="30" t="n"/>
-      <c r="H29" s="30" t="n"/>
-      <c r="I29" s="30" t="n"/>
-      <c r="J29" s="30" t="n"/>
-      <c r="K29" s="30" t="n"/>
-      <c r="L29" s="30" t="n"/>
-      <c r="M29" s="30" t="n"/>
-      <c r="N29" s="31" t="n"/>
-    </row>
-    <row r="30" ht="19.5" customHeight="1" s="70">
-      <c r="A30" s="7" t="n"/>
-      <c r="B30" s="34" t="inlineStr">
-        <is>
-          <t>Remarks / Payment Instructions:</t>
-        </is>
-      </c>
-      <c r="C30" s="35" t="n"/>
-      <c r="D30" s="35" t="n"/>
-      <c r="E30" s="36" t="inlineStr">
-        <is>
-          <t>SUBTOTAL</t>
-        </is>
-      </c>
-      <c r="F30" s="36" t="n"/>
-      <c r="G30" s="36" t="n"/>
-      <c r="H30" s="36" t="n"/>
-      <c r="I30" s="36" t="n"/>
-      <c r="J30" s="36" t="n"/>
-      <c r="K30" s="36" t="n"/>
-      <c r="L30" s="36" t="n"/>
-      <c r="M30" s="37">
-        <f>SUM(M19:M29)</f>
-        <v/>
-      </c>
-      <c r="N30" s="38" t="n"/>
-    </row>
-    <row r="31" ht="19.5" customHeight="1" s="70">
-      <c r="A31" s="7" t="n"/>
-      <c r="B31" s="76" t="n"/>
-      <c r="C31" s="39" t="n"/>
-      <c r="D31" s="39" t="n"/>
-      <c r="E31" s="40" t="inlineStr">
-        <is>
-          <t>DISCOUNT</t>
-        </is>
-      </c>
-      <c r="F31" s="40" t="n"/>
-      <c r="G31" s="40" t="n"/>
-      <c r="H31" s="40" t="n"/>
-      <c r="I31" s="40" t="n"/>
-      <c r="J31" s="40" t="n"/>
-      <c r="K31" s="40" t="n"/>
-      <c r="L31" s="40" t="n"/>
-      <c r="M31" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" s="38" t="n"/>
-    </row>
-    <row r="32" ht="19.5" customHeight="1" s="70">
-      <c r="A32" s="7" t="n"/>
-      <c r="C32" s="39" t="n"/>
-      <c r="D32" s="39" t="n"/>
-      <c r="E32" s="40" t="inlineStr">
-        <is>
-          <t>SUBTOTAL LESS DISCOUNT</t>
-        </is>
-      </c>
-      <c r="F32" s="40" t="n"/>
-      <c r="G32" s="40" t="n"/>
-      <c r="H32" s="40" t="n"/>
-      <c r="I32" s="40" t="n"/>
-      <c r="J32" s="40" t="n"/>
-      <c r="K32" s="40" t="n"/>
-      <c r="L32" s="40" t="n"/>
-      <c r="M32" s="37">
-        <f>M30-M31</f>
-        <v/>
-      </c>
-      <c r="N32" s="38" t="n"/>
-    </row>
-    <row r="33" ht="19.5" customHeight="1" s="70">
-      <c r="A33" s="7" t="n"/>
-      <c r="C33" s="39" t="n"/>
-      <c r="D33" s="39" t="n"/>
-      <c r="E33" s="40" t="inlineStr">
-        <is>
-          <t>TAX RATE</t>
-        </is>
-      </c>
-      <c r="F33" s="40" t="n"/>
-      <c r="G33" s="40" t="n"/>
-      <c r="H33" s="40" t="n"/>
-      <c r="I33" s="40" t="n"/>
-      <c r="J33" s="40" t="n"/>
-      <c r="K33" s="40" t="n"/>
-      <c r="L33" s="40" t="n"/>
-      <c r="M33" s="41" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" s="42" t="n"/>
-    </row>
-    <row r="34" ht="19.5" customHeight="1" s="70">
-      <c r="A34" s="7" t="n"/>
-      <c r="C34" s="39" t="n"/>
-      <c r="D34" s="39" t="n"/>
-      <c r="E34" s="40" t="inlineStr">
-        <is>
-          <t>TOTAL TAX</t>
-        </is>
-      </c>
-      <c r="F34" s="40" t="n"/>
-      <c r="G34" s="40" t="n"/>
-      <c r="H34" s="40" t="n"/>
-      <c r="I34" s="40" t="n"/>
-      <c r="J34" s="40" t="n"/>
-      <c r="K34" s="40" t="n"/>
-      <c r="L34" s="40" t="n"/>
-      <c r="M34" s="37">
-        <f>M32*M33</f>
-        <v/>
-      </c>
-      <c r="N34" s="38" t="n"/>
-    </row>
-    <row r="35" ht="19.5" customHeight="1" s="70">
-      <c r="A35" s="7" t="n"/>
-      <c r="C35" s="39" t="n"/>
-      <c r="D35" s="39" t="n"/>
-      <c r="E35" s="43" t="inlineStr">
-        <is>
-          <t>SHIPPING/HANDLING</t>
-        </is>
-      </c>
-      <c r="F35" s="43" t="n"/>
-      <c r="G35" s="43" t="n"/>
-      <c r="H35" s="43" t="n"/>
-      <c r="I35" s="43" t="n"/>
-      <c r="J35" s="43" t="n"/>
-      <c r="K35" s="43" t="n"/>
-      <c r="L35" s="43" t="n"/>
-      <c r="M35" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" s="45" t="n"/>
-    </row>
-    <row r="36" ht="33.75" customHeight="1" s="70">
-      <c r="A36" s="7" t="n"/>
-      <c r="B36" s="68" t="n"/>
-      <c r="C36" s="39" t="n"/>
-      <c r="D36" s="39" t="n"/>
-      <c r="E36" s="46" t="inlineStr">
-        <is>
-          <t>Balance Due</t>
-        </is>
-      </c>
-      <c r="F36" s="46" t="n"/>
-      <c r="G36" s="46" t="n"/>
-      <c r="H36" s="46" t="n"/>
-      <c r="I36" s="46" t="n"/>
-      <c r="J36" s="46" t="n"/>
-      <c r="K36" s="46" t="n"/>
-      <c r="L36" s="46" t="n"/>
-      <c r="M36" s="47">
-        <f>M32+M34+M35</f>
-        <v/>
-      </c>
-      <c r="N36" s="48" t="n"/>
-    </row>
-    <row r="37" ht="9.75" customHeight="1" s="70">
-      <c r="A37" s="7" t="n"/>
-      <c r="B37" s="71" t="n"/>
-      <c r="N37" s="50" t="n"/>
-    </row>
-    <row r="38" ht="9.75" customHeight="1" s="70">
-      <c r="A38" s="7" t="n"/>
-      <c r="B38" s="71" t="n"/>
-      <c r="C38" s="71" t="n"/>
-      <c r="D38" s="71" t="n"/>
-      <c r="E38" s="71" t="n"/>
-      <c r="F38" s="71" t="n"/>
-      <c r="G38" s="71" t="n"/>
-      <c r="H38" s="71" t="n"/>
-      <c r="I38" s="71" t="n"/>
-      <c r="J38" s="71" t="n"/>
-      <c r="K38" s="71" t="n"/>
-      <c r="L38" s="71" t="n"/>
-      <c r="M38" s="71" t="n"/>
+      <c r="K18" s="45" t="n"/>
+      <c r="L18" s="45" t="n"/>
+      <c r="M18" s="45" t="n"/>
+      <c r="N18" s="23" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1" s="107">
+      <c r="A19" s="53" t="n"/>
+      <c r="B19" s="46" t="n"/>
+      <c r="C19" s="47" t="n"/>
+      <c r="D19" s="47" t="n"/>
+      <c r="E19" s="48" t="n"/>
+      <c r="F19" s="48" t="n"/>
+      <c r="G19" s="48" t="n"/>
+      <c r="H19" s="48" t="n"/>
+      <c r="I19" s="48" t="n"/>
+      <c r="J19" s="48" t="n"/>
+      <c r="K19" s="48" t="n"/>
+      <c r="M19" s="48" t="n"/>
+      <c r="N19" s="23" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1" s="107">
+      <c r="A20" s="53" t="n"/>
+      <c r="B20" s="43" t="n"/>
+      <c r="C20" s="44" t="n"/>
+      <c r="D20" s="44" t="n"/>
+      <c r="E20" s="45" t="n"/>
+      <c r="F20" s="45" t="n"/>
+      <c r="G20" s="45" t="n"/>
+      <c r="H20" s="45" t="n"/>
+      <c r="I20" s="45" t="n"/>
+      <c r="J20" s="45" t="n"/>
+      <c r="K20" s="45" t="n"/>
+      <c r="L20" s="48" t="n"/>
+      <c r="M20" s="45" t="n"/>
+      <c r="N20" s="23" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="107">
+      <c r="A21" s="53" t="n"/>
+      <c r="B21" s="46" t="n"/>
+      <c r="C21" s="47" t="n"/>
+      <c r="D21" s="47" t="n"/>
+      <c r="E21" s="48" t="n"/>
+      <c r="F21" s="48" t="n"/>
+      <c r="G21" s="48" t="n"/>
+      <c r="H21" s="48" t="n"/>
+      <c r="I21" s="48" t="n"/>
+      <c r="J21" s="48" t="n"/>
+      <c r="K21" s="48" t="n"/>
+      <c r="L21" s="48" t="n"/>
+      <c r="M21" s="48" t="n"/>
+      <c r="N21" s="23" t="n"/>
+    </row>
+    <row r="22" ht="18" customHeight="1" s="107">
+      <c r="A22" s="53" t="n"/>
+      <c r="B22" s="43" t="n"/>
+      <c r="C22" s="44" t="n"/>
+      <c r="D22" s="44" t="n"/>
+      <c r="E22" s="45" t="n"/>
+      <c r="F22" s="45" t="n"/>
+      <c r="G22" s="45" t="n"/>
+      <c r="H22" s="45" t="n"/>
+      <c r="I22" s="45" t="n"/>
+      <c r="J22" s="45" t="n"/>
+      <c r="K22" s="45" t="n"/>
+      <c r="L22" s="45" t="n"/>
+      <c r="M22" s="45" t="n"/>
+      <c r="N22" s="23" t="n"/>
+    </row>
+    <row r="23" ht="18" customHeight="1" s="107">
+      <c r="A23" s="53" t="n"/>
+      <c r="B23" s="46" t="n"/>
+      <c r="C23" s="47" t="n"/>
+      <c r="D23" s="47" t="n"/>
+      <c r="E23" s="48" t="n"/>
+      <c r="F23" s="48" t="n"/>
+      <c r="G23" s="48" t="n"/>
+      <c r="H23" s="48" t="n"/>
+      <c r="I23" s="48" t="n"/>
+      <c r="J23" s="48" t="n"/>
+      <c r="K23" s="48" t="n"/>
+      <c r="L23" s="48" t="n"/>
+      <c r="M23" s="48" t="n"/>
+      <c r="N23" s="23" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="107">
+      <c r="A24" s="53" t="n"/>
+      <c r="B24" s="43" t="n"/>
+      <c r="C24" s="44" t="n"/>
+      <c r="D24" s="44" t="n"/>
+      <c r="E24" s="45" t="n"/>
+      <c r="F24" s="45" t="n"/>
+      <c r="G24" s="45" t="n"/>
+      <c r="H24" s="45" t="n"/>
+      <c r="I24" s="45" t="n"/>
+      <c r="J24" s="45" t="n"/>
+      <c r="K24" s="45" t="n"/>
+      <c r="L24" s="45" t="n"/>
+      <c r="M24" s="45" t="n"/>
+      <c r="N24" s="23" t="n"/>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="107">
+      <c r="A25" s="53" t="n"/>
+      <c r="B25" s="46" t="n"/>
+      <c r="C25" s="47" t="n"/>
+      <c r="D25" s="47" t="n"/>
+      <c r="E25" s="48" t="n"/>
+      <c r="F25" s="48" t="n"/>
+      <c r="G25" s="48" t="n"/>
+      <c r="H25" s="48" t="n"/>
+      <c r="I25" s="48" t="n"/>
+      <c r="J25" s="48" t="n"/>
+      <c r="K25" s="48" t="n"/>
+      <c r="L25" s="48" t="n"/>
+      <c r="M25" s="48" t="n"/>
+      <c r="N25" s="23" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="107">
+      <c r="A26" s="53" t="n"/>
+      <c r="B26" s="43" t="n"/>
+      <c r="C26" s="44" t="n"/>
+      <c r="D26" s="44" t="n"/>
+      <c r="E26" s="45" t="n"/>
+      <c r="F26" s="45" t="n"/>
+      <c r="G26" s="45" t="n"/>
+      <c r="H26" s="45" t="n"/>
+      <c r="I26" s="45" t="n"/>
+      <c r="J26" s="45" t="n"/>
+      <c r="K26" s="45" t="n"/>
+      <c r="L26" s="45" t="n"/>
+      <c r="M26" s="45" t="n"/>
+      <c r="N26" s="23" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="107">
+      <c r="A27" s="53" t="n"/>
+      <c r="B27" s="46" t="n"/>
+      <c r="C27" s="47" t="n"/>
+      <c r="D27" s="47" t="n"/>
+      <c r="E27" s="48" t="n"/>
+      <c r="F27" s="48" t="n"/>
+      <c r="G27" s="48" t="n"/>
+      <c r="H27" s="48" t="n"/>
+      <c r="I27" s="48" t="n"/>
+      <c r="J27" s="48" t="n"/>
+      <c r="K27" s="48" t="n"/>
+      <c r="L27" s="48" t="n"/>
+      <c r="M27" s="48" t="n"/>
+      <c r="N27" s="23" t="n"/>
+    </row>
+    <row r="28" ht="18" customFormat="1" customHeight="1" s="39">
+      <c r="A28" s="53" t="n"/>
+      <c r="B28" s="43" t="n"/>
+      <c r="C28" s="44" t="n"/>
+      <c r="D28" s="44" t="n"/>
+      <c r="E28" s="45" t="n"/>
+      <c r="F28" s="45" t="n"/>
+      <c r="G28" s="45" t="n"/>
+      <c r="H28" s="45" t="n"/>
+      <c r="I28" s="45" t="n"/>
+      <c r="J28" s="45" t="n"/>
+      <c r="K28" s="45" t="n"/>
+      <c r="L28" s="45" t="n"/>
+      <c r="M28" s="45" t="n"/>
+      <c r="N28" s="23" t="n"/>
+    </row>
+    <row r="29" ht="18" customFormat="1" customHeight="1" s="39">
+      <c r="A29" s="53" t="n"/>
+      <c r="B29" s="46" t="n"/>
+      <c r="C29" s="47" t="n"/>
+      <c r="D29" s="47" t="n"/>
+      <c r="E29" s="48" t="n"/>
+      <c r="F29" s="48" t="n"/>
+      <c r="G29" s="48" t="n"/>
+      <c r="H29" s="48" t="n"/>
+      <c r="I29" s="48" t="n"/>
+      <c r="J29" s="48" t="n"/>
+      <c r="K29" s="48" t="n"/>
+      <c r="L29" s="48" t="n"/>
+      <c r="M29" s="48" t="n"/>
+      <c r="N29" s="23" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1" s="107">
+      <c r="A30" s="53" t="n"/>
+      <c r="B30" s="37" t="n"/>
+      <c r="C30" s="21" t="n"/>
+      <c r="D30" s="21" t="n"/>
+      <c r="E30" s="22" t="n"/>
+      <c r="F30" s="22" t="n"/>
+      <c r="G30" s="22" t="n"/>
+      <c r="H30" s="22" t="n"/>
+      <c r="I30" s="22" t="n"/>
+      <c r="J30" s="22" t="n"/>
+      <c r="K30" s="22" t="n"/>
+      <c r="L30" s="22" t="n"/>
+      <c r="M30" s="22" t="n"/>
+      <c r="N30" s="23" t="n"/>
+    </row>
+    <row r="31" ht="26" customHeight="1" s="107">
+      <c r="A31" s="52" t="n"/>
+      <c r="B31" s="24" t="n"/>
+      <c r="C31" s="25" t="n"/>
+      <c r="D31" s="25" t="n"/>
+      <c r="E31" s="26" t="n"/>
+      <c r="F31" s="26" t="n"/>
+      <c r="G31" s="26" t="n"/>
+      <c r="H31" s="26" t="n"/>
+      <c r="I31" s="26" t="n"/>
+      <c r="J31" s="26" t="n"/>
+      <c r="K31" s="26" t="n"/>
+      <c r="L31" s="26" t="n"/>
+      <c r="M31" s="40" t="n"/>
+      <c r="N31" s="65" t="n"/>
+      <c r="O31" s="41" t="n"/>
+    </row>
+    <row r="32" ht="33.75" customHeight="1" s="107">
+      <c r="A32" s="52" t="n"/>
+      <c r="B32" s="38" t="n"/>
+      <c r="C32" s="27" t="n"/>
+      <c r="D32" s="27" t="n"/>
+      <c r="E32" s="63" t="n"/>
+      <c r="F32" s="63" t="n"/>
+      <c r="G32" s="63" t="n"/>
+      <c r="H32" s="63" t="n"/>
+      <c r="I32" s="63" t="n"/>
+      <c r="J32" s="63" t="n"/>
+      <c r="K32" s="63" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
+      <c r="L32" s="73" t="n"/>
+      <c r="N32" s="64" t="n"/>
+      <c r="O32" s="41" t="n"/>
+    </row>
+    <row r="33" ht="9.75" customHeight="1" s="107">
+      <c r="A33" s="52" t="n"/>
+      <c r="B33" s="28" t="n"/>
+      <c r="C33" s="28" t="n"/>
+      <c r="D33" s="28" t="n"/>
+      <c r="E33" s="28" t="n"/>
+      <c r="F33" s="28" t="n"/>
+      <c r="G33" s="28" t="n"/>
+      <c r="H33" s="28" t="n"/>
+      <c r="I33" s="28" t="n"/>
+      <c r="J33" s="28" t="n"/>
+      <c r="K33" s="28" t="n"/>
+      <c r="L33" s="28" t="n"/>
+      <c r="M33" s="28" t="n"/>
+      <c r="N33" s="28" t="n"/>
+      <c r="O33" s="41" t="n"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1" s="107">
+      <c r="A34" s="52" t="n"/>
+      <c r="B34" s="112" t="n"/>
+      <c r="N34" s="29" t="n"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1" s="107">
+      <c r="A35" s="52" t="n"/>
+      <c r="B35" s="109" t="n"/>
+      <c r="N35" s="30" t="n"/>
+    </row>
+    <row r="36" ht="21" customHeight="1" s="107">
+      <c r="A36" s="54" t="n"/>
+      <c r="B36" s="110" t="n"/>
+      <c r="N36" s="31" t="n"/>
+    </row>
+    <row r="37" ht="8" customHeight="1" s="107">
+      <c r="A37" s="52" t="n"/>
+      <c r="B37" s="9" t="n"/>
+      <c r="C37" s="56" t="n"/>
+      <c r="D37" s="57" t="n"/>
+      <c r="E37" s="57" t="n"/>
+      <c r="F37" s="57" t="n"/>
+      <c r="G37" s="57" t="n"/>
+      <c r="H37" s="57" t="n"/>
+      <c r="I37" s="57" t="n"/>
+      <c r="J37" s="57" t="n"/>
+      <c r="K37" s="57" t="n"/>
+      <c r="L37" s="58" t="n"/>
+      <c r="M37" s="9" t="n"/>
+      <c r="N37" s="49" t="n"/>
+    </row>
+    <row r="38" ht="24" customHeight="1" s="107">
+      <c r="A38" s="41" t="n"/>
+      <c r="C38" s="60" t="n"/>
+      <c r="D38" s="98" t="inlineStr">
+        <is>
+          <t>Return instructions:</t>
+        </is>
+      </c>
+      <c r="I38" s="61" t="n"/>
+      <c r="J38" s="61" t="n"/>
+      <c r="K38" s="61" t="n"/>
+      <c r="L38" s="62" t="n"/>
       <c r="N38" s="50" t="n"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1" s="70">
-      <c r="A39" s="7" t="n"/>
-      <c r="B39" s="77" t="n"/>
-      <c r="N39" s="51" t="n"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1" s="70">
-      <c r="A40" s="7" t="n"/>
-      <c r="B40" s="73" t="n"/>
-      <c r="N40" s="52" t="n"/>
-    </row>
-    <row r="41" ht="21" customHeight="1" s="70">
-      <c r="A41" s="53" t="n"/>
-      <c r="B41" s="74" t="n"/>
-      <c r="N41" s="54" t="n"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1" s="70">
-      <c r="A42" s="7" t="n"/>
-      <c r="B42" s="9" t="n"/>
-      <c r="C42" s="9" t="n"/>
-      <c r="D42" s="9" t="n"/>
-      <c r="E42" s="9" t="n"/>
-      <c r="F42" s="9" t="n"/>
-      <c r="G42" s="9" t="n"/>
-      <c r="H42" s="9" t="n"/>
-      <c r="I42" s="9" t="n"/>
-      <c r="J42" s="9" t="n"/>
-      <c r="K42" s="9" t="n"/>
-      <c r="L42" s="9" t="n"/>
-      <c r="M42" s="9" t="n"/>
-      <c r="N42" s="55" t="n"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1" s="70">
-      <c r="A43" s="56" t="n"/>
-      <c r="B43" s="57" t="n"/>
-      <c r="C43" s="57" t="n"/>
-      <c r="D43" s="57" t="n"/>
-      <c r="E43" s="57" t="n"/>
-      <c r="F43" s="57" t="n"/>
-      <c r="G43" s="57" t="n"/>
-      <c r="H43" s="57" t="n"/>
-      <c r="I43" s="57" t="n"/>
-      <c r="J43" s="57" t="n"/>
-      <c r="K43" s="57" t="n"/>
-      <c r="L43" s="57" t="n"/>
-      <c r="M43" s="57" t="n"/>
-      <c r="N43" s="58" t="n"/>
+    <row r="39" ht="15" customHeight="1" s="107">
+      <c r="A39" s="41" t="n"/>
+      <c r="C39" s="60" t="n"/>
+      <c r="D39" s="61" t="n"/>
+      <c r="E39" s="61" t="n"/>
+      <c r="F39" s="61" t="n"/>
+      <c r="G39" s="61" t="n"/>
+      <c r="H39" s="61" t="n"/>
+      <c r="I39" s="61" t="n"/>
+      <c r="J39" s="61" t="n"/>
+      <c r="K39" s="61" t="n"/>
+      <c r="L39" s="62" t="n"/>
+      <c r="N39" s="50" t="n"/>
+    </row>
+    <row r="40" ht="17" customHeight="1" s="107">
+      <c r="A40" s="41" t="n"/>
+      <c r="C40" s="124" t="inlineStr">
+        <is>
+          <t>1. Email the Packing Slip to Customer Service via email to https://returns.healthcare.inmar.com request a Return Authorization (RGA).</t>
+        </is>
+      </c>
+      <c r="L40" s="50" t="n"/>
+      <c r="N40" s="50" t="n"/>
+    </row>
+    <row r="41" ht="3" customHeight="1" s="107">
+      <c r="A41" s="41" t="n"/>
+      <c r="C41" s="41" t="n"/>
+      <c r="L41" s="50" t="n"/>
+      <c r="N41" s="50" t="n"/>
+    </row>
+    <row r="42" ht="15" customHeight="1" s="107">
+      <c r="A42" s="41" t="n"/>
+      <c r="C42" s="124" t="inlineStr">
+        <is>
+          <t>2. Alternatively, you can create an RGA by logging in to https://clsnetlink.com</t>
+        </is>
+      </c>
+      <c r="L42" s="50" t="n"/>
+      <c r="N42" s="50" t="n"/>
+    </row>
+    <row r="43" ht="5" customHeight="1" s="107">
+      <c r="A43" s="41" t="n"/>
+      <c r="C43" s="41" t="n"/>
+      <c r="L43" s="50" t="n"/>
+      <c r="N43" s="50" t="n"/>
+    </row>
+    <row r="44" ht="31" customHeight="1" s="107">
+      <c r="A44" s="41" t="n"/>
+      <c r="C44" s="124" t="inlineStr">
+        <is>
+          <t>3. Upon receiving the Returned Goods Authorization Form (RGA), include the RGA along with the Packing Slip and ship the outdated products to the following address:</t>
+        </is>
+      </c>
+      <c r="L44" s="50" t="n"/>
+      <c r="N44" s="50" t="n"/>
+    </row>
+    <row r="45" ht="4" customHeight="1" s="107">
+      <c r="A45" s="41" t="n"/>
+      <c r="C45" s="41" t="n"/>
+      <c r="L45" s="50" t="n"/>
+      <c r="N45" s="50" t="n"/>
+    </row>
+    <row r="46" ht="18" customHeight="1" s="107">
+      <c r="A46" s="41" t="n"/>
+      <c r="C46" s="91" t="inlineStr">
+        <is>
+          <t>INMAR Pharmaceutical Services</t>
+        </is>
+      </c>
+      <c r="E46" s="61" t="n"/>
+      <c r="F46" s="61" t="n"/>
+      <c r="G46" s="61" t="n"/>
+      <c r="H46" s="61" t="n"/>
+      <c r="I46" s="61" t="n"/>
+      <c r="J46" s="61" t="n"/>
+      <c r="K46" s="61" t="n"/>
+      <c r="L46" s="62" t="n"/>
+      <c r="N46" s="50" t="n"/>
+    </row>
+    <row r="47" ht="17" customHeight="1" s="107">
+      <c r="A47" s="41" t="n"/>
+      <c r="C47" s="93" t="inlineStr">
+        <is>
+          <t>4332 Empire Road</t>
+        </is>
+      </c>
+      <c r="E47" s="61" t="n"/>
+      <c r="F47" s="61" t="n"/>
+      <c r="G47" s="61" t="n"/>
+      <c r="H47" s="61" t="n"/>
+      <c r="I47" s="61" t="n"/>
+      <c r="J47" s="61" t="n"/>
+      <c r="K47" s="61" t="n"/>
+      <c r="L47" s="62" t="n"/>
+      <c r="N47" s="50" t="n"/>
+    </row>
+    <row r="48" ht="18" customHeight="1" s="107">
+      <c r="A48" s="41" t="n"/>
+      <c r="C48" s="93" t="inlineStr">
+        <is>
+          <t>Fort Worth, TX 76155</t>
+        </is>
+      </c>
+      <c r="E48" s="61" t="n"/>
+      <c r="F48" s="61" t="n"/>
+      <c r="G48" s="61" t="n"/>
+      <c r="H48" s="61" t="n"/>
+      <c r="I48" s="61" t="n"/>
+      <c r="J48" s="61" t="n"/>
+      <c r="K48" s="61" t="n"/>
+      <c r="L48" s="62" t="n"/>
+      <c r="N48" s="50" t="n"/>
+    </row>
+    <row r="49" hidden="1" ht="18" customHeight="1" s="107">
+      <c r="A49" s="41" t="n"/>
+      <c r="C49" s="60" t="n"/>
+      <c r="D49" s="61" t="n"/>
+      <c r="E49" s="61" t="n"/>
+      <c r="F49" s="61" t="n"/>
+      <c r="G49" s="61" t="n"/>
+      <c r="H49" s="61" t="n"/>
+      <c r="I49" s="61" t="n"/>
+      <c r="J49" s="61" t="n"/>
+      <c r="K49" s="61" t="n"/>
+      <c r="L49" s="62" t="n"/>
+      <c r="N49" s="50" t="n"/>
+    </row>
+    <row r="50" ht="15" customHeight="1" s="107">
+      <c r="A50" s="41" t="n"/>
+      <c r="C50" s="125" t="inlineStr">
+        <is>
+          <t>Please DO NOT mix products from multiple debit memos/packing slips in one shipment. In case of any questions, please contact INMAR customer service at 1-800-967-5952</t>
+        </is>
+      </c>
+      <c r="L50" s="50" t="n"/>
+      <c r="N50" s="50" t="n"/>
+    </row>
+    <row r="51" ht="15" customHeight="1" s="107">
+      <c r="A51" s="41" t="n"/>
+      <c r="C51" s="41" t="n"/>
+      <c r="L51" s="50" t="n"/>
+      <c r="N51" s="50" t="n"/>
+    </row>
+    <row r="52" ht="15" customHeight="1" s="107">
+      <c r="A52" s="41" t="n"/>
+      <c r="C52" s="67" t="n"/>
+      <c r="D52" s="68" t="n"/>
+      <c r="E52" s="68" t="n"/>
+      <c r="F52" s="68" t="n"/>
+      <c r="G52" s="68" t="n"/>
+      <c r="H52" s="68" t="n"/>
+      <c r="I52" s="68" t="n"/>
+      <c r="J52" s="68" t="n"/>
+      <c r="K52" s="68" t="n"/>
+      <c r="L52" s="69" t="n"/>
+      <c r="N52" s="50" t="n"/>
+    </row>
+    <row r="53" ht="15" customHeight="1" s="107">
+      <c r="A53" s="41" t="n"/>
+      <c r="N53" s="50" t="n"/>
+    </row>
+    <row r="54" ht="15" customHeight="1" s="107">
+      <c r="A54" s="41" t="n"/>
+      <c r="N54" s="50" t="n"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1" s="107">
+      <c r="A55" s="55" t="n"/>
+      <c r="B55" s="32" t="n"/>
+      <c r="C55" s="32" t="n"/>
+      <c r="D55" s="32" t="n"/>
+      <c r="E55" s="32" t="n"/>
+      <c r="F55" s="32" t="n"/>
+      <c r="G55" s="32" t="n"/>
+      <c r="H55" s="32" t="n"/>
+      <c r="I55" s="32" t="n"/>
+      <c r="J55" s="32" t="n"/>
+      <c r="K55" s="32" t="n"/>
+      <c r="L55" s="32" t="n"/>
+      <c r="M55" s="32" t="n"/>
+      <c r="N55" s="51" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="39">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="D4:H5"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="C15:M15"/>
+    <mergeCell ref="C42:L43"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="C50:L51"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="C44:L45"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="C40:L41"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="E7:M7"/>
-    <mergeCell ref="B37:M37"/>
-    <mergeCell ref="C16:M16"/>
-    <mergeCell ref="B40:M40"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="E8:M8"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B39:M39"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B36:M36"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="D38:H38"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" scale="51"/>
   <headerFooter>
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12 &amp;K000000&amp;P</oddFooter>

</xml_diff>

<commit_message>
pricing added and excel became more accurate with few changes and added wholesaler and account data, need to cross check the data
</commit_message>
<xml_diff>
--- a/docs/invoice.xlsx
+++ b/docs/invoice.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice Template" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot;-&quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <name val="Arial"/>
       <color indexed="8"/>
@@ -174,13 +174,6 @@
       <u val="single"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-      <u val="single"/>
-    </font>
-    <font>
       <name val="Roboto"/>
       <color indexed="17"/>
       <sz val="12"/>
@@ -195,6 +188,18 @@
       <name val="Roboto"/>
       <b val="1"/>
       <color indexed="15"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <b val="1"/>
+      <color indexed="8"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Roboto"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
     </font>
   </fonts>
@@ -236,7 +241,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -493,30 +498,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="3"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="3"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -624,6 +605,34 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3"/>
+      </left>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color theme="3"/>
       </left>
@@ -641,39 +650,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top style="thin">
-        <color theme="3"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3"/>
-      </left>
-      <right style="thin">
-        <color theme="3"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -698,9 +679,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -840,153 +818,108 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="30" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="29" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="27" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="29" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="32"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="32"/>
-    </xf>
     <xf numFmtId="49" fontId="30" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="31" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2113,47 +2046,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="4.33203125" customWidth="1" style="107" min="1" max="1"/>
-    <col width="11.6640625" customWidth="1" style="107" min="2" max="2"/>
-    <col width="28.6640625" customWidth="1" style="107" min="3" max="3"/>
-    <col width="34" customWidth="1" style="107" min="4" max="4"/>
-    <col width="14.83203125" customWidth="1" style="107" min="5" max="5"/>
-    <col width="9" customWidth="1" style="107" min="6" max="6"/>
-    <col width="10.1640625" customWidth="1" style="107" min="7" max="7"/>
-    <col width="9.1640625" customWidth="1" style="107" min="8" max="8"/>
-    <col width="8.83203125" customWidth="1" style="107" min="9" max="9"/>
-    <col width="6.6640625" customWidth="1" style="107" min="10" max="10"/>
-    <col width="7.6640625" customWidth="1" style="107" min="11" max="11"/>
-    <col width="8.83203125" customWidth="1" style="107" min="12" max="12"/>
-    <col width="13.5" customWidth="1" style="107" min="13" max="13"/>
-    <col width="3.5" customWidth="1" style="107" min="14" max="14"/>
+    <col width="4.33203125" customWidth="1" style="74" min="1" max="1"/>
+    <col width="11.6640625" customWidth="1" style="74" min="2" max="2"/>
+    <col width="28.6640625" customWidth="1" style="74" min="3" max="3"/>
+    <col width="34" customWidth="1" style="74" min="4" max="4"/>
+    <col width="14.83203125" customWidth="1" style="74" min="5" max="5"/>
+    <col width="9" customWidth="1" style="74" min="6" max="6"/>
+    <col width="10.1640625" customWidth="1" style="74" min="7" max="7"/>
+    <col width="9.1640625" customWidth="1" style="74" min="8" max="8"/>
+    <col width="8.83203125" customWidth="1" style="74" min="9" max="9"/>
+    <col width="6.6640625" customWidth="1" style="74" min="10" max="10"/>
+    <col width="7.6640625" customWidth="1" style="74" min="11" max="11"/>
+    <col width="8.83203125" customWidth="1" style="74" min="12" max="12"/>
+    <col width="13.5" customWidth="1" style="74" min="13" max="13"/>
+    <col width="3.5" customWidth="1" style="74" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="107">
+    <row r="1" ht="14.25" customHeight="1" s="74">
       <c r="A1" s="1" t="n"/>
-      <c r="B1" s="33" t="n"/>
-      <c r="C1" s="34" t="n"/>
-      <c r="D1" s="34" t="n"/>
-      <c r="E1" s="34" t="n"/>
-      <c r="F1" s="34" t="n"/>
-      <c r="G1" s="34" t="n"/>
-      <c r="H1" s="34" t="n"/>
-      <c r="I1" s="34" t="n"/>
-      <c r="J1" s="34" t="n"/>
-      <c r="K1" s="34" t="n"/>
-      <c r="L1" s="34" t="n"/>
-      <c r="M1" s="35" t="n"/>
-      <c r="N1" s="36" t="n"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1" s="107">
+      <c r="B1" s="32" t="n"/>
+      <c r="C1" s="33" t="n"/>
+      <c r="D1" s="33" t="n"/>
+      <c r="E1" s="33" t="n"/>
+      <c r="F1" s="33" t="n"/>
+      <c r="G1" s="33" t="n"/>
+      <c r="H1" s="33" t="n"/>
+      <c r="I1" s="33" t="n"/>
+      <c r="J1" s="33" t="n"/>
+      <c r="K1" s="33" t="n"/>
+      <c r="L1" s="33" t="n"/>
+      <c r="M1" s="34" t="n"/>
+      <c r="N1" s="35" t="n"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1" s="74">
       <c r="A2" s="2" t="n"/>
       <c r="B2" s="3" t="n"/>
       <c r="C2" s="4" t="n"/>
@@ -2169,866 +2102,967 @@
       <c r="M2" s="5" t="n"/>
       <c r="N2" s="6" t="n"/>
     </row>
-    <row r="3" ht="73" customHeight="1" s="107" thickBot="1">
+    <row r="3" ht="73" customHeight="1" s="74" thickBot="1">
       <c r="A3" s="7" t="n"/>
-      <c r="B3" s="104" t="inlineStr">
+      <c r="B3" s="105" t="inlineStr">
         <is>
           <t>Manufacturer Packaging Slip</t>
         </is>
       </c>
       <c r="K3" s="9" t="n"/>
-      <c r="L3" s="9" t="n"/>
-      <c r="M3" s="10" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="N3" s="11" t="n"/>
-    </row>
-    <row r="4" ht="18" customHeight="1" s="107">
+      <c r="L3" s="111" t="inlineStr">
+        <is>
+          <t>Quick Returns</t>
+        </is>
+      </c>
+      <c r="M3" s="97" t="n"/>
+      <c r="N3" s="10" t="n"/>
+    </row>
+    <row r="4" ht="18" customHeight="1" s="74" thickBot="1">
       <c r="A4" s="7" t="n"/>
-      <c r="B4" s="70" t="inlineStr">
+      <c r="B4" s="69" t="inlineStr">
         <is>
           <t>DATE</t>
         </is>
       </c>
-      <c r="D4" s="113" t="n"/>
-      <c r="E4" s="114" t="n"/>
-      <c r="F4" s="114" t="n"/>
-      <c r="G4" s="114" t="n"/>
-      <c r="H4" s="115" t="n"/>
-      <c r="I4" s="82" t="n"/>
-      <c r="J4" s="82" t="n"/>
-      <c r="K4" s="82" t="n"/>
-      <c r="L4" s="116" t="inlineStr">
+      <c r="D4" s="76" t="n"/>
+      <c r="E4" s="77" t="n"/>
+      <c r="F4" s="77" t="n"/>
+      <c r="G4" s="77" t="n"/>
+      <c r="H4" s="78" t="n"/>
+      <c r="I4" s="87" t="n"/>
+      <c r="J4" s="87" t="n"/>
+      <c r="K4" s="87" t="n"/>
+      <c r="L4" s="101" t="inlineStr">
         <is>
           <t>INVOICE NO:</t>
         </is>
       </c>
-      <c r="M4" s="117" t="n"/>
-      <c r="N4" s="12" t="n"/>
-    </row>
-    <row r="5" ht="18" customHeight="1" s="107" thickBot="1">
+      <c r="M4" s="102" t="n"/>
+      <c r="N4" s="11" t="n"/>
+    </row>
+    <row r="5" ht="18" customHeight="1" s="74" thickBot="1">
       <c r="A5" s="7" t="n"/>
-      <c r="B5" s="71" t="inlineStr">
-        <is>
-          <t>01/12/2024</t>
-        </is>
-      </c>
-      <c r="D5" s="118" t="n"/>
-      <c r="E5" s="119" t="n"/>
-      <c r="F5" s="119" t="n"/>
-      <c r="G5" s="119" t="n"/>
-      <c r="H5" s="120" t="n"/>
-      <c r="I5" s="82" t="n"/>
-      <c r="J5" s="82" t="n"/>
-      <c r="K5" s="82" t="n"/>
-      <c r="L5" s="121" t="n"/>
-      <c r="M5" s="122" t="n"/>
-      <c r="N5" s="15" t="n"/>
-    </row>
-    <row r="6" ht="18" customHeight="1" s="107">
+      <c r="B5" s="70" t="inlineStr">
+        <is>
+          <t>01/15/2024</t>
+        </is>
+      </c>
+      <c r="D5" s="79" t="n"/>
+      <c r="E5" s="80" t="n"/>
+      <c r="F5" s="80" t="n"/>
+      <c r="G5" s="80" t="n"/>
+      <c r="H5" s="81" t="n"/>
+      <c r="I5" s="87" t="n"/>
+      <c r="J5" s="87" t="n"/>
+      <c r="K5" s="87" t="n"/>
+      <c r="L5" s="94" t="inlineStr">
+        <is>
+          <t>QR01152024AP201</t>
+        </is>
+      </c>
+      <c r="M5" s="95" t="n"/>
+      <c r="N5" s="14" t="n"/>
+    </row>
+    <row r="6" ht="18" customHeight="1" s="74">
       <c r="A6" s="7" t="n"/>
-      <c r="D6" s="83" t="n"/>
-      <c r="E6" s="106" t="n"/>
-      <c r="N6" s="16" t="n"/>
-    </row>
-    <row r="7" ht="22.5" customHeight="1" s="107">
+      <c r="D6" s="73" t="n"/>
+      <c r="E6" s="88" t="n"/>
+      <c r="N6" s="15" t="n"/>
+    </row>
+    <row r="7" ht="22.5" customHeight="1" s="74">
       <c r="A7" s="7" t="n"/>
-      <c r="D7" s="83" t="n"/>
-      <c r="E7" s="111" t="n"/>
-      <c r="N7" s="17" t="n"/>
-    </row>
-    <row r="8" ht="26.25" customHeight="1" s="107">
+      <c r="D7" s="73" t="n"/>
+      <c r="E7" s="99" t="n"/>
+      <c r="N7" s="16" t="n"/>
+    </row>
+    <row r="8" ht="26.25" customHeight="1" s="74">
       <c r="A8" s="7" t="n"/>
-      <c r="B8" s="105" t="inlineStr">
+      <c r="B8" s="96" t="inlineStr">
         <is>
           <t>Account:</t>
         </is>
       </c>
-      <c r="C8" s="123" t="n"/>
-      <c r="D8" s="105" t="inlineStr">
+      <c r="C8" s="97" t="n"/>
+      <c r="D8" s="96" t="inlineStr">
         <is>
           <t>Wholesaler:</t>
         </is>
       </c>
-      <c r="E8" s="80" t="inlineStr">
+      <c r="E8" s="106" t="inlineStr">
         <is>
           <t>Issue Credit to:</t>
         </is>
       </c>
-      <c r="F8" s="123" t="n"/>
-      <c r="G8" s="123" t="n"/>
-      <c r="H8" s="100" t="n"/>
-      <c r="L8" s="66" t="n"/>
-      <c r="M8" s="66" t="n"/>
-      <c r="N8" s="18" t="n"/>
-    </row>
-    <row r="9" ht="8" customHeight="1" s="107">
+      <c r="F8" s="97" t="n"/>
+      <c r="G8" s="97" t="n"/>
+      <c r="H8" s="93" t="n"/>
+      <c r="L8" s="65" t="n"/>
+      <c r="M8" s="65" t="n"/>
+      <c r="N8" s="17" t="n"/>
+    </row>
+    <row r="9" ht="8" customHeight="1" s="74">
       <c r="A9" s="7" t="n"/>
-      <c r="B9" s="82" t="n"/>
-      <c r="D9" s="39" t="n"/>
-      <c r="E9" s="82" t="n"/>
-      <c r="H9" s="39" t="n"/>
-      <c r="I9" s="39" t="n"/>
-      <c r="J9" s="39" t="n"/>
-      <c r="K9" s="39" t="n"/>
-      <c r="L9" s="82" t="n"/>
-      <c r="M9" s="82" t="n"/>
-      <c r="N9" s="19" t="n"/>
-    </row>
-    <row r="10" ht="18" customHeight="1" s="107">
-      <c r="A10" s="52" t="n"/>
-      <c r="B10" s="99" t="inlineStr">
-        <is>
-          <t>Proud Pharmaceuticals</t>
-        </is>
-      </c>
-      <c r="D10" s="99" t="inlineStr">
-        <is>
-          <t>Cardinal Health</t>
-        </is>
-      </c>
-      <c r="E10" s="83" t="inlineStr">
-        <is>
-          <t>Proud Pharmaceuticals</t>
-        </is>
-      </c>
-      <c r="H10" s="101" t="n"/>
-      <c r="L10" s="83" t="n"/>
-      <c r="M10" s="83" t="n"/>
-      <c r="N10" s="20" t="n"/>
-    </row>
-    <row r="11" ht="18" customHeight="1" s="107">
-      <c r="A11" s="52" t="n"/>
-      <c r="B11" s="99" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="D11" s="99" t="inlineStr">
-        <is>
-          <t>Acd</t>
-        </is>
-      </c>
-      <c r="E11" s="83" t="inlineStr">
-        <is>
-          <t>Testing</t>
-        </is>
-      </c>
-      <c r="H11" s="102" t="n"/>
-      <c r="L11" s="83" t="n"/>
-      <c r="M11" s="83" t="n"/>
-      <c r="N11" s="20" t="n"/>
-    </row>
-    <row r="12" ht="18" customHeight="1" s="107">
-      <c r="A12" s="52" t="n"/>
-      <c r="B12" s="99" t="inlineStr">
-        <is>
-          <t>5960 East Shelby Drive, Suite 100</t>
-        </is>
-      </c>
-      <c r="D12" s="99" t="inlineStr">
-        <is>
-          <t>7000 Cardinal Place</t>
-        </is>
-      </c>
-      <c r="E12" s="83" t="inlineStr">
-        <is>
-          <t>5960 East Shelby Drive, Suite 100</t>
-        </is>
-      </c>
-      <c r="H12" s="102" t="n"/>
-      <c r="L12" s="83" t="n"/>
-      <c r="M12" s="83" t="n"/>
-      <c r="N12" s="20" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="107">
-      <c r="A13" s="52" t="n"/>
-      <c r="B13" s="99" t="inlineStr">
-        <is>
-          <t>(800) 727-6331</t>
-        </is>
-      </c>
-      <c r="D13" s="99" t="inlineStr">
-        <is>
-          <t>(800) 926-3161</t>
-        </is>
-      </c>
-      <c r="E13" s="83" t="inlineStr">
-        <is>
-          <t>(800) 727-6331</t>
-        </is>
-      </c>
-      <c r="H13" s="102" t="n"/>
-      <c r="L13" s="83" t="n"/>
-      <c r="M13" s="83" t="n"/>
-      <c r="N13" s="20" t="n"/>
-    </row>
-    <row r="14" ht="18" customHeight="1" s="107">
-      <c r="A14" s="52" t="n"/>
-      <c r="B14" s="99" t="inlineStr">
-        <is>
-          <t>chris.dewitt@parmedpharm.com</t>
-        </is>
-      </c>
-      <c r="D14" s="83" t="n"/>
-      <c r="E14" s="83" t="inlineStr">
-        <is>
-          <t>chris.dewitt@parmedpharm.com</t>
-        </is>
-      </c>
-      <c r="H14" s="103" t="n"/>
-      <c r="L14" s="83" t="n"/>
-      <c r="M14" s="83" t="n"/>
-      <c r="N14" s="20" t="n"/>
-    </row>
-    <row r="15" ht="18" customHeight="1" s="107">
-      <c r="A15" s="52" t="n"/>
-      <c r="B15" s="83" t="n"/>
-      <c r="C15" s="108" t="n"/>
-      <c r="N15" s="15" t="n"/>
-    </row>
-    <row r="16" ht="8" customHeight="1" s="107">
-      <c r="A16" s="52" t="n"/>
-      <c r="B16" s="82" t="n"/>
-      <c r="C16" s="82" t="n"/>
-      <c r="D16" s="82" t="n"/>
-      <c r="E16" s="82" t="n"/>
-      <c r="F16" s="82" t="n"/>
-      <c r="G16" s="82" t="n"/>
-      <c r="H16" s="82" t="n"/>
-      <c r="I16" s="82" t="n"/>
-      <c r="J16" s="82" t="n"/>
-      <c r="K16" s="82" t="n"/>
-      <c r="L16" s="82" t="n"/>
-      <c r="M16" s="82" t="n"/>
+      <c r="B9" s="87" t="n"/>
+      <c r="D9" s="108" t="n"/>
+      <c r="E9" s="87" t="n"/>
+      <c r="H9" s="108" t="n"/>
+      <c r="I9" s="108" t="n"/>
+      <c r="J9" s="108" t="n"/>
+      <c r="K9" s="108" t="n"/>
+      <c r="L9" s="87" t="n"/>
+      <c r="M9" s="87" t="n"/>
+      <c r="N9" s="18" t="n"/>
+    </row>
+    <row r="10" ht="18" customHeight="1" s="74">
+      <c r="A10" s="51" t="n"/>
+      <c r="B10" s="109" t="inlineStr">
+        <is>
+          <t>AUTREY PHARMACY 2</t>
+        </is>
+      </c>
+      <c r="D10" s="12" t="inlineStr">
+        <is>
+          <t>AMERISOURCEBERGEN DRUG CORPORATION</t>
+        </is>
+      </c>
+      <c r="E10" s="73" t="inlineStr">
+        <is>
+          <t>AUTREY PHARMACY 2</t>
+        </is>
+      </c>
+      <c r="H10" s="98" t="n"/>
+      <c r="L10" s="73" t="n"/>
+      <c r="M10" s="73" t="n"/>
+      <c r="N10" s="19" t="n"/>
+    </row>
+    <row r="11" ht="18" customHeight="1" s="74">
+      <c r="A11" s="51" t="n"/>
+      <c r="B11" s="109" t="inlineStr">
+        <is>
+          <t>1365 E RUBEN TORRES BLVD</t>
+        </is>
+      </c>
+      <c r="D11" s="12" t="inlineStr">
+        <is>
+          <t>108 ROUTE 17K SUITE 1</t>
+        </is>
+      </c>
+      <c r="E11" s="73" t="inlineStr">
+        <is>
+          <t>1365 E RUBEN TORRES BLVD</t>
+        </is>
+      </c>
+      <c r="H11" s="75" t="n"/>
+      <c r="L11" s="73" t="n"/>
+      <c r="M11" s="73" t="n"/>
+      <c r="N11" s="19" t="n"/>
+    </row>
+    <row r="12" ht="18" customHeight="1" s="74">
+      <c r="A12" s="51" t="n"/>
+      <c r="B12" s="109" t="inlineStr">
+        <is>
+          <t>BROWNSVILLE, TX 78521</t>
+        </is>
+      </c>
+      <c r="D12" s="12" t="inlineStr">
+        <is>
+          <t>NEWBURGH. NY, 12550-5008</t>
+        </is>
+      </c>
+      <c r="E12" s="73" t="inlineStr">
+        <is>
+          <t>BROWNSVILLE, TX 78521</t>
+        </is>
+      </c>
+      <c r="H12" s="75" t="n"/>
+      <c r="L12" s="73" t="n"/>
+      <c r="M12" s="73" t="n"/>
+      <c r="N12" s="19" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="74">
+      <c r="A13" s="51" t="n"/>
+      <c r="B13" s="109" t="inlineStr">
+        <is>
+          <t>EC</t>
+        </is>
+      </c>
+      <c r="D13" s="12" t="inlineStr">
+        <is>
+          <t>Account#: 100199545</t>
+        </is>
+      </c>
+      <c r="E13" s="73" t="inlineStr">
+        <is>
+          <t>EC</t>
+        </is>
+      </c>
+      <c r="H13" s="75" t="n"/>
+      <c r="L13" s="73" t="n"/>
+      <c r="M13" s="73" t="n"/>
+      <c r="N13" s="19" t="n"/>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="74">
+      <c r="A14" s="51" t="n"/>
+      <c r="B14" s="109" t="inlineStr">
+        <is>
+          <t>Phone: 956-542-5100, fax: 956-542-5103</t>
+        </is>
+      </c>
+      <c r="D14" s="73" t="inlineStr">
+        <is>
+          <t>Phone: 844-222-2273</t>
+        </is>
+      </c>
+      <c r="E14" s="73" t="inlineStr">
+        <is>
+          <t>Phone: 956-542-5100, fax: 956-542-5103</t>
+        </is>
+      </c>
+      <c r="H14" s="90" t="n"/>
+      <c r="L14" s="73" t="n"/>
+      <c r="M14" s="73" t="n"/>
+      <c r="N14" s="19" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="74">
+      <c r="A15" s="51" t="n"/>
+      <c r="B15" s="109" t="inlineStr">
+        <is>
+          <t>DEA: FA3706895, Exp: 06/30/2023</t>
+        </is>
+      </c>
+      <c r="D15" s="73" t="inlineStr">
+        <is>
+          <t>DEA: RA0522056</t>
+        </is>
+      </c>
+      <c r="E15" s="73" t="inlineStr">
+        <is>
+          <t>DEA: FA3706895, Exp: 06/30/2023</t>
+        </is>
+      </c>
+      <c r="H15" s="90" t="n"/>
+      <c r="L15" s="73" t="n"/>
+      <c r="M15" s="73" t="n"/>
+      <c r="N15" s="19" t="n"/>
+    </row>
+    <row r="16" ht="18" customFormat="1" customHeight="1" s="108">
+      <c r="A16" s="51" t="n"/>
+      <c r="B16" s="109" t="inlineStr">
+        <is>
+          <t>Authorized Classes: 2, 2N, 3, 3N, 4. 5</t>
+        </is>
+      </c>
+      <c r="D16" s="73" t="n"/>
+      <c r="E16" s="73" t="inlineStr">
+        <is>
+          <t>Authorized Classes: 2, 2N, 3, 3N, 4. 5</t>
+        </is>
+      </c>
+      <c r="H16" s="90" t="n"/>
+      <c r="L16" s="73" t="n"/>
+      <c r="M16" s="73" t="n"/>
       <c r="N16" s="19" t="n"/>
     </row>
-    <row r="17" ht="25" customHeight="1" s="107">
-      <c r="A17" s="52" t="n"/>
-      <c r="B17" s="42" t="inlineStr">
+    <row r="17" ht="18" customHeight="1" s="74">
+      <c r="A17" s="51" t="n"/>
+      <c r="B17" s="73" t="n"/>
+      <c r="C17" s="86" t="n"/>
+      <c r="N17" s="14" t="n"/>
+    </row>
+    <row r="18" ht="8" customHeight="1" s="74">
+      <c r="A18" s="51" t="n"/>
+      <c r="B18" s="87" t="n"/>
+      <c r="C18" s="87" t="n"/>
+      <c r="D18" s="87" t="n"/>
+      <c r="E18" s="87" t="n"/>
+      <c r="F18" s="87" t="n"/>
+      <c r="G18" s="87" t="n"/>
+      <c r="H18" s="87" t="n"/>
+      <c r="I18" s="87" t="n"/>
+      <c r="J18" s="87" t="n"/>
+      <c r="K18" s="87" t="n"/>
+      <c r="L18" s="87" t="n"/>
+      <c r="M18" s="87" t="n"/>
+      <c r="N18" s="18" t="n"/>
+    </row>
+    <row r="19" ht="25" customHeight="1" s="74">
+      <c r="A19" s="51" t="n"/>
+      <c r="B19" s="41" t="inlineStr">
         <is>
           <t>NDC/UPC</t>
         </is>
       </c>
-      <c r="C17" s="42" t="inlineStr">
+      <c r="C19" s="41" t="inlineStr">
         <is>
           <t>Manufacturer</t>
         </is>
       </c>
-      <c r="D17" s="42" t="inlineStr">
+      <c r="D19" s="41" t="inlineStr">
         <is>
           <t>Product name</t>
         </is>
       </c>
-      <c r="E17" s="42" t="inlineStr">
+      <c r="E19" s="41" t="inlineStr">
         <is>
           <t>Strength</t>
         </is>
       </c>
-      <c r="F17" s="42" t="inlineStr">
+      <c r="F19" s="41" t="inlineStr">
         <is>
           <t>DSG</t>
         </is>
       </c>
-      <c r="G17" s="42" t="inlineStr">
+      <c r="G19" s="41" t="inlineStr">
         <is>
           <t>Lot</t>
         </is>
       </c>
-      <c r="H17" s="42" t="inlineStr">
+      <c r="H19" s="41" t="inlineStr">
         <is>
           <t>Exp</t>
         </is>
       </c>
-      <c r="I17" s="42" t="inlineStr">
+      <c r="I19" s="41" t="inlineStr">
         <is>
           <t>Pkg Size</t>
         </is>
       </c>
-      <c r="J17" s="42" t="inlineStr">
+      <c r="J19" s="41" t="inlineStr">
         <is>
           <t>Full Qty</t>
         </is>
       </c>
-      <c r="K17" s="59" t="inlineStr">
+      <c r="K19" s="58" t="inlineStr">
         <is>
           <t>Partial Qty</t>
         </is>
       </c>
-      <c r="L17" s="42" t="inlineStr">
+      <c r="L19" s="41" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="M17" s="42" t="inlineStr">
+      <c r="M19" s="41" t="inlineStr">
         <is>
           <t>Est Value</t>
         </is>
       </c>
-      <c r="N17" s="12" t="n"/>
-    </row>
-    <row r="18" ht="18" customHeight="1" s="107">
-      <c r="A18" s="53" t="n"/>
-      <c r="B18" s="43" t="inlineStr">
-        <is>
-          <t>5511153205</t>
-        </is>
-      </c>
-      <c r="C18" s="44" t="inlineStr">
-        <is>
-          <t>Dr. Reddy's Laboratories Ltd</t>
-        </is>
-      </c>
-      <c r="D18" s="44" t="inlineStr">
-        <is>
-          <t>Divalproex sodium</t>
-        </is>
-      </c>
-      <c r="E18" s="45" t="inlineStr">
-        <is>
-          <t>125 mg/1</t>
-        </is>
-      </c>
-      <c r="F18" s="45" t="inlineStr">
-        <is>
-          <t>CAPSULE</t>
-        </is>
-      </c>
-      <c r="G18" s="45" t="inlineStr">
-        <is>
-          <t>C2115420</t>
-        </is>
-      </c>
-      <c r="H18" s="45" t="inlineStr">
-        <is>
-          <t>10/23/31</t>
-        </is>
-      </c>
-      <c r="I18" s="45" t="inlineStr">
+      <c r="N19" s="11" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1" s="74">
+      <c r="A20" s="52" t="n"/>
+      <c r="B20" s="42" t="inlineStr">
+        <is>
+          <t>6818024906</t>
+        </is>
+      </c>
+      <c r="C20" s="43" t="inlineStr">
+        <is>
+          <t>Lupin Pharmaceuticals, Inc.</t>
+        </is>
+      </c>
+      <c r="D20" s="43" t="inlineStr">
+        <is>
+          <t>memantine hydrochloride</t>
+        </is>
+      </c>
+      <c r="E20" s="44" t="inlineStr">
+        <is>
+          <t>28 mg/1</t>
+        </is>
+      </c>
+      <c r="F20" s="44" t="inlineStr">
+        <is>
+          <t>CAPSULE, EXTENDED RELEASE</t>
+        </is>
+      </c>
+      <c r="G20" s="44" t="inlineStr">
+        <is>
+          <t>H102306</t>
+        </is>
+      </c>
+      <c r="H20" s="44" t="inlineStr">
+        <is>
+          <t>09/23/30</t>
+        </is>
+      </c>
+      <c r="I20" s="44" t="inlineStr">
+        <is>
+          <t>30 CT</t>
+        </is>
+      </c>
+      <c r="J20" s="44" t="n">
+        <v>4</v>
+      </c>
+      <c r="K20" s="44" t="n"/>
+      <c r="L20" s="44" t="n">
+        <v>35</v>
+      </c>
+      <c r="M20" s="44" t="n">
+        <v>140</v>
+      </c>
+      <c r="N20" s="22" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="74">
+      <c r="A21" s="52" t="n"/>
+      <c r="B21" s="45" t="inlineStr">
+        <is>
+          <t>6787743305</t>
+        </is>
+      </c>
+      <c r="C21" s="46" t="inlineStr">
+        <is>
+          <t>Ascend Laboratories, LLC</t>
+        </is>
+      </c>
+      <c r="D21" s="46" t="inlineStr">
+        <is>
+          <t>Aripiprazole</t>
+        </is>
+      </c>
+      <c r="E21" s="47" t="inlineStr">
+        <is>
+          <t>15 mg/1</t>
+        </is>
+      </c>
+      <c r="F21" s="47" t="inlineStr">
+        <is>
+          <t>TABLET</t>
+        </is>
+      </c>
+      <c r="G21" s="47" t="inlineStr">
+        <is>
+          <t>22140477</t>
+        </is>
+      </c>
+      <c r="H21" s="47" t="inlineStr">
+        <is>
+          <t>01/24/31</t>
+        </is>
+      </c>
+      <c r="I21" s="47" t="inlineStr">
         <is>
           <t>500 CT</t>
         </is>
       </c>
-      <c r="J18" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="K18" s="45" t="n"/>
-      <c r="L18" s="45" t="n"/>
-      <c r="M18" s="45" t="n"/>
-      <c r="N18" s="23" t="n"/>
-    </row>
-    <row r="19" ht="18" customHeight="1" s="107">
-      <c r="A19" s="53" t="n"/>
-      <c r="B19" s="46" t="n"/>
-      <c r="C19" s="47" t="n"/>
-      <c r="D19" s="47" t="n"/>
-      <c r="E19" s="48" t="n"/>
-      <c r="F19" s="48" t="n"/>
-      <c r="G19" s="48" t="n"/>
-      <c r="H19" s="48" t="n"/>
-      <c r="I19" s="48" t="n"/>
-      <c r="J19" s="48" t="n"/>
-      <c r="K19" s="48" t="n"/>
-      <c r="M19" s="48" t="n"/>
-      <c r="N19" s="23" t="n"/>
-    </row>
-    <row r="20" ht="18" customHeight="1" s="107">
-      <c r="A20" s="53" t="n"/>
-      <c r="B20" s="43" t="n"/>
-      <c r="C20" s="44" t="n"/>
-      <c r="D20" s="44" t="n"/>
-      <c r="E20" s="45" t="n"/>
-      <c r="F20" s="45" t="n"/>
-      <c r="G20" s="45" t="n"/>
-      <c r="H20" s="45" t="n"/>
-      <c r="I20" s="45" t="n"/>
-      <c r="J20" s="45" t="n"/>
-      <c r="K20" s="45" t="n"/>
-      <c r="L20" s="48" t="n"/>
-      <c r="M20" s="45" t="n"/>
-      <c r="N20" s="23" t="n"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" s="107">
-      <c r="A21" s="53" t="n"/>
-      <c r="B21" s="46" t="n"/>
-      <c r="C21" s="47" t="n"/>
-      <c r="D21" s="47" t="n"/>
-      <c r="E21" s="48" t="n"/>
-      <c r="F21" s="48" t="n"/>
-      <c r="G21" s="48" t="n"/>
-      <c r="H21" s="48" t="n"/>
-      <c r="I21" s="48" t="n"/>
-      <c r="J21" s="48" t="n"/>
-      <c r="K21" s="48" t="n"/>
-      <c r="L21" s="48" t="n"/>
-      <c r="M21" s="48" t="n"/>
-      <c r="N21" s="23" t="n"/>
-    </row>
-    <row r="22" ht="18" customHeight="1" s="107">
-      <c r="A22" s="53" t="n"/>
-      <c r="B22" s="43" t="n"/>
-      <c r="C22" s="44" t="n"/>
-      <c r="D22" s="44" t="n"/>
-      <c r="E22" s="45" t="n"/>
-      <c r="F22" s="45" t="n"/>
-      <c r="G22" s="45" t="n"/>
-      <c r="H22" s="45" t="n"/>
-      <c r="I22" s="45" t="n"/>
-      <c r="J22" s="45" t="n"/>
-      <c r="K22" s="45" t="n"/>
-      <c r="L22" s="45" t="n"/>
-      <c r="M22" s="45" t="n"/>
-      <c r="N22" s="23" t="n"/>
-    </row>
-    <row r="23" ht="18" customHeight="1" s="107">
-      <c r="A23" s="53" t="n"/>
-      <c r="B23" s="46" t="n"/>
-      <c r="C23" s="47" t="n"/>
-      <c r="D23" s="47" t="n"/>
-      <c r="E23" s="48" t="n"/>
-      <c r="F23" s="48" t="n"/>
-      <c r="G23" s="48" t="n"/>
-      <c r="H23" s="48" t="n"/>
-      <c r="I23" s="48" t="n"/>
-      <c r="J23" s="48" t="n"/>
-      <c r="K23" s="48" t="n"/>
-      <c r="L23" s="48" t="n"/>
-      <c r="M23" s="48" t="n"/>
-      <c r="N23" s="23" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="107">
-      <c r="A24" s="53" t="n"/>
-      <c r="B24" s="43" t="n"/>
-      <c r="C24" s="44" t="n"/>
-      <c r="D24" s="44" t="n"/>
-      <c r="E24" s="45" t="n"/>
-      <c r="F24" s="45" t="n"/>
-      <c r="G24" s="45" t="n"/>
-      <c r="H24" s="45" t="n"/>
-      <c r="I24" s="45" t="n"/>
-      <c r="J24" s="45" t="n"/>
-      <c r="K24" s="45" t="n"/>
-      <c r="L24" s="45" t="n"/>
-      <c r="M24" s="45" t="n"/>
-      <c r="N24" s="23" t="n"/>
-    </row>
-    <row r="25" ht="18" customHeight="1" s="107">
-      <c r="A25" s="53" t="n"/>
-      <c r="B25" s="46" t="n"/>
-      <c r="C25" s="47" t="n"/>
-      <c r="D25" s="47" t="n"/>
-      <c r="E25" s="48" t="n"/>
-      <c r="F25" s="48" t="n"/>
-      <c r="G25" s="48" t="n"/>
-      <c r="H25" s="48" t="n"/>
-      <c r="I25" s="48" t="n"/>
-      <c r="J25" s="48" t="n"/>
-      <c r="K25" s="48" t="n"/>
-      <c r="L25" s="48" t="n"/>
-      <c r="M25" s="48" t="n"/>
-      <c r="N25" s="23" t="n"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" s="107">
-      <c r="A26" s="53" t="n"/>
-      <c r="B26" s="43" t="n"/>
-      <c r="C26" s="44" t="n"/>
-      <c r="D26" s="44" t="n"/>
-      <c r="E26" s="45" t="n"/>
-      <c r="F26" s="45" t="n"/>
-      <c r="G26" s="45" t="n"/>
-      <c r="H26" s="45" t="n"/>
-      <c r="I26" s="45" t="n"/>
-      <c r="J26" s="45" t="n"/>
-      <c r="K26" s="45" t="n"/>
-      <c r="L26" s="45" t="n"/>
-      <c r="M26" s="45" t="n"/>
-      <c r="N26" s="23" t="n"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" s="107">
-      <c r="A27" s="53" t="n"/>
-      <c r="B27" s="46" t="n"/>
-      <c r="C27" s="47" t="n"/>
-      <c r="D27" s="47" t="n"/>
-      <c r="E27" s="48" t="n"/>
-      <c r="F27" s="48" t="n"/>
-      <c r="G27" s="48" t="n"/>
-      <c r="H27" s="48" t="n"/>
-      <c r="I27" s="48" t="n"/>
-      <c r="J27" s="48" t="n"/>
-      <c r="K27" s="48" t="n"/>
-      <c r="L27" s="48" t="n"/>
-      <c r="M27" s="48" t="n"/>
-      <c r="N27" s="23" t="n"/>
-    </row>
-    <row r="28" ht="18" customFormat="1" customHeight="1" s="39">
-      <c r="A28" s="53" t="n"/>
-      <c r="B28" s="43" t="n"/>
-      <c r="C28" s="44" t="n"/>
-      <c r="D28" s="44" t="n"/>
-      <c r="E28" s="45" t="n"/>
-      <c r="F28" s="45" t="n"/>
-      <c r="G28" s="45" t="n"/>
-      <c r="H28" s="45" t="n"/>
-      <c r="I28" s="45" t="n"/>
-      <c r="J28" s="45" t="n"/>
-      <c r="K28" s="45" t="n"/>
-      <c r="L28" s="45" t="n"/>
-      <c r="M28" s="45" t="n"/>
-      <c r="N28" s="23" t="n"/>
-    </row>
-    <row r="29" ht="18" customFormat="1" customHeight="1" s="39">
-      <c r="A29" s="53" t="n"/>
-      <c r="B29" s="46" t="n"/>
-      <c r="C29" s="47" t="n"/>
-      <c r="D29" s="47" t="n"/>
-      <c r="E29" s="48" t="n"/>
-      <c r="F29" s="48" t="n"/>
-      <c r="G29" s="48" t="n"/>
-      <c r="H29" s="48" t="n"/>
-      <c r="I29" s="48" t="n"/>
-      <c r="J29" s="48" t="n"/>
-      <c r="K29" s="48" t="n"/>
-      <c r="L29" s="48" t="n"/>
-      <c r="M29" s="48" t="n"/>
-      <c r="N29" s="23" t="n"/>
-    </row>
-    <row r="30" ht="18" customHeight="1" s="107">
-      <c r="A30" s="53" t="n"/>
-      <c r="B30" s="37" t="n"/>
-      <c r="C30" s="21" t="n"/>
-      <c r="D30" s="21" t="n"/>
-      <c r="E30" s="22" t="n"/>
-      <c r="F30" s="22" t="n"/>
-      <c r="G30" s="22" t="n"/>
-      <c r="H30" s="22" t="n"/>
-      <c r="I30" s="22" t="n"/>
-      <c r="J30" s="22" t="n"/>
-      <c r="K30" s="22" t="n"/>
-      <c r="L30" s="22" t="n"/>
-      <c r="M30" s="22" t="n"/>
-      <c r="N30" s="23" t="n"/>
-    </row>
-    <row r="31" ht="26" customHeight="1" s="107">
+      <c r="J21" s="47" t="n">
+        <v>35</v>
+      </c>
+      <c r="K21" s="47" t="n"/>
+      <c r="L21" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="M21" s="47" t="n">
+        <v>66.15000000000001</v>
+      </c>
+      <c r="N21" s="22" t="n"/>
+    </row>
+    <row r="22" ht="18" customHeight="1" s="74">
+      <c r="A22" s="52" t="n"/>
+      <c r="B22" s="42" t="n"/>
+      <c r="C22" s="43" t="n"/>
+      <c r="D22" s="43" t="n"/>
+      <c r="E22" s="44" t="n"/>
+      <c r="F22" s="44" t="n"/>
+      <c r="G22" s="44" t="n"/>
+      <c r="H22" s="44" t="n"/>
+      <c r="I22" s="44" t="n"/>
+      <c r="J22" s="44" t="n"/>
+      <c r="K22" s="44" t="n"/>
+      <c r="L22" s="47" t="n"/>
+      <c r="M22" s="44" t="n"/>
+      <c r="N22" s="22" t="n"/>
+    </row>
+    <row r="23" ht="18" customHeight="1" s="74">
+      <c r="A23" s="52" t="n"/>
+      <c r="B23" s="45" t="n"/>
+      <c r="C23" s="46" t="n"/>
+      <c r="D23" s="46" t="n"/>
+      <c r="E23" s="47" t="n"/>
+      <c r="F23" s="47" t="n"/>
+      <c r="G23" s="47" t="n"/>
+      <c r="H23" s="47" t="n"/>
+      <c r="I23" s="47" t="n"/>
+      <c r="J23" s="47" t="n"/>
+      <c r="K23" s="47" t="n"/>
+      <c r="L23" s="47" t="n"/>
+      <c r="M23" s="47" t="n"/>
+      <c r="N23" s="22" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="74">
+      <c r="A24" s="52" t="n"/>
+      <c r="B24" s="42" t="n"/>
+      <c r="C24" s="43" t="n"/>
+      <c r="D24" s="43" t="n"/>
+      <c r="E24" s="44" t="n"/>
+      <c r="F24" s="44" t="n"/>
+      <c r="G24" s="44" t="n"/>
+      <c r="H24" s="44" t="n"/>
+      <c r="I24" s="44" t="n"/>
+      <c r="J24" s="44" t="n"/>
+      <c r="K24" s="44" t="n"/>
+      <c r="L24" s="44" t="n"/>
+      <c r="M24" s="44" t="n"/>
+      <c r="N24" s="22" t="n"/>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="74">
+      <c r="A25" s="52" t="n"/>
+      <c r="B25" s="45" t="n"/>
+      <c r="C25" s="46" t="n"/>
+      <c r="D25" s="46" t="n"/>
+      <c r="E25" s="47" t="n"/>
+      <c r="F25" s="47" t="n"/>
+      <c r="G25" s="47" t="n"/>
+      <c r="H25" s="47" t="n"/>
+      <c r="I25" s="47" t="n"/>
+      <c r="J25" s="47" t="n"/>
+      <c r="K25" s="47" t="n"/>
+      <c r="L25" s="47" t="n"/>
+      <c r="M25" s="47" t="n"/>
+      <c r="N25" s="22" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="74">
+      <c r="A26" s="52" t="n"/>
+      <c r="B26" s="42" t="n"/>
+      <c r="C26" s="43" t="n"/>
+      <c r="D26" s="43" t="n"/>
+      <c r="E26" s="44" t="n"/>
+      <c r="F26" s="44" t="n"/>
+      <c r="G26" s="44" t="n"/>
+      <c r="H26" s="44" t="n"/>
+      <c r="I26" s="44" t="n"/>
+      <c r="J26" s="44" t="n"/>
+      <c r="K26" s="44" t="n"/>
+      <c r="L26" s="44" t="n"/>
+      <c r="M26" s="44" t="n"/>
+      <c r="N26" s="22" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="74">
+      <c r="A27" s="52" t="n"/>
+      <c r="B27" s="45" t="n"/>
+      <c r="C27" s="46" t="n"/>
+      <c r="D27" s="46" t="n"/>
+      <c r="E27" s="47" t="n"/>
+      <c r="F27" s="47" t="n"/>
+      <c r="G27" s="47" t="n"/>
+      <c r="H27" s="47" t="n"/>
+      <c r="I27" s="47" t="n"/>
+      <c r="J27" s="47" t="n"/>
+      <c r="K27" s="47" t="n"/>
+      <c r="L27" s="47" t="n"/>
+      <c r="M27" s="47" t="n"/>
+      <c r="N27" s="22" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1" s="74">
+      <c r="A28" s="52" t="n"/>
+      <c r="B28" s="42" t="n"/>
+      <c r="C28" s="43" t="n"/>
+      <c r="D28" s="43" t="n"/>
+      <c r="E28" s="44" t="n"/>
+      <c r="F28" s="44" t="n"/>
+      <c r="G28" s="44" t="n"/>
+      <c r="H28" s="44" t="n"/>
+      <c r="I28" s="44" t="n"/>
+      <c r="J28" s="44" t="n"/>
+      <c r="K28" s="44" t="n"/>
+      <c r="L28" s="44" t="n"/>
+      <c r="M28" s="44" t="n"/>
+      <c r="N28" s="22" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1" s="74">
+      <c r="A29" s="52" t="n"/>
+      <c r="B29" s="45" t="n"/>
+      <c r="C29" s="46" t="n"/>
+      <c r="D29" s="46" t="n"/>
+      <c r="E29" s="47" t="n"/>
+      <c r="F29" s="47" t="n"/>
+      <c r="G29" s="47" t="n"/>
+      <c r="H29" s="47" t="n"/>
+      <c r="I29" s="47" t="n"/>
+      <c r="J29" s="47" t="n"/>
+      <c r="K29" s="47" t="n"/>
+      <c r="L29" s="47" t="n"/>
+      <c r="M29" s="47" t="n"/>
+      <c r="N29" s="22" t="n"/>
+    </row>
+    <row r="30" ht="18" customFormat="1" customHeight="1" s="108">
+      <c r="A30" s="52" t="n"/>
+      <c r="B30" s="42" t="n"/>
+      <c r="C30" s="43" t="n"/>
+      <c r="D30" s="43" t="n"/>
+      <c r="E30" s="44" t="n"/>
+      <c r="F30" s="44" t="n"/>
+      <c r="G30" s="44" t="n"/>
+      <c r="H30" s="44" t="n"/>
+      <c r="I30" s="44" t="n"/>
+      <c r="J30" s="44" t="n"/>
+      <c r="K30" s="44" t="n"/>
+      <c r="L30" s="44" t="n"/>
+      <c r="M30" s="44" t="n"/>
+      <c r="N30" s="22" t="n"/>
+    </row>
+    <row r="31" ht="18" customFormat="1" customHeight="1" s="108">
       <c r="A31" s="52" t="n"/>
-      <c r="B31" s="24" t="n"/>
-      <c r="C31" s="25" t="n"/>
-      <c r="D31" s="25" t="n"/>
-      <c r="E31" s="26" t="n"/>
-      <c r="F31" s="26" t="n"/>
-      <c r="G31" s="26" t="n"/>
-      <c r="H31" s="26" t="n"/>
-      <c r="I31" s="26" t="n"/>
-      <c r="J31" s="26" t="n"/>
-      <c r="K31" s="26" t="n"/>
-      <c r="L31" s="26" t="n"/>
-      <c r="M31" s="40" t="n"/>
-      <c r="N31" s="65" t="n"/>
-      <c r="O31" s="41" t="n"/>
-    </row>
-    <row r="32" ht="33.75" customHeight="1" s="107">
+      <c r="B31" s="45" t="n"/>
+      <c r="C31" s="46" t="n"/>
+      <c r="D31" s="46" t="n"/>
+      <c r="E31" s="47" t="n"/>
+      <c r="F31" s="47" t="n"/>
+      <c r="G31" s="47" t="n"/>
+      <c r="H31" s="47" t="n"/>
+      <c r="I31" s="47" t="n"/>
+      <c r="J31" s="47" t="n"/>
+      <c r="K31" s="47" t="n"/>
+      <c r="L31" s="47" t="n"/>
+      <c r="M31" s="47" t="n"/>
+      <c r="N31" s="22" t="n"/>
+    </row>
+    <row r="32" ht="18" customHeight="1" s="74">
       <c r="A32" s="52" t="n"/>
-      <c r="B32" s="38" t="n"/>
-      <c r="C32" s="27" t="n"/>
-      <c r="D32" s="27" t="n"/>
-      <c r="E32" s="63" t="n"/>
-      <c r="F32" s="63" t="n"/>
-      <c r="G32" s="63" t="n"/>
-      <c r="H32" s="63" t="n"/>
-      <c r="I32" s="63" t="n"/>
-      <c r="J32" s="63" t="n"/>
-      <c r="K32" s="63" t="inlineStr">
+      <c r="B32" s="36" t="n"/>
+      <c r="C32" s="20" t="n"/>
+      <c r="D32" s="20" t="n"/>
+      <c r="E32" s="21" t="n"/>
+      <c r="F32" s="21" t="n"/>
+      <c r="G32" s="21" t="n"/>
+      <c r="H32" s="21" t="n"/>
+      <c r="I32" s="21" t="n"/>
+      <c r="J32" s="21" t="n"/>
+      <c r="K32" s="21" t="n"/>
+      <c r="L32" s="21" t="n"/>
+      <c r="M32" s="21" t="n"/>
+      <c r="N32" s="22" t="n"/>
+    </row>
+    <row r="33" ht="26" customHeight="1" s="74">
+      <c r="A33" s="51" t="n"/>
+      <c r="B33" s="23" t="n"/>
+      <c r="C33" s="24" t="n"/>
+      <c r="D33" s="24" t="n"/>
+      <c r="E33" s="25" t="n"/>
+      <c r="F33" s="25" t="n"/>
+      <c r="G33" s="25" t="n"/>
+      <c r="H33" s="25" t="n"/>
+      <c r="I33" s="25" t="n"/>
+      <c r="J33" s="25" t="n"/>
+      <c r="K33" s="25" t="n"/>
+      <c r="L33" s="25" t="n"/>
+      <c r="M33" s="39" t="n"/>
+      <c r="N33" s="64" t="n"/>
+      <c r="O33" s="85" t="n"/>
+    </row>
+    <row r="34" ht="33.75" customHeight="1" s="74">
+      <c r="A34" s="51" t="n"/>
+      <c r="B34" s="37" t="n"/>
+      <c r="C34" s="26" t="n"/>
+      <c r="D34" s="26" t="n"/>
+      <c r="E34" s="62" t="n"/>
+      <c r="F34" s="62" t="n"/>
+      <c r="G34" s="62" t="n"/>
+      <c r="H34" s="62" t="n"/>
+      <c r="I34" s="62" t="n"/>
+      <c r="J34" s="62" t="n"/>
+      <c r="K34" s="62" t="inlineStr">
         <is>
           <t>Total:</t>
         </is>
       </c>
-      <c r="L32" s="73" t="n"/>
-      <c r="N32" s="64" t="n"/>
-      <c r="O32" s="41" t="n"/>
-    </row>
-    <row r="33" ht="9.75" customHeight="1" s="107">
-      <c r="A33" s="52" t="n"/>
-      <c r="B33" s="28" t="n"/>
-      <c r="C33" s="28" t="n"/>
-      <c r="D33" s="28" t="n"/>
-      <c r="E33" s="28" t="n"/>
-      <c r="F33" s="28" t="n"/>
-      <c r="G33" s="28" t="n"/>
-      <c r="H33" s="28" t="n"/>
-      <c r="I33" s="28" t="n"/>
-      <c r="J33" s="28" t="n"/>
-      <c r="K33" s="28" t="n"/>
-      <c r="L33" s="28" t="n"/>
-      <c r="M33" s="28" t="n"/>
-      <c r="N33" s="28" t="n"/>
-      <c r="O33" s="41" t="n"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1" s="107">
-      <c r="A34" s="52" t="n"/>
-      <c r="B34" s="112" t="n"/>
-      <c r="N34" s="29" t="n"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1" s="107">
-      <c r="A35" s="52" t="n"/>
-      <c r="B35" s="109" t="n"/>
-      <c r="N35" s="30" t="n"/>
-    </row>
-    <row r="36" ht="21" customHeight="1" s="107">
-      <c r="A36" s="54" t="n"/>
-      <c r="B36" s="110" t="n"/>
-      <c r="N36" s="31" t="n"/>
-    </row>
-    <row r="37" ht="8" customHeight="1" s="107">
-      <c r="A37" s="52" t="n"/>
-      <c r="B37" s="9" t="n"/>
-      <c r="C37" s="56" t="n"/>
-      <c r="D37" s="57" t="n"/>
-      <c r="E37" s="57" t="n"/>
-      <c r="F37" s="57" t="n"/>
-      <c r="G37" s="57" t="n"/>
-      <c r="H37" s="57" t="n"/>
-      <c r="I37" s="57" t="n"/>
-      <c r="J37" s="57" t="n"/>
-      <c r="K37" s="57" t="n"/>
-      <c r="L37" s="58" t="n"/>
-      <c r="M37" s="9" t="n"/>
-      <c r="N37" s="49" t="n"/>
-    </row>
-    <row r="38" ht="24" customHeight="1" s="107">
-      <c r="A38" s="41" t="n"/>
-      <c r="C38" s="60" t="n"/>
-      <c r="D38" s="98" t="inlineStr">
+      <c r="L34" s="82" t="n">
+        <v>206.15</v>
+      </c>
+      <c r="N34" s="63" t="n"/>
+      <c r="O34" s="85" t="n"/>
+    </row>
+    <row r="35" ht="9.75" customHeight="1" s="74">
+      <c r="A35" s="51" t="n"/>
+      <c r="B35" s="27" t="n"/>
+      <c r="C35" s="27" t="n"/>
+      <c r="D35" s="27" t="n"/>
+      <c r="E35" s="27" t="n"/>
+      <c r="F35" s="27" t="n"/>
+      <c r="G35" s="27" t="n"/>
+      <c r="H35" s="27" t="n"/>
+      <c r="I35" s="27" t="n"/>
+      <c r="J35" s="27" t="n"/>
+      <c r="K35" s="27" t="n"/>
+      <c r="L35" s="27" t="n"/>
+      <c r="M35" s="27" t="n"/>
+      <c r="N35" s="27" t="n"/>
+      <c r="O35" s="85" t="n"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" s="74">
+      <c r="A36" s="51" t="n"/>
+      <c r="B36" s="91" t="n"/>
+      <c r="N36" s="28" t="n"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" s="74">
+      <c r="A37" s="51" t="n"/>
+      <c r="B37" s="104" t="n"/>
+      <c r="N37" s="29" t="n"/>
+    </row>
+    <row r="38" ht="21" customHeight="1" s="74">
+      <c r="A38" s="53" t="n"/>
+      <c r="B38" s="103" t="n"/>
+      <c r="N38" s="30" t="n"/>
+    </row>
+    <row r="39" ht="8" customHeight="1" s="74">
+      <c r="A39" s="51" t="n"/>
+      <c r="B39" s="9" t="n"/>
+      <c r="C39" s="55" t="n"/>
+      <c r="D39" s="56" t="n"/>
+      <c r="E39" s="56" t="n"/>
+      <c r="F39" s="56" t="n"/>
+      <c r="G39" s="56" t="n"/>
+      <c r="H39" s="56" t="n"/>
+      <c r="I39" s="56" t="n"/>
+      <c r="J39" s="56" t="n"/>
+      <c r="K39" s="56" t="n"/>
+      <c r="L39" s="57" t="n"/>
+      <c r="M39" s="9" t="n"/>
+      <c r="N39" s="48" t="n"/>
+    </row>
+    <row r="40" ht="24" customHeight="1" s="74">
+      <c r="A40" s="85" t="n"/>
+      <c r="C40" s="59" t="n"/>
+      <c r="D40" s="107" t="inlineStr">
         <is>
           <t>Return instructions:</t>
         </is>
       </c>
-      <c r="I38" s="61" t="n"/>
-      <c r="J38" s="61" t="n"/>
-      <c r="K38" s="61" t="n"/>
-      <c r="L38" s="62" t="n"/>
-      <c r="N38" s="50" t="n"/>
-    </row>
-    <row r="39" ht="15" customHeight="1" s="107">
-      <c r="A39" s="41" t="n"/>
-      <c r="C39" s="60" t="n"/>
-      <c r="D39" s="61" t="n"/>
-      <c r="E39" s="61" t="n"/>
-      <c r="F39" s="61" t="n"/>
-      <c r="G39" s="61" t="n"/>
-      <c r="H39" s="61" t="n"/>
-      <c r="I39" s="61" t="n"/>
-      <c r="J39" s="61" t="n"/>
-      <c r="K39" s="61" t="n"/>
-      <c r="L39" s="62" t="n"/>
-      <c r="N39" s="50" t="n"/>
-    </row>
-    <row r="40" ht="17" customHeight="1" s="107">
-      <c r="A40" s="41" t="n"/>
-      <c r="C40" s="124" t="inlineStr">
+      <c r="I40" s="60" t="n"/>
+      <c r="J40" s="60" t="n"/>
+      <c r="K40" s="60" t="n"/>
+      <c r="L40" s="61" t="n"/>
+      <c r="N40" s="84" t="n"/>
+    </row>
+    <row r="41" ht="15" customHeight="1" s="74">
+      <c r="A41" s="85" t="n"/>
+      <c r="C41" s="59" t="n"/>
+      <c r="D41" s="60" t="n"/>
+      <c r="E41" s="60" t="n"/>
+      <c r="F41" s="60" t="n"/>
+      <c r="G41" s="60" t="n"/>
+      <c r="H41" s="60" t="n"/>
+      <c r="I41" s="60" t="n"/>
+      <c r="J41" s="60" t="n"/>
+      <c r="K41" s="60" t="n"/>
+      <c r="L41" s="61" t="n"/>
+      <c r="N41" s="84" t="n"/>
+    </row>
+    <row r="42" ht="17" customHeight="1" s="74">
+      <c r="A42" s="85" t="n"/>
+      <c r="C42" s="83" t="inlineStr">
         <is>
           <t>1. Email the Packing Slip to Customer Service via email to https://returns.healthcare.inmar.com request a Return Authorization (RGA).</t>
         </is>
       </c>
-      <c r="L40" s="50" t="n"/>
-      <c r="N40" s="50" t="n"/>
-    </row>
-    <row r="41" ht="3" customHeight="1" s="107">
-      <c r="A41" s="41" t="n"/>
-      <c r="C41" s="41" t="n"/>
-      <c r="L41" s="50" t="n"/>
-      <c r="N41" s="50" t="n"/>
-    </row>
-    <row r="42" ht="15" customHeight="1" s="107">
-      <c r="A42" s="41" t="n"/>
-      <c r="C42" s="124" t="inlineStr">
+      <c r="L42" s="84" t="n"/>
+      <c r="N42" s="84" t="n"/>
+    </row>
+    <row r="43" ht="3" customHeight="1" s="74">
+      <c r="A43" s="85" t="n"/>
+      <c r="C43" s="85" t="n"/>
+      <c r="L43" s="84" t="n"/>
+      <c r="N43" s="84" t="n"/>
+    </row>
+    <row r="44" ht="15" customHeight="1" s="74">
+      <c r="A44" s="85" t="n"/>
+      <c r="C44" s="83" t="inlineStr">
         <is>
           <t>2. Alternatively, you can create an RGA by logging in to https://clsnetlink.com</t>
         </is>
       </c>
-      <c r="L42" s="50" t="n"/>
-      <c r="N42" s="50" t="n"/>
-    </row>
-    <row r="43" ht="5" customHeight="1" s="107">
-      <c r="A43" s="41" t="n"/>
-      <c r="C43" s="41" t="n"/>
-      <c r="L43" s="50" t="n"/>
-      <c r="N43" s="50" t="n"/>
-    </row>
-    <row r="44" ht="31" customHeight="1" s="107">
-      <c r="A44" s="41" t="n"/>
-      <c r="C44" s="124" t="inlineStr">
+      <c r="L44" s="84" t="n"/>
+      <c r="N44" s="84" t="n"/>
+    </row>
+    <row r="45" ht="5" customHeight="1" s="74">
+      <c r="A45" s="85" t="n"/>
+      <c r="C45" s="85" t="n"/>
+      <c r="L45" s="84" t="n"/>
+      <c r="N45" s="84" t="n"/>
+    </row>
+    <row r="46" ht="31" customHeight="1" s="74">
+      <c r="A46" s="85" t="n"/>
+      <c r="C46" s="83" t="inlineStr">
         <is>
           <t>3. Upon receiving the Returned Goods Authorization Form (RGA), include the RGA along with the Packing Slip and ship the outdated products to the following address:</t>
         </is>
       </c>
-      <c r="L44" s="50" t="n"/>
-      <c r="N44" s="50" t="n"/>
-    </row>
-    <row r="45" ht="4" customHeight="1" s="107">
-      <c r="A45" s="41" t="n"/>
-      <c r="C45" s="41" t="n"/>
-      <c r="L45" s="50" t="n"/>
-      <c r="N45" s="50" t="n"/>
-    </row>
-    <row r="46" ht="18" customHeight="1" s="107">
-      <c r="A46" s="41" t="n"/>
-      <c r="C46" s="91" t="inlineStr">
+      <c r="L46" s="84" t="n"/>
+      <c r="N46" s="84" t="n"/>
+    </row>
+    <row r="47" ht="4" customHeight="1" s="74">
+      <c r="A47" s="85" t="n"/>
+      <c r="C47" s="85" t="n"/>
+      <c r="L47" s="84" t="n"/>
+      <c r="N47" s="84" t="n"/>
+    </row>
+    <row r="48" ht="18" customHeight="1" s="74">
+      <c r="A48" s="85" t="n"/>
+      <c r="C48" s="100" t="inlineStr">
         <is>
           <t>INMAR Pharmaceutical Services</t>
         </is>
       </c>
-      <c r="E46" s="61" t="n"/>
-      <c r="F46" s="61" t="n"/>
-      <c r="G46" s="61" t="n"/>
-      <c r="H46" s="61" t="n"/>
-      <c r="I46" s="61" t="n"/>
-      <c r="J46" s="61" t="n"/>
-      <c r="K46" s="61" t="n"/>
-      <c r="L46" s="62" t="n"/>
-      <c r="N46" s="50" t="n"/>
-    </row>
-    <row r="47" ht="17" customHeight="1" s="107">
-      <c r="A47" s="41" t="n"/>
-      <c r="C47" s="93" t="inlineStr">
+      <c r="E48" s="60" t="n"/>
+      <c r="F48" s="60" t="n"/>
+      <c r="G48" s="60" t="n"/>
+      <c r="H48" s="60" t="n"/>
+      <c r="I48" s="60" t="n"/>
+      <c r="J48" s="60" t="n"/>
+      <c r="K48" s="60" t="n"/>
+      <c r="L48" s="61" t="n"/>
+      <c r="N48" s="84" t="n"/>
+    </row>
+    <row r="49" ht="17" customHeight="1" s="74">
+      <c r="A49" s="85" t="n"/>
+      <c r="C49" s="92" t="inlineStr">
         <is>
           <t>4332 Empire Road</t>
         </is>
       </c>
-      <c r="E47" s="61" t="n"/>
-      <c r="F47" s="61" t="n"/>
-      <c r="G47" s="61" t="n"/>
-      <c r="H47" s="61" t="n"/>
-      <c r="I47" s="61" t="n"/>
-      <c r="J47" s="61" t="n"/>
-      <c r="K47" s="61" t="n"/>
-      <c r="L47" s="62" t="n"/>
-      <c r="N47" s="50" t="n"/>
-    </row>
-    <row r="48" ht="18" customHeight="1" s="107">
-      <c r="A48" s="41" t="n"/>
-      <c r="C48" s="93" t="inlineStr">
+      <c r="E49" s="60" t="n"/>
+      <c r="F49" s="60" t="n"/>
+      <c r="G49" s="60" t="n"/>
+      <c r="H49" s="60" t="n"/>
+      <c r="I49" s="60" t="n"/>
+      <c r="J49" s="60" t="n"/>
+      <c r="K49" s="60" t="n"/>
+      <c r="L49" s="61" t="n"/>
+      <c r="N49" s="84" t="n"/>
+    </row>
+    <row r="50" ht="18" customHeight="1" s="74">
+      <c r="A50" s="85" t="n"/>
+      <c r="C50" s="92" t="inlineStr">
         <is>
           <t>Fort Worth, TX 76155</t>
         </is>
       </c>
-      <c r="E48" s="61" t="n"/>
-      <c r="F48" s="61" t="n"/>
-      <c r="G48" s="61" t="n"/>
-      <c r="H48" s="61" t="n"/>
-      <c r="I48" s="61" t="n"/>
-      <c r="J48" s="61" t="n"/>
-      <c r="K48" s="61" t="n"/>
-      <c r="L48" s="62" t="n"/>
-      <c r="N48" s="50" t="n"/>
-    </row>
-    <row r="49" hidden="1" ht="18" customHeight="1" s="107">
-      <c r="A49" s="41" t="n"/>
-      <c r="C49" s="60" t="n"/>
-      <c r="D49" s="61" t="n"/>
-      <c r="E49" s="61" t="n"/>
-      <c r="F49" s="61" t="n"/>
-      <c r="G49" s="61" t="n"/>
-      <c r="H49" s="61" t="n"/>
-      <c r="I49" s="61" t="n"/>
-      <c r="J49" s="61" t="n"/>
-      <c r="K49" s="61" t="n"/>
-      <c r="L49" s="62" t="n"/>
-      <c r="N49" s="50" t="n"/>
-    </row>
-    <row r="50" ht="15" customHeight="1" s="107">
-      <c r="A50" s="41" t="n"/>
-      <c r="C50" s="125" t="inlineStr">
+      <c r="E50" s="60" t="n"/>
+      <c r="F50" s="60" t="n"/>
+      <c r="G50" s="60" t="n"/>
+      <c r="H50" s="60" t="n"/>
+      <c r="I50" s="60" t="n"/>
+      <c r="J50" s="60" t="n"/>
+      <c r="K50" s="60" t="n"/>
+      <c r="L50" s="61" t="n"/>
+      <c r="N50" s="84" t="n"/>
+    </row>
+    <row r="51" hidden="1" ht="18" customHeight="1" s="74">
+      <c r="A51" s="85" t="n"/>
+      <c r="C51" s="59" t="n"/>
+      <c r="D51" s="60" t="n"/>
+      <c r="E51" s="60" t="n"/>
+      <c r="F51" s="60" t="n"/>
+      <c r="G51" s="60" t="n"/>
+      <c r="H51" s="60" t="n"/>
+      <c r="I51" s="60" t="n"/>
+      <c r="J51" s="60" t="n"/>
+      <c r="K51" s="60" t="n"/>
+      <c r="L51" s="61" t="n"/>
+      <c r="N51" s="84" t="n"/>
+    </row>
+    <row r="52" ht="15" customHeight="1" s="74">
+      <c r="A52" s="85" t="n"/>
+      <c r="C52" s="89" t="inlineStr">
         <is>
           <t>Please DO NOT mix products from multiple debit memos/packing slips in one shipment. In case of any questions, please contact INMAR customer service at 1-800-967-5952</t>
         </is>
       </c>
-      <c r="L50" s="50" t="n"/>
-      <c r="N50" s="50" t="n"/>
-    </row>
-    <row r="51" ht="15" customHeight="1" s="107">
-      <c r="A51" s="41" t="n"/>
-      <c r="C51" s="41" t="n"/>
-      <c r="L51" s="50" t="n"/>
-      <c r="N51" s="50" t="n"/>
-    </row>
-    <row r="52" ht="15" customHeight="1" s="107">
-      <c r="A52" s="41" t="n"/>
-      <c r="C52" s="67" t="n"/>
-      <c r="D52" s="68" t="n"/>
-      <c r="E52" s="68" t="n"/>
-      <c r="F52" s="68" t="n"/>
-      <c r="G52" s="68" t="n"/>
-      <c r="H52" s="68" t="n"/>
-      <c r="I52" s="68" t="n"/>
-      <c r="J52" s="68" t="n"/>
-      <c r="K52" s="68" t="n"/>
-      <c r="L52" s="69" t="n"/>
-      <c r="N52" s="50" t="n"/>
-    </row>
-    <row r="53" ht="15" customHeight="1" s="107">
-      <c r="A53" s="41" t="n"/>
-      <c r="N53" s="50" t="n"/>
-    </row>
-    <row r="54" ht="15" customHeight="1" s="107">
-      <c r="A54" s="41" t="n"/>
-      <c r="N54" s="50" t="n"/>
-    </row>
-    <row r="55" ht="15.75" customHeight="1" s="107">
-      <c r="A55" s="55" t="n"/>
-      <c r="B55" s="32" t="n"/>
-      <c r="C55" s="32" t="n"/>
-      <c r="D55" s="32" t="n"/>
-      <c r="E55" s="32" t="n"/>
-      <c r="F55" s="32" t="n"/>
-      <c r="G55" s="32" t="n"/>
-      <c r="H55" s="32" t="n"/>
-      <c r="I55" s="32" t="n"/>
-      <c r="J55" s="32" t="n"/>
-      <c r="K55" s="32" t="n"/>
-      <c r="L55" s="32" t="n"/>
-      <c r="M55" s="32" t="n"/>
-      <c r="N55" s="51" t="n"/>
+      <c r="L52" s="84" t="n"/>
+      <c r="N52" s="84" t="n"/>
+    </row>
+    <row r="53" ht="15" customHeight="1" s="74">
+      <c r="A53" s="85" t="n"/>
+      <c r="C53" s="85" t="n"/>
+      <c r="L53" s="84" t="n"/>
+      <c r="N53" s="84" t="n"/>
+    </row>
+    <row r="54" ht="15" customHeight="1" s="74">
+      <c r="A54" s="85" t="n"/>
+      <c r="C54" s="66" t="n"/>
+      <c r="D54" s="67" t="n"/>
+      <c r="E54" s="67" t="n"/>
+      <c r="F54" s="67" t="n"/>
+      <c r="G54" s="67" t="n"/>
+      <c r="H54" s="67" t="n"/>
+      <c r="I54" s="67" t="n"/>
+      <c r="J54" s="67" t="n"/>
+      <c r="K54" s="67" t="n"/>
+      <c r="L54" s="68" t="n"/>
+      <c r="N54" s="84" t="n"/>
+    </row>
+    <row r="55" ht="15" customHeight="1" s="74">
+      <c r="A55" s="85" t="n"/>
+      <c r="N55" s="84" t="n"/>
+    </row>
+    <row r="56" ht="15" customHeight="1" s="74">
+      <c r="A56" s="85" t="n"/>
+      <c r="N56" s="84" t="n"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1" s="74">
+      <c r="A57" s="54" t="n"/>
+      <c r="B57" s="31" t="n"/>
+      <c r="C57" s="31" t="n"/>
+      <c r="D57" s="31" t="n"/>
+      <c r="E57" s="31" t="n"/>
+      <c r="F57" s="31" t="n"/>
+      <c r="G57" s="31" t="n"/>
+      <c r="H57" s="31" t="n"/>
+      <c r="I57" s="31" t="n"/>
+      <c r="J57" s="31" t="n"/>
+      <c r="K57" s="31" t="n"/>
+      <c r="L57" s="31" t="n"/>
+      <c r="M57" s="31" t="n"/>
+      <c r="N57" s="50" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="45">
     <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="D4:H5"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="C15:M15"/>
     <mergeCell ref="C42:L43"/>
     <mergeCell ref="H12:K12"/>
     <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="D40:H40"/>
     <mergeCell ref="E6:M6"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="C50:L51"/>
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="H14:K14"/>
-    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B38:M38"/>
     <mergeCell ref="C44:L45"/>
-    <mergeCell ref="C47:D47"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="C50:D50"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="C46:L47"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="C40:L41"/>
     <mergeCell ref="H10:K10"/>
+    <mergeCell ref="E16:G16"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E7:M7"/>
-    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C52:L53"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B36:M36"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B35:M35"/>
     <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C17:M17"/>
     <mergeCell ref="B3:J3"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="H11:K11"/>
     <mergeCell ref="E8:G8"/>
-    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="C49:D49"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" scale="51"/>

</xml_diff>

<commit_message>
added some api to support boxes and stored all the values in box when closing
</commit_message>
<xml_diff>
--- a/docs/invoice.xlsx
+++ b/docs/invoice.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -654,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -684,9 +684,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -828,12 +825,90 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="32"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -846,80 +921,28 @@
     <xf numFmtId="49" fontId="27" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="29" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="32"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2049,44 +2072,44 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="H10" sqref="H10:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="4.33203125" customWidth="1" style="74" min="1" max="1"/>
-    <col width="11.6640625" customWidth="1" style="74" min="2" max="2"/>
-    <col width="28.6640625" customWidth="1" style="74" min="3" max="3"/>
-    <col width="34" customWidth="1" style="74" min="4" max="4"/>
-    <col width="14.83203125" customWidth="1" style="74" min="5" max="5"/>
-    <col width="9" customWidth="1" style="74" min="6" max="6"/>
-    <col width="10.1640625" customWidth="1" style="74" min="7" max="7"/>
-    <col width="9.1640625" customWidth="1" style="74" min="8" max="8"/>
-    <col width="8.83203125" customWidth="1" style="74" min="9" max="9"/>
-    <col width="6.6640625" customWidth="1" style="74" min="10" max="10"/>
-    <col width="7.6640625" customWidth="1" style="74" min="11" max="11"/>
-    <col width="8.83203125" customWidth="1" style="74" min="12" max="12"/>
-    <col width="13.5" customWidth="1" style="74" min="13" max="13"/>
-    <col width="3.5" customWidth="1" style="74" min="14" max="14"/>
+    <col width="4.33203125" customWidth="1" style="78" min="1" max="1"/>
+    <col width="11.6640625" customWidth="1" style="78" min="2" max="2"/>
+    <col width="28.6640625" customWidth="1" style="78" min="3" max="3"/>
+    <col width="34" customWidth="1" style="78" min="4" max="4"/>
+    <col width="14.83203125" customWidth="1" style="78" min="5" max="5"/>
+    <col width="9" customWidth="1" style="78" min="6" max="6"/>
+    <col width="10.1640625" customWidth="1" style="78" min="7" max="7"/>
+    <col width="9.1640625" customWidth="1" style="78" min="8" max="8"/>
+    <col width="8.83203125" customWidth="1" style="78" min="9" max="9"/>
+    <col width="6.6640625" customWidth="1" style="78" min="10" max="10"/>
+    <col width="7.6640625" customWidth="1" style="78" min="11" max="11"/>
+    <col width="8.83203125" customWidth="1" style="78" min="12" max="12"/>
+    <col width="13.5" customWidth="1" style="78" min="13" max="13"/>
+    <col width="3.5" customWidth="1" style="78" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="74">
+    <row r="1" ht="14.25" customHeight="1" s="78">
       <c r="A1" s="1" t="n"/>
-      <c r="B1" s="32" t="n"/>
-      <c r="C1" s="33" t="n"/>
-      <c r="D1" s="33" t="n"/>
-      <c r="E1" s="33" t="n"/>
-      <c r="F1" s="33" t="n"/>
-      <c r="G1" s="33" t="n"/>
-      <c r="H1" s="33" t="n"/>
-      <c r="I1" s="33" t="n"/>
-      <c r="J1" s="33" t="n"/>
-      <c r="K1" s="33" t="n"/>
-      <c r="L1" s="33" t="n"/>
-      <c r="M1" s="34" t="n"/>
-      <c r="N1" s="35" t="n"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1" s="74">
+      <c r="B1" s="31" t="n"/>
+      <c r="C1" s="32" t="n"/>
+      <c r="D1" s="32" t="n"/>
+      <c r="E1" s="32" t="n"/>
+      <c r="F1" s="32" t="n"/>
+      <c r="G1" s="32" t="n"/>
+      <c r="H1" s="32" t="n"/>
+      <c r="I1" s="32" t="n"/>
+      <c r="J1" s="32" t="n"/>
+      <c r="K1" s="32" t="n"/>
+      <c r="L1" s="32" t="n"/>
+      <c r="M1" s="33" t="n"/>
+      <c r="N1" s="34" t="n"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1" s="78">
       <c r="A2" s="2" t="n"/>
       <c r="B2" s="3" t="n"/>
       <c r="C2" s="4" t="n"/>
@@ -2102,919 +2125,919 @@
       <c r="M2" s="5" t="n"/>
       <c r="N2" s="6" t="n"/>
     </row>
-    <row r="3" ht="73" customHeight="1" s="74" thickBot="1">
+    <row r="3" ht="73" customHeight="1" s="78" thickBot="1">
       <c r="A3" s="7" t="n"/>
-      <c r="B3" s="105" t="inlineStr">
+      <c r="B3" s="77" t="inlineStr">
         <is>
           <t>Manufacturer Packaging Slip</t>
         </is>
       </c>
       <c r="K3" s="9" t="n"/>
-      <c r="L3" s="111" t="inlineStr">
+      <c r="L3" s="75" t="inlineStr">
         <is>
           <t>Quick Returns</t>
         </is>
       </c>
-      <c r="M3" s="97" t="n"/>
+      <c r="M3" s="81" t="n"/>
       <c r="N3" s="10" t="n"/>
     </row>
-    <row r="4" ht="18" customHeight="1" s="74" thickBot="1">
+    <row r="4" ht="18" customHeight="1" s="78" thickBot="1">
       <c r="A4" s="7" t="n"/>
-      <c r="B4" s="69" t="inlineStr">
+      <c r="B4" s="68" t="inlineStr">
         <is>
           <t>DATE</t>
         </is>
       </c>
-      <c r="D4" s="76" t="n"/>
-      <c r="E4" s="77" t="n"/>
-      <c r="F4" s="77" t="n"/>
-      <c r="G4" s="77" t="n"/>
-      <c r="H4" s="78" t="n"/>
-      <c r="I4" s="87" t="n"/>
-      <c r="J4" s="87" t="n"/>
-      <c r="K4" s="87" t="n"/>
-      <c r="L4" s="101" t="inlineStr">
+      <c r="D4" s="103" t="n"/>
+      <c r="E4" s="104" t="n"/>
+      <c r="F4" s="104" t="n"/>
+      <c r="G4" s="104" t="n"/>
+      <c r="H4" s="105" t="n"/>
+      <c r="I4" s="97" t="n"/>
+      <c r="J4" s="97" t="n"/>
+      <c r="K4" s="97" t="n"/>
+      <c r="L4" s="112" t="inlineStr">
         <is>
           <t>INVOICE NO:</t>
         </is>
       </c>
-      <c r="M4" s="102" t="n"/>
+      <c r="M4" s="113" t="n"/>
       <c r="N4" s="11" t="n"/>
     </row>
-    <row r="5" ht="18" customHeight="1" s="74" thickBot="1">
+    <row r="5" ht="18" customHeight="1" s="78" thickBot="1">
       <c r="A5" s="7" t="n"/>
-      <c r="B5" s="70" t="inlineStr">
-        <is>
-          <t>01/15/2024</t>
-        </is>
-      </c>
-      <c r="D5" s="79" t="n"/>
-      <c r="E5" s="80" t="n"/>
-      <c r="F5" s="80" t="n"/>
-      <c r="G5" s="80" t="n"/>
-      <c r="H5" s="81" t="n"/>
-      <c r="I5" s="87" t="n"/>
-      <c r="J5" s="87" t="n"/>
-      <c r="K5" s="87" t="n"/>
-      <c r="L5" s="94" t="inlineStr">
-        <is>
-          <t>QR01152024AP201</t>
-        </is>
-      </c>
-      <c r="M5" s="95" t="n"/>
-      <c r="N5" s="14" t="n"/>
-    </row>
-    <row r="6" ht="18" customHeight="1" s="74">
+      <c r="B5" s="69" t="inlineStr">
+        <is>
+          <t>01/25/2024</t>
+        </is>
+      </c>
+      <c r="D5" s="106" t="n"/>
+      <c r="E5" s="107" t="n"/>
+      <c r="F5" s="107" t="n"/>
+      <c r="G5" s="107" t="n"/>
+      <c r="H5" s="108" t="n"/>
+      <c r="I5" s="97" t="n"/>
+      <c r="J5" s="97" t="n"/>
+      <c r="K5" s="97" t="n"/>
+      <c r="L5" s="110" t="inlineStr">
+        <is>
+          <t>QR01252024AP401</t>
+        </is>
+      </c>
+      <c r="M5" s="111" t="n"/>
+      <c r="N5" s="13" t="n"/>
+    </row>
+    <row r="6" ht="18" customHeight="1" s="78">
       <c r="A6" s="7" t="n"/>
-      <c r="D6" s="73" t="n"/>
-      <c r="E6" s="88" t="n"/>
-      <c r="N6" s="15" t="n"/>
-    </row>
-    <row r="7" ht="22.5" customHeight="1" s="74">
+      <c r="D6" s="12" t="n"/>
+      <c r="E6" s="98" t="n"/>
+      <c r="N6" s="14" t="n"/>
+    </row>
+    <row r="7" ht="22.5" customHeight="1" s="78">
       <c r="A7" s="7" t="n"/>
-      <c r="D7" s="73" t="n"/>
-      <c r="E7" s="99" t="n"/>
-      <c r="N7" s="16" t="n"/>
-    </row>
-    <row r="8" ht="26.25" customHeight="1" s="74">
+      <c r="D7" s="12" t="n"/>
+      <c r="E7" s="102" t="n"/>
+      <c r="N7" s="15" t="n"/>
+    </row>
+    <row r="8" ht="26.25" customHeight="1" s="78">
       <c r="A8" s="7" t="n"/>
-      <c r="B8" s="96" t="inlineStr">
+      <c r="B8" s="100" t="inlineStr">
         <is>
           <t>Account:</t>
         </is>
       </c>
-      <c r="C8" s="97" t="n"/>
-      <c r="D8" s="96" t="inlineStr">
+      <c r="C8" s="81" t="n"/>
+      <c r="D8" s="100" t="inlineStr">
         <is>
           <t>Wholesaler:</t>
         </is>
       </c>
-      <c r="E8" s="106" t="inlineStr">
+      <c r="E8" s="80" t="inlineStr">
         <is>
           <t>Issue Credit to:</t>
         </is>
       </c>
-      <c r="F8" s="97" t="n"/>
-      <c r="G8" s="97" t="n"/>
-      <c r="H8" s="93" t="n"/>
-      <c r="L8" s="65" t="n"/>
-      <c r="M8" s="65" t="n"/>
-      <c r="N8" s="17" t="n"/>
-    </row>
-    <row r="9" ht="8" customHeight="1" s="74">
+      <c r="F8" s="81" t="n"/>
+      <c r="G8" s="81" t="n"/>
+      <c r="H8" s="99" t="n"/>
+      <c r="L8" s="64" t="n"/>
+      <c r="M8" s="64" t="n"/>
+      <c r="N8" s="16" t="n"/>
+    </row>
+    <row r="9" ht="8" customHeight="1" s="78">
       <c r="A9" s="7" t="n"/>
-      <c r="B9" s="87" t="n"/>
-      <c r="D9" s="108" t="n"/>
-      <c r="E9" s="87" t="n"/>
-      <c r="H9" s="108" t="n"/>
-      <c r="I9" s="108" t="n"/>
-      <c r="J9" s="108" t="n"/>
-      <c r="K9" s="108" t="n"/>
-      <c r="L9" s="87" t="n"/>
-      <c r="M9" s="87" t="n"/>
-      <c r="N9" s="18" t="n"/>
-    </row>
-    <row r="10" ht="18" customHeight="1" s="74">
-      <c r="A10" s="51" t="n"/>
-      <c r="B10" s="109" t="inlineStr">
-        <is>
-          <t>AUTREY PHARMACY 2</t>
-        </is>
-      </c>
-      <c r="D10" s="12" t="inlineStr">
+      <c r="B9" s="97" t="n"/>
+      <c r="D9" s="37" t="n"/>
+      <c r="E9" s="97" t="n"/>
+      <c r="H9" s="37" t="n"/>
+      <c r="I9" s="37" t="n"/>
+      <c r="J9" s="37" t="n"/>
+      <c r="K9" s="37" t="n"/>
+      <c r="L9" s="97" t="n"/>
+      <c r="M9" s="97" t="n"/>
+      <c r="N9" s="17" t="n"/>
+    </row>
+    <row r="10" ht="35" customHeight="1" s="78">
+      <c r="A10" s="50" t="n"/>
+      <c r="B10" s="114" t="inlineStr">
+        <is>
+          <t>AUTREY PHARMACY 4</t>
+        </is>
+      </c>
+      <c r="D10" s="115" t="inlineStr">
         <is>
           <t>AMERISOURCEBERGEN DRUG CORPORATION</t>
         </is>
       </c>
-      <c r="E10" s="73" t="inlineStr">
-        <is>
-          <t>AUTREY PHARMACY 2</t>
-        </is>
-      </c>
-      <c r="H10" s="98" t="n"/>
-      <c r="L10" s="73" t="n"/>
-      <c r="M10" s="73" t="n"/>
-      <c r="N10" s="19" t="n"/>
-    </row>
-    <row r="11" ht="18" customHeight="1" s="74">
-      <c r="A11" s="51" t="n"/>
-      <c r="B11" s="109" t="inlineStr">
-        <is>
-          <t>1365 E RUBEN TORRES BLVD</t>
-        </is>
-      </c>
-      <c r="D11" s="12" t="inlineStr">
+      <c r="E10" s="118" t="inlineStr">
+        <is>
+          <t>AUTREY PHARMACY 4</t>
+        </is>
+      </c>
+      <c r="H10" s="101" t="n"/>
+      <c r="L10" s="12" t="n"/>
+      <c r="M10" s="12" t="n"/>
+      <c r="N10" s="18" t="n"/>
+    </row>
+    <row r="11" ht="18" customHeight="1" s="78">
+      <c r="A11" s="50" t="n"/>
+      <c r="B11" s="114" t="inlineStr">
+        <is>
+          <t>3503 BOCA CHICA BLVD, SUITE 1</t>
+        </is>
+      </c>
+      <c r="D11" s="115" t="inlineStr">
         <is>
           <t>108 ROUTE 17K SUITE 1</t>
         </is>
       </c>
-      <c r="E11" s="73" t="inlineStr">
-        <is>
-          <t>1365 E RUBEN TORRES BLVD</t>
-        </is>
-      </c>
-      <c r="H11" s="75" t="n"/>
-      <c r="L11" s="73" t="n"/>
-      <c r="M11" s="73" t="n"/>
-      <c r="N11" s="19" t="n"/>
-    </row>
-    <row r="12" ht="18" customHeight="1" s="74">
-      <c r="A12" s="51" t="n"/>
-      <c r="B12" s="109" t="inlineStr">
-        <is>
-          <t>BROWNSVILLE, TX 78521</t>
-        </is>
-      </c>
-      <c r="D12" s="12" t="inlineStr">
+      <c r="E11" s="118" t="inlineStr">
+        <is>
+          <t>3503 BOCA CHICA BLVD, SUITE 1</t>
+        </is>
+      </c>
+      <c r="H11" s="79" t="n"/>
+      <c r="L11" s="12" t="n"/>
+      <c r="M11" s="12" t="n"/>
+      <c r="N11" s="18" t="n"/>
+    </row>
+    <row r="12" ht="18" customHeight="1" s="78">
+      <c r="A12" s="50" t="n"/>
+      <c r="B12" s="114" t="inlineStr">
+        <is>
+          <t>BROWNSVILLE, TX, 78521</t>
+        </is>
+      </c>
+      <c r="D12" s="115" t="inlineStr">
         <is>
           <t>NEWBURGH. NY, 12550-5008</t>
         </is>
       </c>
-      <c r="E12" s="73" t="inlineStr">
-        <is>
-          <t>BROWNSVILLE, TX 78521</t>
-        </is>
-      </c>
-      <c r="H12" s="75" t="n"/>
-      <c r="L12" s="73" t="n"/>
-      <c r="M12" s="73" t="n"/>
-      <c r="N12" s="19" t="n"/>
-    </row>
-    <row r="13" ht="18" customHeight="1" s="74">
-      <c r="A13" s="51" t="n"/>
-      <c r="B13" s="109" t="inlineStr">
-        <is>
-          <t>EC</t>
-        </is>
-      </c>
-      <c r="D13" s="12" t="inlineStr">
+      <c r="E12" s="118" t="inlineStr">
+        <is>
+          <t>BROWNSVILLE, TX, 78521</t>
+        </is>
+      </c>
+      <c r="H12" s="79" t="n"/>
+      <c r="L12" s="12" t="n"/>
+      <c r="M12" s="12" t="n"/>
+      <c r="N12" s="18" t="n"/>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="78">
+      <c r="A13" s="50" t="n"/>
+      <c r="B13" s="114" t="inlineStr">
+        <is>
+          <t>contact name</t>
+        </is>
+      </c>
+      <c r="D13" s="115" t="inlineStr">
         <is>
           <t>Account#: 100199545</t>
         </is>
       </c>
-      <c r="E13" s="73" t="inlineStr">
-        <is>
-          <t>EC</t>
-        </is>
-      </c>
-      <c r="H13" s="75" t="n"/>
-      <c r="L13" s="73" t="n"/>
-      <c r="M13" s="73" t="n"/>
-      <c r="N13" s="19" t="n"/>
-    </row>
-    <row r="14" ht="18" customHeight="1" s="74">
-      <c r="A14" s="51" t="n"/>
-      <c r="B14" s="109" t="inlineStr">
-        <is>
-          <t>Phone: 956-542-5100, fax: 956-542-5103</t>
-        </is>
-      </c>
-      <c r="D14" s="73" t="inlineStr">
+      <c r="E13" s="118" t="inlineStr">
+        <is>
+          <t>contact name</t>
+        </is>
+      </c>
+      <c r="H13" s="79" t="n"/>
+      <c r="L13" s="12" t="n"/>
+      <c r="M13" s="12" t="n"/>
+      <c r="N13" s="18" t="n"/>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="78">
+      <c r="A14" s="50" t="n"/>
+      <c r="B14" s="114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phone: 956-621-1000, fax: </t>
+        </is>
+      </c>
+      <c r="D14" s="118" t="inlineStr">
         <is>
           <t>Phone: 844-222-2273</t>
         </is>
       </c>
-      <c r="E14" s="73" t="inlineStr">
-        <is>
-          <t>Phone: 956-542-5100, fax: 956-542-5103</t>
-        </is>
-      </c>
-      <c r="H14" s="90" t="n"/>
-      <c r="L14" s="73" t="n"/>
-      <c r="M14" s="73" t="n"/>
-      <c r="N14" s="19" t="n"/>
-    </row>
-    <row r="15" ht="18" customHeight="1" s="74">
-      <c r="A15" s="51" t="n"/>
-      <c r="B15" s="109" t="inlineStr">
-        <is>
-          <t>DEA: FA3706895, Exp: 06/30/2023</t>
-        </is>
-      </c>
-      <c r="D15" s="73" t="inlineStr">
+      <c r="E14" s="118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phone: 956-621-1000, fax: </t>
+        </is>
+      </c>
+      <c r="H14" s="83" t="n"/>
+      <c r="L14" s="12" t="n"/>
+      <c r="M14" s="12" t="n"/>
+      <c r="N14" s="18" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="78">
+      <c r="A15" s="50" t="n"/>
+      <c r="B15" s="114" t="inlineStr">
+        <is>
+          <t>DEA: FA6707511, Exp: 06/30/2023</t>
+        </is>
+      </c>
+      <c r="D15" s="118" t="inlineStr">
         <is>
           <t>DEA: RA0522056</t>
         </is>
       </c>
-      <c r="E15" s="73" t="inlineStr">
-        <is>
-          <t>DEA: FA3706895, Exp: 06/30/2023</t>
-        </is>
-      </c>
-      <c r="H15" s="90" t="n"/>
-      <c r="L15" s="73" t="n"/>
-      <c r="M15" s="73" t="n"/>
-      <c r="N15" s="19" t="n"/>
-    </row>
-    <row r="16" ht="18" customFormat="1" customHeight="1" s="108">
-      <c r="A16" s="51" t="n"/>
-      <c r="B16" s="109" t="inlineStr">
+      <c r="E15" s="118" t="inlineStr">
+        <is>
+          <t>DEA: FA6707511, Exp: 06/30/2023</t>
+        </is>
+      </c>
+      <c r="H15" s="83" t="n"/>
+      <c r="L15" s="12" t="n"/>
+      <c r="M15" s="12" t="n"/>
+      <c r="N15" s="18" t="n"/>
+    </row>
+    <row r="16" ht="18" customFormat="1" customHeight="1" s="37">
+      <c r="A16" s="50" t="n"/>
+      <c r="B16" s="114" t="inlineStr">
         <is>
           <t>Authorized Classes: 2, 2N, 3, 3N, 4. 5</t>
         </is>
       </c>
-      <c r="D16" s="73" t="n"/>
-      <c r="E16" s="73" t="inlineStr">
+      <c r="D16" s="118" t="n"/>
+      <c r="E16" s="118" t="inlineStr">
         <is>
           <t>Authorized Classes: 2, 2N, 3, 3N, 4. 5</t>
         </is>
       </c>
-      <c r="H16" s="90" t="n"/>
-      <c r="L16" s="73" t="n"/>
-      <c r="M16" s="73" t="n"/>
-      <c r="N16" s="19" t="n"/>
-    </row>
-    <row r="17" ht="18" customHeight="1" s="74">
-      <c r="A17" s="51" t="n"/>
-      <c r="B17" s="73" t="n"/>
-      <c r="C17" s="86" t="n"/>
-      <c r="N17" s="14" t="n"/>
-    </row>
-    <row r="18" ht="8" customHeight="1" s="74">
-      <c r="A18" s="51" t="n"/>
-      <c r="B18" s="87" t="n"/>
-      <c r="C18" s="87" t="n"/>
-      <c r="D18" s="87" t="n"/>
-      <c r="E18" s="87" t="n"/>
-      <c r="F18" s="87" t="n"/>
-      <c r="G18" s="87" t="n"/>
-      <c r="H18" s="87" t="n"/>
-      <c r="I18" s="87" t="n"/>
-      <c r="J18" s="87" t="n"/>
-      <c r="K18" s="87" t="n"/>
-      <c r="L18" s="87" t="n"/>
-      <c r="M18" s="87" t="n"/>
-      <c r="N18" s="18" t="n"/>
-    </row>
-    <row r="19" ht="25" customHeight="1" s="74">
-      <c r="A19" s="51" t="n"/>
-      <c r="B19" s="41" t="inlineStr">
+      <c r="H16" s="83" t="n"/>
+      <c r="L16" s="12" t="n"/>
+      <c r="M16" s="12" t="n"/>
+      <c r="N16" s="18" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="78">
+      <c r="A17" s="50" t="n"/>
+      <c r="B17" s="12" t="n"/>
+      <c r="C17" s="96" t="n"/>
+      <c r="N17" s="13" t="n"/>
+    </row>
+    <row r="18" ht="8" customHeight="1" s="78">
+      <c r="A18" s="50" t="n"/>
+      <c r="B18" s="97" t="n"/>
+      <c r="C18" s="97" t="n"/>
+      <c r="D18" s="97" t="n"/>
+      <c r="E18" s="97" t="n"/>
+      <c r="F18" s="97" t="n"/>
+      <c r="G18" s="97" t="n"/>
+      <c r="H18" s="97" t="n"/>
+      <c r="I18" s="97" t="n"/>
+      <c r="J18" s="97" t="n"/>
+      <c r="K18" s="97" t="n"/>
+      <c r="L18" s="97" t="n"/>
+      <c r="M18" s="97" t="n"/>
+      <c r="N18" s="17" t="n"/>
+    </row>
+    <row r="19" ht="25" customHeight="1" s="78">
+      <c r="A19" s="50" t="n"/>
+      <c r="B19" s="40" t="inlineStr">
         <is>
           <t>NDC/UPC</t>
         </is>
       </c>
-      <c r="C19" s="41" t="inlineStr">
+      <c r="C19" s="40" t="inlineStr">
         <is>
           <t>Manufacturer</t>
         </is>
       </c>
-      <c r="D19" s="41" t="inlineStr">
+      <c r="D19" s="40" t="inlineStr">
         <is>
           <t>Product name</t>
         </is>
       </c>
-      <c r="E19" s="41" t="inlineStr">
+      <c r="E19" s="40" t="inlineStr">
         <is>
           <t>Strength</t>
         </is>
       </c>
-      <c r="F19" s="41" t="inlineStr">
+      <c r="F19" s="40" t="inlineStr">
         <is>
           <t>DSG</t>
         </is>
       </c>
-      <c r="G19" s="41" t="inlineStr">
+      <c r="G19" s="40" t="inlineStr">
         <is>
           <t>Lot</t>
         </is>
       </c>
-      <c r="H19" s="41" t="inlineStr">
+      <c r="H19" s="40" t="inlineStr">
         <is>
           <t>Exp</t>
         </is>
       </c>
-      <c r="I19" s="41" t="inlineStr">
+      <c r="I19" s="40" t="inlineStr">
         <is>
           <t>Pkg Size</t>
         </is>
       </c>
-      <c r="J19" s="41" t="inlineStr">
+      <c r="J19" s="40" t="inlineStr">
         <is>
           <t>Full Qty</t>
         </is>
       </c>
-      <c r="K19" s="58" t="inlineStr">
+      <c r="K19" s="57" t="inlineStr">
         <is>
           <t>Partial Qty</t>
         </is>
       </c>
-      <c r="L19" s="41" t="inlineStr">
+      <c r="L19" s="40" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="M19" s="41" t="inlineStr">
+      <c r="M19" s="40" t="inlineStr">
         <is>
           <t>Est Value</t>
         </is>
       </c>
       <c r="N19" s="11" t="n"/>
     </row>
-    <row r="20" ht="18" customHeight="1" s="74">
-      <c r="A20" s="52" t="n"/>
-      <c r="B20" s="42" t="inlineStr">
-        <is>
-          <t>6818024906</t>
-        </is>
-      </c>
-      <c r="C20" s="43" t="inlineStr">
-        <is>
-          <t>Lupin Pharmaceuticals, Inc.</t>
-        </is>
-      </c>
-      <c r="D20" s="43" t="inlineStr">
-        <is>
-          <t>memantine hydrochloride</t>
-        </is>
-      </c>
-      <c r="E20" s="44" t="inlineStr">
-        <is>
-          <t>28 mg/1</t>
-        </is>
-      </c>
-      <c r="F20" s="44" t="inlineStr">
-        <is>
-          <t>CAPSULE, EXTENDED RELEASE</t>
-        </is>
-      </c>
-      <c r="G20" s="44" t="inlineStr">
-        <is>
-          <t>H102306</t>
-        </is>
-      </c>
-      <c r="H20" s="44" t="inlineStr">
-        <is>
-          <t>09/23/30</t>
-        </is>
-      </c>
-      <c r="I20" s="44" t="inlineStr">
-        <is>
-          <t>30 CT</t>
-        </is>
-      </c>
-      <c r="J20" s="44" t="n">
-        <v>4</v>
-      </c>
-      <c r="K20" s="44" t="n"/>
-      <c r="L20" s="44" t="n">
-        <v>35</v>
-      </c>
-      <c r="M20" s="44" t="n">
-        <v>140</v>
-      </c>
-      <c r="N20" s="22" t="n"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" s="74">
-      <c r="A21" s="52" t="n"/>
-      <c r="B21" s="45" t="inlineStr">
+    <row r="20" ht="18" customHeight="1" s="78">
+      <c r="A20" s="51" t="n"/>
+      <c r="B20" s="41" t="inlineStr">
         <is>
           <t>6787743305</t>
         </is>
       </c>
-      <c r="C21" s="46" t="inlineStr">
+      <c r="C20" s="42" t="inlineStr">
         <is>
           <t>Ascend Laboratories, LLC</t>
         </is>
       </c>
-      <c r="D21" s="46" t="inlineStr">
+      <c r="D20" s="42" t="inlineStr">
         <is>
           <t>Aripiprazole</t>
         </is>
       </c>
-      <c r="E21" s="47" t="inlineStr">
+      <c r="E20" s="43" t="inlineStr">
         <is>
           <t>15 mg/1</t>
         </is>
       </c>
-      <c r="F21" s="47" t="inlineStr">
+      <c r="F20" s="43" t="inlineStr">
         <is>
           <t>TABLET</t>
         </is>
       </c>
-      <c r="G21" s="47" t="inlineStr">
+      <c r="G20" s="43" t="inlineStr">
         <is>
           <t>22140477</t>
         </is>
       </c>
-      <c r="H21" s="47" t="inlineStr">
+      <c r="H20" s="43" t="inlineStr">
         <is>
           <t>01/24/31</t>
         </is>
       </c>
-      <c r="I21" s="47" t="inlineStr">
+      <c r="I20" s="43" t="inlineStr">
         <is>
           <t>500 CT</t>
         </is>
       </c>
-      <c r="J21" s="47" t="n">
-        <v>35</v>
-      </c>
-      <c r="K21" s="47" t="n"/>
+      <c r="J20" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="43" t="n"/>
+      <c r="L20" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" s="21" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="78">
+      <c r="A21" s="51" t="n"/>
+      <c r="B21" s="44" t="inlineStr">
+        <is>
+          <t>6787743305</t>
+        </is>
+      </c>
+      <c r="C21" s="45" t="inlineStr">
+        <is>
+          <t>Ascend Laboratories, LLC</t>
+        </is>
+      </c>
+      <c r="D21" s="45" t="inlineStr">
+        <is>
+          <t>Aripiprazole</t>
+        </is>
+      </c>
+      <c r="E21" s="46" t="inlineStr">
+        <is>
+          <t>15 mg/1</t>
+        </is>
+      </c>
+      <c r="F21" s="46" t="inlineStr">
+        <is>
+          <t>TABLET</t>
+        </is>
+      </c>
+      <c r="G21" s="46" t="inlineStr">
+        <is>
+          <t>22140477</t>
+        </is>
+      </c>
+      <c r="H21" s="46" t="inlineStr">
+        <is>
+          <t>01/24/31</t>
+        </is>
+      </c>
+      <c r="I21" s="46" t="inlineStr">
+        <is>
+          <t>500 CT</t>
+        </is>
+      </c>
+      <c r="J21" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="46" t="n"/>
       <c r="L21" t="n">
-        <v>1.89</v>
-      </c>
-      <c r="M21" s="47" t="n">
-        <v>66.15000000000001</v>
-      </c>
-      <c r="N21" s="22" t="n"/>
-    </row>
-    <row r="22" ht="18" customHeight="1" s="74">
-      <c r="A22" s="52" t="n"/>
-      <c r="B22" s="42" t="n"/>
-      <c r="C22" s="43" t="n"/>
-      <c r="D22" s="43" t="n"/>
-      <c r="E22" s="44" t="n"/>
-      <c r="F22" s="44" t="n"/>
-      <c r="G22" s="44" t="n"/>
-      <c r="H22" s="44" t="n"/>
-      <c r="I22" s="44" t="n"/>
-      <c r="J22" s="44" t="n"/>
-      <c r="K22" s="44" t="n"/>
-      <c r="L22" s="47" t="n"/>
-      <c r="M22" s="44" t="n"/>
-      <c r="N22" s="22" t="n"/>
-    </row>
-    <row r="23" ht="18" customHeight="1" s="74">
-      <c r="A23" s="52" t="n"/>
-      <c r="B23" s="45" t="n"/>
-      <c r="C23" s="46" t="n"/>
-      <c r="D23" s="46" t="n"/>
-      <c r="E23" s="47" t="n"/>
-      <c r="F23" s="47" t="n"/>
-      <c r="G23" s="47" t="n"/>
-      <c r="H23" s="47" t="n"/>
-      <c r="I23" s="47" t="n"/>
-      <c r="J23" s="47" t="n"/>
-      <c r="K23" s="47" t="n"/>
-      <c r="L23" s="47" t="n"/>
-      <c r="M23" s="47" t="n"/>
-      <c r="N23" s="22" t="n"/>
-    </row>
-    <row r="24" ht="18" customHeight="1" s="74">
-      <c r="A24" s="52" t="n"/>
-      <c r="B24" s="42" t="n"/>
-      <c r="C24" s="43" t="n"/>
-      <c r="D24" s="43" t="n"/>
-      <c r="E24" s="44" t="n"/>
-      <c r="F24" s="44" t="n"/>
-      <c r="G24" s="44" t="n"/>
-      <c r="H24" s="44" t="n"/>
-      <c r="I24" s="44" t="n"/>
-      <c r="J24" s="44" t="n"/>
-      <c r="K24" s="44" t="n"/>
-      <c r="L24" s="44" t="n"/>
-      <c r="M24" s="44" t="n"/>
-      <c r="N24" s="22" t="n"/>
-    </row>
-    <row r="25" ht="18" customHeight="1" s="74">
-      <c r="A25" s="52" t="n"/>
-      <c r="B25" s="45" t="n"/>
-      <c r="C25" s="46" t="n"/>
-      <c r="D25" s="46" t="n"/>
-      <c r="E25" s="47" t="n"/>
-      <c r="F25" s="47" t="n"/>
-      <c r="G25" s="47" t="n"/>
-      <c r="H25" s="47" t="n"/>
-      <c r="I25" s="47" t="n"/>
-      <c r="J25" s="47" t="n"/>
-      <c r="K25" s="47" t="n"/>
-      <c r="L25" s="47" t="n"/>
-      <c r="M25" s="47" t="n"/>
-      <c r="N25" s="22" t="n"/>
-    </row>
-    <row r="26" ht="18" customHeight="1" s="74">
-      <c r="A26" s="52" t="n"/>
-      <c r="B26" s="42" t="n"/>
-      <c r="C26" s="43" t="n"/>
-      <c r="D26" s="43" t="n"/>
-      <c r="E26" s="44" t="n"/>
-      <c r="F26" s="44" t="n"/>
-      <c r="G26" s="44" t="n"/>
-      <c r="H26" s="44" t="n"/>
-      <c r="I26" s="44" t="n"/>
-      <c r="J26" s="44" t="n"/>
-      <c r="K26" s="44" t="n"/>
-      <c r="L26" s="44" t="n"/>
-      <c r="M26" s="44" t="n"/>
-      <c r="N26" s="22" t="n"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" s="74">
-      <c r="A27" s="52" t="n"/>
-      <c r="B27" s="45" t="n"/>
-      <c r="C27" s="46" t="n"/>
-      <c r="D27" s="46" t="n"/>
-      <c r="E27" s="47" t="n"/>
-      <c r="F27" s="47" t="n"/>
-      <c r="G27" s="47" t="n"/>
-      <c r="H27" s="47" t="n"/>
-      <c r="I27" s="47" t="n"/>
-      <c r="J27" s="47" t="n"/>
-      <c r="K27" s="47" t="n"/>
-      <c r="L27" s="47" t="n"/>
-      <c r="M27" s="47" t="n"/>
-      <c r="N27" s="22" t="n"/>
-    </row>
-    <row r="28" ht="18" customHeight="1" s="74">
-      <c r="A28" s="52" t="n"/>
-      <c r="B28" s="42" t="n"/>
-      <c r="C28" s="43" t="n"/>
-      <c r="D28" s="43" t="n"/>
-      <c r="E28" s="44" t="n"/>
-      <c r="F28" s="44" t="n"/>
-      <c r="G28" s="44" t="n"/>
-      <c r="H28" s="44" t="n"/>
-      <c r="I28" s="44" t="n"/>
-      <c r="J28" s="44" t="n"/>
-      <c r="K28" s="44" t="n"/>
-      <c r="L28" s="44" t="n"/>
-      <c r="M28" s="44" t="n"/>
-      <c r="N28" s="22" t="n"/>
-    </row>
-    <row r="29" ht="18" customHeight="1" s="74">
-      <c r="A29" s="52" t="n"/>
-      <c r="B29" s="45" t="n"/>
-      <c r="C29" s="46" t="n"/>
-      <c r="D29" s="46" t="n"/>
-      <c r="E29" s="47" t="n"/>
-      <c r="F29" s="47" t="n"/>
-      <c r="G29" s="47" t="n"/>
-      <c r="H29" s="47" t="n"/>
-      <c r="I29" s="47" t="n"/>
-      <c r="J29" s="47" t="n"/>
-      <c r="K29" s="47" t="n"/>
-      <c r="L29" s="47" t="n"/>
-      <c r="M29" s="47" t="n"/>
-      <c r="N29" s="22" t="n"/>
-    </row>
-    <row r="30" ht="18" customFormat="1" customHeight="1" s="108">
-      <c r="A30" s="52" t="n"/>
-      <c r="B30" s="42" t="n"/>
-      <c r="C30" s="43" t="n"/>
-      <c r="D30" s="43" t="n"/>
-      <c r="E30" s="44" t="n"/>
-      <c r="F30" s="44" t="n"/>
-      <c r="G30" s="44" t="n"/>
-      <c r="H30" s="44" t="n"/>
-      <c r="I30" s="44" t="n"/>
-      <c r="J30" s="44" t="n"/>
-      <c r="K30" s="44" t="n"/>
-      <c r="L30" s="44" t="n"/>
-      <c r="M30" s="44" t="n"/>
-      <c r="N30" s="22" t="n"/>
-    </row>
-    <row r="31" ht="18" customFormat="1" customHeight="1" s="108">
-      <c r="A31" s="52" t="n"/>
-      <c r="B31" s="45" t="n"/>
-      <c r="C31" s="46" t="n"/>
-      <c r="D31" s="46" t="n"/>
-      <c r="E31" s="47" t="n"/>
-      <c r="F31" s="47" t="n"/>
-      <c r="G31" s="47" t="n"/>
-      <c r="H31" s="47" t="n"/>
-      <c r="I31" s="47" t="n"/>
-      <c r="J31" s="47" t="n"/>
-      <c r="K31" s="47" t="n"/>
-      <c r="L31" s="47" t="n"/>
-      <c r="M31" s="47" t="n"/>
-      <c r="N31" s="22" t="n"/>
-    </row>
-    <row r="32" ht="18" customHeight="1" s="74">
-      <c r="A32" s="52" t="n"/>
-      <c r="B32" s="36" t="n"/>
-      <c r="C32" s="20" t="n"/>
-      <c r="D32" s="20" t="n"/>
-      <c r="E32" s="21" t="n"/>
-      <c r="F32" s="21" t="n"/>
-      <c r="G32" s="21" t="n"/>
-      <c r="H32" s="21" t="n"/>
-      <c r="I32" s="21" t="n"/>
-      <c r="J32" s="21" t="n"/>
-      <c r="K32" s="21" t="n"/>
-      <c r="L32" s="21" t="n"/>
-      <c r="M32" s="21" t="n"/>
-      <c r="N32" s="22" t="n"/>
-    </row>
-    <row r="33" ht="26" customHeight="1" s="74">
-      <c r="A33" s="51" t="n"/>
-      <c r="B33" s="23" t="n"/>
-      <c r="C33" s="24" t="n"/>
-      <c r="D33" s="24" t="n"/>
-      <c r="E33" s="25" t="n"/>
-      <c r="F33" s="25" t="n"/>
-      <c r="G33" s="25" t="n"/>
-      <c r="H33" s="25" t="n"/>
-      <c r="I33" s="25" t="n"/>
-      <c r="J33" s="25" t="n"/>
-      <c r="K33" s="25" t="n"/>
-      <c r="L33" s="25" t="n"/>
-      <c r="M33" s="39" t="n"/>
-      <c r="N33" s="64" t="n"/>
-      <c r="O33" s="85" t="n"/>
-    </row>
-    <row r="34" ht="33.75" customHeight="1" s="74">
-      <c r="A34" s="51" t="n"/>
-      <c r="B34" s="37" t="n"/>
-      <c r="C34" s="26" t="n"/>
-      <c r="D34" s="26" t="n"/>
-      <c r="E34" s="62" t="n"/>
-      <c r="F34" s="62" t="n"/>
-      <c r="G34" s="62" t="n"/>
-      <c r="H34" s="62" t="n"/>
-      <c r="I34" s="62" t="n"/>
-      <c r="J34" s="62" t="n"/>
-      <c r="K34" s="62" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="M21" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="21" t="n"/>
+    </row>
+    <row r="22" ht="18" customHeight="1" s="78">
+      <c r="A22" s="51" t="n"/>
+      <c r="B22" s="41" t="n"/>
+      <c r="C22" s="42" t="n"/>
+      <c r="D22" s="42" t="n"/>
+      <c r="E22" s="43" t="n"/>
+      <c r="F22" s="43" t="n"/>
+      <c r="G22" s="43" t="n"/>
+      <c r="H22" s="43" t="n"/>
+      <c r="I22" s="43" t="n"/>
+      <c r="J22" s="43" t="n"/>
+      <c r="K22" s="43" t="n"/>
+      <c r="L22" s="46" t="n"/>
+      <c r="M22" s="43" t="n"/>
+      <c r="N22" s="21" t="n"/>
+    </row>
+    <row r="23" ht="18" customHeight="1" s="78">
+      <c r="A23" s="51" t="n"/>
+      <c r="B23" s="44" t="n"/>
+      <c r="C23" s="45" t="n"/>
+      <c r="D23" s="45" t="n"/>
+      <c r="E23" s="46" t="n"/>
+      <c r="F23" s="46" t="n"/>
+      <c r="G23" s="46" t="n"/>
+      <c r="H23" s="46" t="n"/>
+      <c r="I23" s="46" t="n"/>
+      <c r="J23" s="46" t="n"/>
+      <c r="K23" s="46" t="n"/>
+      <c r="L23" s="46" t="n"/>
+      <c r="M23" s="46" t="n"/>
+      <c r="N23" s="21" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="78">
+      <c r="A24" s="51" t="n"/>
+      <c r="B24" s="41" t="n"/>
+      <c r="C24" s="42" t="n"/>
+      <c r="D24" s="42" t="n"/>
+      <c r="E24" s="43" t="n"/>
+      <c r="F24" s="43" t="n"/>
+      <c r="G24" s="43" t="n"/>
+      <c r="H24" s="43" t="n"/>
+      <c r="I24" s="43" t="n"/>
+      <c r="J24" s="43" t="n"/>
+      <c r="K24" s="43" t="n"/>
+      <c r="L24" s="43" t="n"/>
+      <c r="M24" s="43" t="n"/>
+      <c r="N24" s="21" t="n"/>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="78">
+      <c r="A25" s="51" t="n"/>
+      <c r="B25" s="44" t="n"/>
+      <c r="C25" s="45" t="n"/>
+      <c r="D25" s="45" t="n"/>
+      <c r="E25" s="46" t="n"/>
+      <c r="F25" s="46" t="n"/>
+      <c r="G25" s="46" t="n"/>
+      <c r="H25" s="46" t="n"/>
+      <c r="I25" s="46" t="n"/>
+      <c r="J25" s="46" t="n"/>
+      <c r="K25" s="46" t="n"/>
+      <c r="L25" s="46" t="n"/>
+      <c r="M25" s="46" t="n"/>
+      <c r="N25" s="21" t="n"/>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="78">
+      <c r="A26" s="51" t="n"/>
+      <c r="B26" s="41" t="n"/>
+      <c r="C26" s="42" t="n"/>
+      <c r="D26" s="42" t="n"/>
+      <c r="E26" s="43" t="n"/>
+      <c r="F26" s="43" t="n"/>
+      <c r="G26" s="43" t="n"/>
+      <c r="H26" s="43" t="n"/>
+      <c r="I26" s="43" t="n"/>
+      <c r="J26" s="43" t="n"/>
+      <c r="K26" s="43" t="n"/>
+      <c r="L26" s="43" t="n"/>
+      <c r="M26" s="43" t="n"/>
+      <c r="N26" s="21" t="n"/>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="78">
+      <c r="A27" s="51" t="n"/>
+      <c r="B27" s="44" t="n"/>
+      <c r="C27" s="45" t="n"/>
+      <c r="D27" s="45" t="n"/>
+      <c r="E27" s="46" t="n"/>
+      <c r="F27" s="46" t="n"/>
+      <c r="G27" s="46" t="n"/>
+      <c r="H27" s="46" t="n"/>
+      <c r="I27" s="46" t="n"/>
+      <c r="J27" s="46" t="n"/>
+      <c r="K27" s="46" t="n"/>
+      <c r="L27" s="46" t="n"/>
+      <c r="M27" s="46" t="n"/>
+      <c r="N27" s="21" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1" s="78">
+      <c r="A28" s="51" t="n"/>
+      <c r="B28" s="41" t="n"/>
+      <c r="C28" s="42" t="n"/>
+      <c r="D28" s="42" t="n"/>
+      <c r="E28" s="43" t="n"/>
+      <c r="F28" s="43" t="n"/>
+      <c r="G28" s="43" t="n"/>
+      <c r="H28" s="43" t="n"/>
+      <c r="I28" s="43" t="n"/>
+      <c r="J28" s="43" t="n"/>
+      <c r="K28" s="43" t="n"/>
+      <c r="L28" s="43" t="n"/>
+      <c r="M28" s="43" t="n"/>
+      <c r="N28" s="21" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1" s="78">
+      <c r="A29" s="51" t="n"/>
+      <c r="B29" s="44" t="n"/>
+      <c r="C29" s="45" t="n"/>
+      <c r="D29" s="45" t="n"/>
+      <c r="E29" s="46" t="n"/>
+      <c r="F29" s="46" t="n"/>
+      <c r="G29" s="46" t="n"/>
+      <c r="H29" s="46" t="n"/>
+      <c r="I29" s="46" t="n"/>
+      <c r="J29" s="46" t="n"/>
+      <c r="K29" s="46" t="n"/>
+      <c r="L29" s="46" t="n"/>
+      <c r="M29" s="46" t="n"/>
+      <c r="N29" s="21" t="n"/>
+    </row>
+    <row r="30" ht="18" customFormat="1" customHeight="1" s="37">
+      <c r="A30" s="51" t="n"/>
+      <c r="B30" s="41" t="n"/>
+      <c r="C30" s="42" t="n"/>
+      <c r="D30" s="42" t="n"/>
+      <c r="E30" s="43" t="n"/>
+      <c r="F30" s="43" t="n"/>
+      <c r="G30" s="43" t="n"/>
+      <c r="H30" s="43" t="n"/>
+      <c r="I30" s="43" t="n"/>
+      <c r="J30" s="43" t="n"/>
+      <c r="K30" s="43" t="n"/>
+      <c r="L30" s="43" t="n"/>
+      <c r="M30" s="43" t="n"/>
+      <c r="N30" s="21" t="n"/>
+    </row>
+    <row r="31" ht="18" customFormat="1" customHeight="1" s="37">
+      <c r="A31" s="51" t="n"/>
+      <c r="B31" s="44" t="n"/>
+      <c r="C31" s="45" t="n"/>
+      <c r="D31" s="45" t="n"/>
+      <c r="E31" s="46" t="n"/>
+      <c r="F31" s="46" t="n"/>
+      <c r="G31" s="46" t="n"/>
+      <c r="H31" s="46" t="n"/>
+      <c r="I31" s="46" t="n"/>
+      <c r="J31" s="46" t="n"/>
+      <c r="K31" s="46" t="n"/>
+      <c r="L31" s="46" t="n"/>
+      <c r="M31" s="46" t="n"/>
+      <c r="N31" s="21" t="n"/>
+    </row>
+    <row r="32" ht="18" customHeight="1" s="78">
+      <c r="A32" s="51" t="n"/>
+      <c r="B32" s="35" t="n"/>
+      <c r="C32" s="19" t="n"/>
+      <c r="D32" s="19" t="n"/>
+      <c r="E32" s="20" t="n"/>
+      <c r="F32" s="20" t="n"/>
+      <c r="G32" s="20" t="n"/>
+      <c r="H32" s="20" t="n"/>
+      <c r="I32" s="20" t="n"/>
+      <c r="J32" s="20" t="n"/>
+      <c r="K32" s="20" t="n"/>
+      <c r="L32" s="20" t="n"/>
+      <c r="M32" s="20" t="n"/>
+      <c r="N32" s="21" t="n"/>
+    </row>
+    <row r="33" ht="26" customHeight="1" s="78">
+      <c r="A33" s="50" t="n"/>
+      <c r="B33" s="22" t="n"/>
+      <c r="C33" s="23" t="n"/>
+      <c r="D33" s="23" t="n"/>
+      <c r="E33" s="24" t="n"/>
+      <c r="F33" s="24" t="n"/>
+      <c r="G33" s="24" t="n"/>
+      <c r="H33" s="24" t="n"/>
+      <c r="I33" s="24" t="n"/>
+      <c r="J33" s="24" t="n"/>
+      <c r="K33" s="24" t="n"/>
+      <c r="L33" s="24" t="n"/>
+      <c r="M33" s="38" t="n"/>
+      <c r="N33" s="63" t="n"/>
+      <c r="O33" s="91" t="n"/>
+    </row>
+    <row r="34" ht="33.75" customHeight="1" s="78">
+      <c r="A34" s="50" t="n"/>
+      <c r="B34" s="36" t="n"/>
+      <c r="C34" s="25" t="n"/>
+      <c r="D34" s="25" t="n"/>
+      <c r="E34" s="61" t="n"/>
+      <c r="F34" s="61" t="n"/>
+      <c r="G34" s="61" t="n"/>
+      <c r="H34" s="61" t="n"/>
+      <c r="I34" s="61" t="n"/>
+      <c r="J34" s="61" t="n"/>
+      <c r="K34" s="61" t="inlineStr">
         <is>
           <t>Total:</t>
         </is>
       </c>
-      <c r="L34" s="82" t="n">
-        <v>206.15</v>
-      </c>
-      <c r="N34" s="63" t="n"/>
-      <c r="O34" s="85" t="n"/>
-    </row>
-    <row r="35" ht="9.75" customHeight="1" s="74">
-      <c r="A35" s="51" t="n"/>
-      <c r="B35" s="27" t="n"/>
-      <c r="C35" s="27" t="n"/>
-      <c r="D35" s="27" t="n"/>
-      <c r="E35" s="27" t="n"/>
-      <c r="F35" s="27" t="n"/>
-      <c r="G35" s="27" t="n"/>
-      <c r="H35" s="27" t="n"/>
-      <c r="I35" s="27" t="n"/>
-      <c r="J35" s="27" t="n"/>
-      <c r="K35" s="27" t="n"/>
-      <c r="L35" s="27" t="n"/>
-      <c r="M35" s="27" t="n"/>
-      <c r="N35" s="27" t="n"/>
-      <c r="O35" s="85" t="n"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1" s="74">
-      <c r="A36" s="51" t="n"/>
-      <c r="B36" s="91" t="n"/>
-      <c r="N36" s="28" t="n"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1" s="74">
-      <c r="A37" s="51" t="n"/>
-      <c r="B37" s="104" t="n"/>
-      <c r="N37" s="29" t="n"/>
-    </row>
-    <row r="38" ht="21" customHeight="1" s="74">
-      <c r="A38" s="53" t="n"/>
-      <c r="B38" s="103" t="n"/>
-      <c r="N38" s="30" t="n"/>
-    </row>
-    <row r="39" ht="8" customHeight="1" s="74">
-      <c r="A39" s="51" t="n"/>
+      <c r="L34" s="109" t="n">
+        <v>2</v>
+      </c>
+      <c r="N34" s="62" t="n"/>
+      <c r="O34" s="91" t="n"/>
+    </row>
+    <row r="35" ht="9.75" customHeight="1" s="78">
+      <c r="A35" s="50" t="n"/>
+      <c r="B35" s="26" t="n"/>
+      <c r="C35" s="26" t="n"/>
+      <c r="D35" s="26" t="n"/>
+      <c r="E35" s="26" t="n"/>
+      <c r="F35" s="26" t="n"/>
+      <c r="G35" s="26" t="n"/>
+      <c r="H35" s="26" t="n"/>
+      <c r="I35" s="26" t="n"/>
+      <c r="J35" s="26" t="n"/>
+      <c r="K35" s="26" t="n"/>
+      <c r="L35" s="26" t="n"/>
+      <c r="M35" s="26" t="n"/>
+      <c r="N35" s="26" t="n"/>
+      <c r="O35" s="91" t="n"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" s="78">
+      <c r="A36" s="50" t="n"/>
+      <c r="B36" s="88" t="n"/>
+      <c r="N36" s="27" t="n"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" s="78">
+      <c r="A37" s="50" t="n"/>
+      <c r="B37" s="95" t="n"/>
+      <c r="N37" s="28" t="n"/>
+    </row>
+    <row r="38" ht="21" customHeight="1" s="78">
+      <c r="A38" s="52" t="n"/>
+      <c r="B38" s="94" t="n"/>
+      <c r="N38" s="29" t="n"/>
+    </row>
+    <row r="39" ht="8" customHeight="1" s="78">
+      <c r="A39" s="50" t="n"/>
       <c r="B39" s="9" t="n"/>
-      <c r="C39" s="55" t="n"/>
-      <c r="D39" s="56" t="n"/>
-      <c r="E39" s="56" t="n"/>
-      <c r="F39" s="56" t="n"/>
-      <c r="G39" s="56" t="n"/>
-      <c r="H39" s="56" t="n"/>
-      <c r="I39" s="56" t="n"/>
-      <c r="J39" s="56" t="n"/>
-      <c r="K39" s="56" t="n"/>
-      <c r="L39" s="57" t="n"/>
+      <c r="C39" s="54" t="n"/>
+      <c r="D39" s="55" t="n"/>
+      <c r="E39" s="55" t="n"/>
+      <c r="F39" s="55" t="n"/>
+      <c r="G39" s="55" t="n"/>
+      <c r="H39" s="55" t="n"/>
+      <c r="I39" s="55" t="n"/>
+      <c r="J39" s="55" t="n"/>
+      <c r="K39" s="55" t="n"/>
+      <c r="L39" s="56" t="n"/>
       <c r="M39" s="9" t="n"/>
-      <c r="N39" s="48" t="n"/>
-    </row>
-    <row r="40" ht="24" customHeight="1" s="74">
-      <c r="A40" s="85" t="n"/>
-      <c r="C40" s="59" t="n"/>
-      <c r="D40" s="107" t="inlineStr">
+      <c r="N39" s="47" t="n"/>
+    </row>
+    <row r="40" ht="24" customHeight="1" s="78">
+      <c r="A40" s="91" t="n"/>
+      <c r="C40" s="58" t="n"/>
+      <c r="D40" s="82" t="inlineStr">
         <is>
           <t>Return instructions:</t>
         </is>
       </c>
-      <c r="I40" s="60" t="n"/>
-      <c r="J40" s="60" t="n"/>
-      <c r="K40" s="60" t="n"/>
-      <c r="L40" s="61" t="n"/>
-      <c r="N40" s="84" t="n"/>
-    </row>
-    <row r="41" ht="15" customHeight="1" s="74">
-      <c r="A41" s="85" t="n"/>
-      <c r="C41" s="59" t="n"/>
-      <c r="D41" s="60" t="n"/>
-      <c r="E41" s="60" t="n"/>
-      <c r="F41" s="60" t="n"/>
-      <c r="G41" s="60" t="n"/>
-      <c r="H41" s="60" t="n"/>
-      <c r="I41" s="60" t="n"/>
-      <c r="J41" s="60" t="n"/>
-      <c r="K41" s="60" t="n"/>
-      <c r="L41" s="61" t="n"/>
-      <c r="N41" s="84" t="n"/>
-    </row>
-    <row r="42" ht="17" customHeight="1" s="74">
-      <c r="A42" s="85" t="n"/>
-      <c r="C42" s="83" t="inlineStr">
+      <c r="I40" s="59" t="n"/>
+      <c r="J40" s="59" t="n"/>
+      <c r="K40" s="59" t="n"/>
+      <c r="L40" s="60" t="n"/>
+      <c r="N40" s="90" t="n"/>
+    </row>
+    <row r="41" ht="15" customHeight="1" s="78">
+      <c r="A41" s="91" t="n"/>
+      <c r="C41" s="58" t="n"/>
+      <c r="D41" s="59" t="n"/>
+      <c r="E41" s="59" t="n"/>
+      <c r="F41" s="59" t="n"/>
+      <c r="G41" s="59" t="n"/>
+      <c r="H41" s="59" t="n"/>
+      <c r="I41" s="59" t="n"/>
+      <c r="J41" s="59" t="n"/>
+      <c r="K41" s="59" t="n"/>
+      <c r="L41" s="60" t="n"/>
+      <c r="N41" s="90" t="n"/>
+    </row>
+    <row r="42" ht="17" customHeight="1" s="78">
+      <c r="A42" s="91" t="n"/>
+      <c r="C42" s="89" t="inlineStr">
         <is>
           <t>1. Email the Packing Slip to Customer Service via email to https://returns.healthcare.inmar.com request a Return Authorization (RGA).</t>
         </is>
       </c>
-      <c r="L42" s="84" t="n"/>
-      <c r="N42" s="84" t="n"/>
-    </row>
-    <row r="43" ht="3" customHeight="1" s="74">
-      <c r="A43" s="85" t="n"/>
-      <c r="C43" s="85" t="n"/>
-      <c r="L43" s="84" t="n"/>
-      <c r="N43" s="84" t="n"/>
-    </row>
-    <row r="44" ht="15" customHeight="1" s="74">
-      <c r="A44" s="85" t="n"/>
-      <c r="C44" s="83" t="inlineStr">
+      <c r="L42" s="90" t="n"/>
+      <c r="N42" s="90" t="n"/>
+    </row>
+    <row r="43" ht="3" customHeight="1" s="78">
+      <c r="A43" s="91" t="n"/>
+      <c r="C43" s="91" t="n"/>
+      <c r="L43" s="90" t="n"/>
+      <c r="N43" s="90" t="n"/>
+    </row>
+    <row r="44" ht="15" customHeight="1" s="78">
+      <c r="A44" s="91" t="n"/>
+      <c r="C44" s="89" t="inlineStr">
         <is>
           <t>2. Alternatively, you can create an RGA by logging in to https://clsnetlink.com</t>
         </is>
       </c>
-      <c r="L44" s="84" t="n"/>
-      <c r="N44" s="84" t="n"/>
-    </row>
-    <row r="45" ht="5" customHeight="1" s="74">
-      <c r="A45" s="85" t="n"/>
-      <c r="C45" s="85" t="n"/>
-      <c r="L45" s="84" t="n"/>
-      <c r="N45" s="84" t="n"/>
-    </row>
-    <row r="46" ht="31" customHeight="1" s="74">
-      <c r="A46" s="85" t="n"/>
-      <c r="C46" s="83" t="inlineStr">
+      <c r="L44" s="90" t="n"/>
+      <c r="N44" s="90" t="n"/>
+    </row>
+    <row r="45" ht="5" customHeight="1" s="78">
+      <c r="A45" s="91" t="n"/>
+      <c r="C45" s="91" t="n"/>
+      <c r="L45" s="90" t="n"/>
+      <c r="N45" s="90" t="n"/>
+    </row>
+    <row r="46" ht="31" customHeight="1" s="78">
+      <c r="A46" s="91" t="n"/>
+      <c r="C46" s="89" t="inlineStr">
         <is>
           <t>3. Upon receiving the Returned Goods Authorization Form (RGA), include the RGA along with the Packing Slip and ship the outdated products to the following address:</t>
         </is>
       </c>
-      <c r="L46" s="84" t="n"/>
-      <c r="N46" s="84" t="n"/>
-    </row>
-    <row r="47" ht="4" customHeight="1" s="74">
-      <c r="A47" s="85" t="n"/>
-      <c r="C47" s="85" t="n"/>
-      <c r="L47" s="84" t="n"/>
-      <c r="N47" s="84" t="n"/>
-    </row>
-    <row r="48" ht="18" customHeight="1" s="74">
-      <c r="A48" s="85" t="n"/>
-      <c r="C48" s="100" t="inlineStr">
+      <c r="L46" s="90" t="n"/>
+      <c r="N46" s="90" t="n"/>
+    </row>
+    <row r="47" ht="4" customHeight="1" s="78">
+      <c r="A47" s="91" t="n"/>
+      <c r="C47" s="91" t="n"/>
+      <c r="L47" s="90" t="n"/>
+      <c r="N47" s="90" t="n"/>
+    </row>
+    <row r="48" ht="18" customHeight="1" s="78">
+      <c r="A48" s="91" t="n"/>
+      <c r="C48" s="93" t="inlineStr">
         <is>
           <t>INMAR Pharmaceutical Services</t>
         </is>
       </c>
-      <c r="E48" s="60" t="n"/>
-      <c r="F48" s="60" t="n"/>
-      <c r="G48" s="60" t="n"/>
-      <c r="H48" s="60" t="n"/>
-      <c r="I48" s="60" t="n"/>
-      <c r="J48" s="60" t="n"/>
-      <c r="K48" s="60" t="n"/>
-      <c r="L48" s="61" t="n"/>
-      <c r="N48" s="84" t="n"/>
-    </row>
-    <row r="49" ht="17" customHeight="1" s="74">
-      <c r="A49" s="85" t="n"/>
+      <c r="E48" s="59" t="n"/>
+      <c r="F48" s="59" t="n"/>
+      <c r="G48" s="59" t="n"/>
+      <c r="H48" s="59" t="n"/>
+      <c r="I48" s="59" t="n"/>
+      <c r="J48" s="59" t="n"/>
+      <c r="K48" s="59" t="n"/>
+      <c r="L48" s="60" t="n"/>
+      <c r="N48" s="90" t="n"/>
+    </row>
+    <row r="49" ht="17" customHeight="1" s="78">
+      <c r="A49" s="91" t="n"/>
       <c r="C49" s="92" t="inlineStr">
         <is>
           <t>4332 Empire Road</t>
         </is>
       </c>
-      <c r="E49" s="60" t="n"/>
-      <c r="F49" s="60" t="n"/>
-      <c r="G49" s="60" t="n"/>
-      <c r="H49" s="60" t="n"/>
-      <c r="I49" s="60" t="n"/>
-      <c r="J49" s="60" t="n"/>
-      <c r="K49" s="60" t="n"/>
-      <c r="L49" s="61" t="n"/>
-      <c r="N49" s="84" t="n"/>
-    </row>
-    <row r="50" ht="18" customHeight="1" s="74">
-      <c r="A50" s="85" t="n"/>
+      <c r="E49" s="59" t="n"/>
+      <c r="F49" s="59" t="n"/>
+      <c r="G49" s="59" t="n"/>
+      <c r="H49" s="59" t="n"/>
+      <c r="I49" s="59" t="n"/>
+      <c r="J49" s="59" t="n"/>
+      <c r="K49" s="59" t="n"/>
+      <c r="L49" s="60" t="n"/>
+      <c r="N49" s="90" t="n"/>
+    </row>
+    <row r="50" ht="18" customHeight="1" s="78">
+      <c r="A50" s="91" t="n"/>
       <c r="C50" s="92" t="inlineStr">
         <is>
           <t>Fort Worth, TX 76155</t>
         </is>
       </c>
-      <c r="E50" s="60" t="n"/>
-      <c r="F50" s="60" t="n"/>
-      <c r="G50" s="60" t="n"/>
-      <c r="H50" s="60" t="n"/>
-      <c r="I50" s="60" t="n"/>
-      <c r="J50" s="60" t="n"/>
-      <c r="K50" s="60" t="n"/>
-      <c r="L50" s="61" t="n"/>
-      <c r="N50" s="84" t="n"/>
-    </row>
-    <row r="51" hidden="1" ht="18" customHeight="1" s="74">
-      <c r="A51" s="85" t="n"/>
-      <c r="C51" s="59" t="n"/>
-      <c r="D51" s="60" t="n"/>
-      <c r="E51" s="60" t="n"/>
-      <c r="F51" s="60" t="n"/>
-      <c r="G51" s="60" t="n"/>
-      <c r="H51" s="60" t="n"/>
-      <c r="I51" s="60" t="n"/>
-      <c r="J51" s="60" t="n"/>
-      <c r="K51" s="60" t="n"/>
-      <c r="L51" s="61" t="n"/>
-      <c r="N51" s="84" t="n"/>
-    </row>
-    <row r="52" ht="15" customHeight="1" s="74">
-      <c r="A52" s="85" t="n"/>
-      <c r="C52" s="89" t="inlineStr">
+      <c r="E50" s="59" t="n"/>
+      <c r="F50" s="59" t="n"/>
+      <c r="G50" s="59" t="n"/>
+      <c r="H50" s="59" t="n"/>
+      <c r="I50" s="59" t="n"/>
+      <c r="J50" s="59" t="n"/>
+      <c r="K50" s="59" t="n"/>
+      <c r="L50" s="60" t="n"/>
+      <c r="N50" s="90" t="n"/>
+    </row>
+    <row r="51" hidden="1" ht="18" customHeight="1" s="78">
+      <c r="A51" s="91" t="n"/>
+      <c r="C51" s="58" t="n"/>
+      <c r="D51" s="59" t="n"/>
+      <c r="E51" s="59" t="n"/>
+      <c r="F51" s="59" t="n"/>
+      <c r="G51" s="59" t="n"/>
+      <c r="H51" s="59" t="n"/>
+      <c r="I51" s="59" t="n"/>
+      <c r="J51" s="59" t="n"/>
+      <c r="K51" s="59" t="n"/>
+      <c r="L51" s="60" t="n"/>
+      <c r="N51" s="90" t="n"/>
+    </row>
+    <row r="52" ht="15" customHeight="1" s="78">
+      <c r="A52" s="91" t="n"/>
+      <c r="C52" s="84" t="inlineStr">
         <is>
           <t>Please DO NOT mix products from multiple debit memos/packing slips in one shipment. In case of any questions, please contact INMAR customer service at 1-800-967-5952</t>
         </is>
       </c>
-      <c r="L52" s="84" t="n"/>
-      <c r="N52" s="84" t="n"/>
-    </row>
-    <row r="53" ht="15" customHeight="1" s="74">
-      <c r="A53" s="85" t="n"/>
-      <c r="C53" s="85" t="n"/>
-      <c r="L53" s="84" t="n"/>
-      <c r="N53" s="84" t="n"/>
-    </row>
-    <row r="54" ht="15" customHeight="1" s="74">
-      <c r="A54" s="85" t="n"/>
-      <c r="C54" s="66" t="n"/>
-      <c r="D54" s="67" t="n"/>
-      <c r="E54" s="67" t="n"/>
-      <c r="F54" s="67" t="n"/>
-      <c r="G54" s="67" t="n"/>
-      <c r="H54" s="67" t="n"/>
-      <c r="I54" s="67" t="n"/>
-      <c r="J54" s="67" t="n"/>
-      <c r="K54" s="67" t="n"/>
-      <c r="L54" s="68" t="n"/>
-      <c r="N54" s="84" t="n"/>
-    </row>
-    <row r="55" ht="15" customHeight="1" s="74">
-      <c r="A55" s="85" t="n"/>
-      <c r="N55" s="84" t="n"/>
-    </row>
-    <row r="56" ht="15" customHeight="1" s="74">
-      <c r="A56" s="85" t="n"/>
-      <c r="N56" s="84" t="n"/>
-    </row>
-    <row r="57" ht="15.75" customHeight="1" s="74">
-      <c r="A57" s="54" t="n"/>
-      <c r="B57" s="31" t="n"/>
-      <c r="C57" s="31" t="n"/>
-      <c r="D57" s="31" t="n"/>
-      <c r="E57" s="31" t="n"/>
-      <c r="F57" s="31" t="n"/>
-      <c r="G57" s="31" t="n"/>
-      <c r="H57" s="31" t="n"/>
-      <c r="I57" s="31" t="n"/>
-      <c r="J57" s="31" t="n"/>
-      <c r="K57" s="31" t="n"/>
-      <c r="L57" s="31" t="n"/>
-      <c r="M57" s="31" t="n"/>
-      <c r="N57" s="50" t="n"/>
+      <c r="L52" s="90" t="n"/>
+      <c r="N52" s="90" t="n"/>
+    </row>
+    <row r="53" ht="25" customFormat="1" customHeight="1" s="117">
+      <c r="A53" s="72" t="n"/>
+      <c r="C53" s="91" t="n"/>
+      <c r="L53" s="90" t="n"/>
+      <c r="N53" s="74" t="n"/>
+    </row>
+    <row r="54" ht="15" customHeight="1" s="78">
+      <c r="A54" s="91" t="n"/>
+      <c r="C54" s="65" t="n"/>
+      <c r="D54" s="66" t="n"/>
+      <c r="E54" s="66" t="n"/>
+      <c r="F54" s="66" t="n"/>
+      <c r="G54" s="66" t="n"/>
+      <c r="H54" s="66" t="n"/>
+      <c r="I54" s="66" t="n"/>
+      <c r="J54" s="66" t="n"/>
+      <c r="K54" s="66" t="n"/>
+      <c r="L54" s="67" t="n"/>
+      <c r="N54" s="90" t="n"/>
+    </row>
+    <row r="55" ht="15" customHeight="1" s="78">
+      <c r="A55" s="91" t="n"/>
+      <c r="N55" s="90" t="n"/>
+    </row>
+    <row r="56" ht="15" customHeight="1" s="78">
+      <c r="A56" s="91" t="n"/>
+      <c r="N56" s="90" t="n"/>
+    </row>
+    <row r="57" ht="15.75" customHeight="1" s="78">
+      <c r="A57" s="53" t="n"/>
+      <c r="B57" s="30" t="n"/>
+      <c r="C57" s="30" t="n"/>
+      <c r="D57" s="30" t="n"/>
+      <c r="E57" s="30" t="n"/>
+      <c r="F57" s="30" t="n"/>
+      <c r="G57" s="30" t="n"/>
+      <c r="H57" s="30" t="n"/>
+      <c r="I57" s="30" t="n"/>
+      <c r="J57" s="30" t="n"/>
+      <c r="K57" s="30" t="n"/>
+      <c r="L57" s="30" t="n"/>
+      <c r="M57" s="30" t="n"/>
+      <c r="N57" s="49" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="45">
@@ -3031,10 +3054,10 @@
     <mergeCell ref="D40:H40"/>
     <mergeCell ref="E6:M6"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="H14:K14"/>
     <mergeCell ref="B38:M38"/>
     <mergeCell ref="C44:L45"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="H8:K8"/>
@@ -3056,8 +3079,8 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C17:M17"/>
+    <mergeCell ref="L34:M34"/>
     <mergeCell ref="B3:J3"/>
-    <mergeCell ref="L34:M34"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="H11:K11"/>

</xml_diff>

<commit_message>
basic setup for boxes is done with header added and boxes are listed and exporting to debit memo can be done anytime, create templated for inventory
</commit_message>
<xml_diff>
--- a/docs/invoice.xlsx
+++ b/docs/invoice.xlsx
@@ -2168,7 +2168,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="69" t="inlineStr">
         <is>
-          <t>01/25/2024</t>
+          <t>02/06/2024</t>
         </is>
       </c>
       <c r="D5" s="106" t="n"/>
@@ -2181,7 +2181,7 @@
       <c r="K5" s="97" t="n"/>
       <c r="L5" s="110" t="inlineStr">
         <is>
-          <t>QR01252024AP401</t>
+          <t>QR02062024LP01</t>
         </is>
       </c>
       <c r="M5" s="111" t="n"/>
@@ -2241,17 +2241,17 @@
       <c r="A10" s="50" t="n"/>
       <c r="B10" s="114" t="inlineStr">
         <is>
-          <t>AUTREY PHARMACY 4</t>
+          <t>LM PHARMACY</t>
         </is>
       </c>
       <c r="D10" s="115" t="inlineStr">
         <is>
-          <t>AMERISOURCEBERGEN DRUG CORPORATION</t>
+          <t>KINARY</t>
         </is>
       </c>
       <c r="E10" s="118" t="inlineStr">
         <is>
-          <t>AUTREY PHARMACY 4</t>
+          <t>LM PHARMACY</t>
         </is>
       </c>
       <c r="H10" s="101" t="n"/>
@@ -2263,17 +2263,17 @@
       <c r="A11" s="50" t="n"/>
       <c r="B11" s="114" t="inlineStr">
         <is>
-          <t>3503 BOCA CHICA BLVD, SUITE 1</t>
+          <t>900W SAM HOUSTON BLVD STE 3</t>
         </is>
       </c>
       <c r="D11" s="115" t="inlineStr">
         <is>
-          <t>108 ROUTE 17K SUITE 1</t>
+          <t>152.35 TENTH AVE</t>
         </is>
       </c>
       <c r="E11" s="118" t="inlineStr">
         <is>
-          <t>3503 BOCA CHICA BLVD, SUITE 1</t>
+          <t>900W SAM HOUSTON BLVD STE 3</t>
         </is>
       </c>
       <c r="H11" s="79" t="n"/>
@@ -2285,17 +2285,17 @@
       <c r="A12" s="50" t="n"/>
       <c r="B12" s="114" t="inlineStr">
         <is>
-          <t>BROWNSVILLE, TX, 78521</t>
+          <t>PHARR, TX 78577</t>
         </is>
       </c>
       <c r="D12" s="115" t="inlineStr">
         <is>
-          <t>NEWBURGH. NY, 12550-5008</t>
+          <t>WHITESTONE, NY,11357</t>
         </is>
       </c>
       <c r="E12" s="118" t="inlineStr">
         <is>
-          <t>BROWNSVILLE, TX, 78521</t>
+          <t>PHARR, TX 78577</t>
         </is>
       </c>
       <c r="H12" s="79" t="n"/>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="D13" s="115" t="inlineStr">
         <is>
-          <t>Account#: 100199545</t>
+          <t xml:space="preserve">Account#: </t>
         </is>
       </c>
       <c r="E13" s="118" t="inlineStr">
@@ -2329,17 +2329,17 @@
       <c r="A14" s="50" t="n"/>
       <c r="B14" s="114" t="inlineStr">
         <is>
-          <t xml:space="preserve">Phone: 956-621-1000, fax: </t>
+          <t xml:space="preserve">Phone: 201-595-1234, fax: </t>
         </is>
       </c>
       <c r="D14" s="118" t="inlineStr">
         <is>
-          <t>Phone: 844-222-2273</t>
+          <t>Phone: 718-767-1234/ 888-527-6806</t>
         </is>
       </c>
       <c r="E14" s="118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Phone: 956-621-1000, fax: </t>
+          <t xml:space="preserve">Phone: 201-595-1234, fax: </t>
         </is>
       </c>
       <c r="H14" s="83" t="n"/>
@@ -2351,17 +2351,17 @@
       <c r="A15" s="50" t="n"/>
       <c r="B15" s="114" t="inlineStr">
         <is>
-          <t>DEA: FA6707511, Exp: 06/30/2023</t>
+          <t>DEA: BL5101009, Exp: 08/31/2023</t>
         </is>
       </c>
       <c r="D15" s="118" t="inlineStr">
         <is>
-          <t>DEA: RA0522056</t>
+          <t>DEA: RK0416900</t>
         </is>
       </c>
       <c r="E15" s="118" t="inlineStr">
         <is>
-          <t>DEA: FA6707511, Exp: 06/30/2023</t>
+          <t>DEA: BL5101009, Exp: 08/31/2023</t>
         </is>
       </c>
       <c r="H15" s="83" t="n"/>
@@ -2477,22 +2477,22 @@
       <c r="A20" s="51" t="n"/>
       <c r="B20" s="41" t="inlineStr">
         <is>
-          <t>6787743305</t>
+          <t>2315574603</t>
         </is>
       </c>
       <c r="C20" s="42" t="inlineStr">
         <is>
-          <t>Ascend Laboratories, LLC</t>
+          <t>Avet Pharmaceuticals Inc.</t>
         </is>
       </c>
       <c r="D20" s="42" t="inlineStr">
         <is>
-          <t>Aripiprazole</t>
+          <t>Rasagiline mesylate</t>
         </is>
       </c>
       <c r="E20" s="43" t="inlineStr">
         <is>
-          <t>15 mg/1</t>
+          <t>.5 mg/1</t>
         </is>
       </c>
       <c r="F20" s="43" t="inlineStr">
@@ -2502,17 +2502,17 @@
       </c>
       <c r="G20" s="43" t="inlineStr">
         <is>
-          <t>22140477</t>
+          <t>RCY01AD6</t>
         </is>
       </c>
       <c r="H20" s="43" t="inlineStr">
         <is>
-          <t>01/24/31</t>
+          <t>12/23/31</t>
         </is>
       </c>
       <c r="I20" s="43" t="inlineStr">
         <is>
-          <t>500 CT</t>
+          <t>30 CT</t>
         </is>
       </c>
       <c r="J20" s="43" t="n">
@@ -2531,22 +2531,22 @@
       <c r="A21" s="51" t="n"/>
       <c r="B21" s="44" t="inlineStr">
         <is>
-          <t>6787743305</t>
+          <t>6275651818</t>
         </is>
       </c>
       <c r="C21" s="45" t="inlineStr">
         <is>
-          <t>Ascend Laboratories, LLC</t>
+          <t>Sun Pharmaceutical Industries, Inc.</t>
         </is>
       </c>
       <c r="D21" s="45" t="inlineStr">
         <is>
-          <t>Aripiprazole</t>
+          <t>CARBIDOPA AND LEVODOPA</t>
         </is>
       </c>
       <c r="E21" s="46" t="inlineStr">
         <is>
-          <t>15 mg/1</t>
+          <t>25 mg/1</t>
         </is>
       </c>
       <c r="F21" s="46" t="inlineStr">
@@ -2556,17 +2556,17 @@
       </c>
       <c r="G21" s="46" t="inlineStr">
         <is>
-          <t>22140477</t>
+          <t>HAD1849A</t>
         </is>
       </c>
       <c r="H21" s="46" t="inlineStr">
         <is>
-          <t>01/24/31</t>
+          <t>04/24/30</t>
         </is>
       </c>
       <c r="I21" s="46" t="inlineStr">
         <is>
-          <t>500 CT</t>
+          <t>1000 CT</t>
         </is>
       </c>
       <c r="J21" s="46" t="n">

</xml_diff>

<commit_message>
inventory page developed and functionalities added
</commit_message>
<xml_diff>
--- a/docs/invoice.xlsx
+++ b/docs/invoice.xlsx
@@ -2168,7 +2168,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="69" t="inlineStr">
         <is>
-          <t>02/06/2024</t>
+          <t>02/14/2024</t>
         </is>
       </c>
       <c r="D5" s="106" t="n"/>
@@ -2181,7 +2181,7 @@
       <c r="K5" s="97" t="n"/>
       <c r="L5" s="110" t="inlineStr">
         <is>
-          <t>QR02062024LP01</t>
+          <t>QR02142024AP101</t>
         </is>
       </c>
       <c r="M5" s="111" t="n"/>
@@ -2241,17 +2241,17 @@
       <c r="A10" s="50" t="n"/>
       <c r="B10" s="114" t="inlineStr">
         <is>
-          <t>LM PHARMACY</t>
+          <t>AUTREY PHARMACY 1</t>
         </is>
       </c>
       <c r="D10" s="115" t="inlineStr">
         <is>
-          <t>KINARY</t>
+          <t>AMERISOURCEBERGEN DRUG CORPORATION</t>
         </is>
       </c>
       <c r="E10" s="118" t="inlineStr">
         <is>
-          <t>LM PHARMACY</t>
+          <t>AUTREY PHARMACY 1</t>
         </is>
       </c>
       <c r="H10" s="101" t="n"/>
@@ -2263,17 +2263,17 @@
       <c r="A11" s="50" t="n"/>
       <c r="B11" s="114" t="inlineStr">
         <is>
-          <t>900W SAM HOUSTON BLVD STE 3</t>
+          <t>1205 CENTRAL BLVD</t>
         </is>
       </c>
       <c r="D11" s="115" t="inlineStr">
         <is>
-          <t>152.35 TENTH AVE</t>
+          <t>108 ROUTE 17K SUITE 1</t>
         </is>
       </c>
       <c r="E11" s="118" t="inlineStr">
         <is>
-          <t>900W SAM HOUSTON BLVD STE 3</t>
+          <t>1205 CENTRAL BLVD</t>
         </is>
       </c>
       <c r="H11" s="79" t="n"/>
@@ -2285,17 +2285,17 @@
       <c r="A12" s="50" t="n"/>
       <c r="B12" s="114" t="inlineStr">
         <is>
-          <t>PHARR, TX 78577</t>
+          <t>BROWNSVILLE, TX, 78520</t>
         </is>
       </c>
       <c r="D12" s="115" t="inlineStr">
         <is>
-          <t>WHITESTONE, NY,11357</t>
+          <t>NEWBURGH. NY, 12550-5008</t>
         </is>
       </c>
       <c r="E12" s="118" t="inlineStr">
         <is>
-          <t>PHARR, TX 78577</t>
+          <t>BROWNSVILLE, TX, 78520</t>
         </is>
       </c>
       <c r="H12" s="79" t="n"/>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="D13" s="115" t="inlineStr">
         <is>
-          <t xml:space="preserve">Account#: </t>
+          <t>Account#: 100199545</t>
         </is>
       </c>
       <c r="E13" s="118" t="inlineStr">
@@ -2329,17 +2329,17 @@
       <c r="A14" s="50" t="n"/>
       <c r="B14" s="114" t="inlineStr">
         <is>
-          <t xml:space="preserve">Phone: 201-595-1234, fax: </t>
+          <t xml:space="preserve">Phone: 956-548-0801, fax: </t>
         </is>
       </c>
       <c r="D14" s="118" t="inlineStr">
         <is>
-          <t>Phone: 718-767-1234/ 888-527-6806</t>
+          <t>Phone: 844-222-2273</t>
         </is>
       </c>
       <c r="E14" s="118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Phone: 201-595-1234, fax: </t>
+          <t xml:space="preserve">Phone: 956-548-0801, fax: </t>
         </is>
       </c>
       <c r="H14" s="83" t="n"/>
@@ -2351,17 +2351,17 @@
       <c r="A15" s="50" t="n"/>
       <c r="B15" s="114" t="inlineStr">
         <is>
-          <t>DEA: BL5101009, Exp: 08/31/2023</t>
+          <t>DEA: FA3704358, Exp: 06/30/2023</t>
         </is>
       </c>
       <c r="D15" s="118" t="inlineStr">
         <is>
-          <t>DEA: RK0416900</t>
+          <t>DEA: RA0522056</t>
         </is>
       </c>
       <c r="E15" s="118" t="inlineStr">
         <is>
-          <t>DEA: BL5101009, Exp: 08/31/2023</t>
+          <t>DEA: FA3704358, Exp: 06/30/2023</t>
         </is>
       </c>
       <c r="H15" s="83" t="n"/>
@@ -2477,22 +2477,22 @@
       <c r="A20" s="51" t="n"/>
       <c r="B20" s="41" t="inlineStr">
         <is>
-          <t>2315574603</t>
+          <t>6787743305</t>
         </is>
       </c>
       <c r="C20" s="42" t="inlineStr">
         <is>
-          <t>Avet Pharmaceuticals Inc.</t>
+          <t>Ascend Laboratories, LLC</t>
         </is>
       </c>
       <c r="D20" s="42" t="inlineStr">
         <is>
-          <t>Rasagiline mesylate</t>
+          <t>Aripiprazole</t>
         </is>
       </c>
       <c r="E20" s="43" t="inlineStr">
         <is>
-          <t>.5 mg/1</t>
+          <t>15 mg/1</t>
         </is>
       </c>
       <c r="F20" s="43" t="inlineStr">
@@ -2502,17 +2502,17 @@
       </c>
       <c r="G20" s="43" t="inlineStr">
         <is>
-          <t>RCY01AD6</t>
+          <t>22140477</t>
         </is>
       </c>
       <c r="H20" s="43" t="inlineStr">
         <is>
-          <t>12/23/31</t>
+          <t>01/24/31</t>
         </is>
       </c>
       <c r="I20" s="43" t="inlineStr">
         <is>
-          <t>30 CT</t>
+          <t>500 CT</t>
         </is>
       </c>
       <c r="J20" s="43" t="n">
@@ -2531,22 +2531,22 @@
       <c r="A21" s="51" t="n"/>
       <c r="B21" s="44" t="inlineStr">
         <is>
-          <t>6275651818</t>
+          <t>6787743305</t>
         </is>
       </c>
       <c r="C21" s="45" t="inlineStr">
         <is>
-          <t>Sun Pharmaceutical Industries, Inc.</t>
+          <t>Ascend Laboratories, LLC</t>
         </is>
       </c>
       <c r="D21" s="45" t="inlineStr">
         <is>
-          <t>CARBIDOPA AND LEVODOPA</t>
+          <t>Aripiprazole</t>
         </is>
       </c>
       <c r="E21" s="46" t="inlineStr">
         <is>
-          <t>25 mg/1</t>
+          <t>15 mg/1</t>
         </is>
       </c>
       <c r="F21" s="46" t="inlineStr">
@@ -2556,17 +2556,17 @@
       </c>
       <c r="G21" s="46" t="inlineStr">
         <is>
-          <t>HAD1849A</t>
+          <t>22140477</t>
         </is>
       </c>
       <c r="H21" s="46" t="inlineStr">
         <is>
-          <t>04/24/30</t>
+          <t>01/24/31</t>
         </is>
       </c>
       <c r="I21" s="46" t="inlineStr">
         <is>
-          <t>1000 CT</t>
+          <t>500 CT</t>
         </is>
       </c>
       <c r="J21" s="46" t="n">
@@ -2594,7 +2594,9 @@
       <c r="J22" s="43" t="n"/>
       <c r="K22" s="43" t="n"/>
       <c r="L22" s="46" t="n"/>
-      <c r="M22" s="43" t="n"/>
+      <c r="M22" s="43" t="n">
+        <v>1</v>
+      </c>
       <c r="N22" s="21" t="n"/>
     </row>
     <row r="23" ht="18" customHeight="1" s="78">

</xml_diff>

<commit_message>
adding medicine code worked out
</commit_message>
<xml_diff>
--- a/docs/invoice.xlsx
+++ b/docs/invoice.xlsx
@@ -2168,7 +2168,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="69" t="inlineStr">
         <is>
-          <t>02/14/2024</t>
+          <t>02/20/2024</t>
         </is>
       </c>
       <c r="D5" s="106" t="n"/>
@@ -2181,7 +2181,7 @@
       <c r="K5" s="97" t="n"/>
       <c r="L5" s="110" t="inlineStr">
         <is>
-          <t>QR02142024AP101</t>
+          <t>QR02202024AP101</t>
         </is>
       </c>
       <c r="M5" s="111" t="n"/>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="D10" s="115" t="inlineStr">
         <is>
-          <t>AMERISOURCEBERGEN DRUG CORPORATION</t>
+          <t>KINARY</t>
         </is>
       </c>
       <c r="E10" s="118" t="inlineStr">
@@ -2268,7 +2268,7 @@
       </c>
       <c r="D11" s="115" t="inlineStr">
         <is>
-          <t>108 ROUTE 17K SUITE 1</t>
+          <t>152.35 TENTH AVE</t>
         </is>
       </c>
       <c r="E11" s="118" t="inlineStr">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="D12" s="115" t="inlineStr">
         <is>
-          <t>NEWBURGH. NY, 12550-5008</t>
+          <t>WHITESTONE, NY,11357</t>
         </is>
       </c>
       <c r="E12" s="118" t="inlineStr">
@@ -2312,7 +2312,7 @@
       </c>
       <c r="D13" s="115" t="inlineStr">
         <is>
-          <t>Account#: 100199545</t>
+          <t xml:space="preserve">Account#: </t>
         </is>
       </c>
       <c r="E13" s="118" t="inlineStr">
@@ -2334,7 +2334,7 @@
       </c>
       <c r="D14" s="118" t="inlineStr">
         <is>
-          <t>Phone: 844-222-2273</t>
+          <t>Phone: 718-767-1234/ 888-527-6806</t>
         </is>
       </c>
       <c r="E14" s="118" t="inlineStr">
@@ -2356,7 +2356,7 @@
       </c>
       <c r="D15" s="118" t="inlineStr">
         <is>
-          <t>DEA: RA0522056</t>
+          <t>DEA: RK0416900</t>
         </is>
       </c>
       <c r="E15" s="118" t="inlineStr">
@@ -2477,22 +2477,22 @@
       <c r="A20" s="51" t="n"/>
       <c r="B20" s="41" t="inlineStr">
         <is>
-          <t>6787743305</t>
+          <t>2315574603</t>
         </is>
       </c>
       <c r="C20" s="42" t="inlineStr">
         <is>
-          <t>Ascend Laboratories, LLC</t>
+          <t>Avet Pharmaceuticals Inc.</t>
         </is>
       </c>
       <c r="D20" s="42" t="inlineStr">
         <is>
-          <t>Aripiprazole</t>
+          <t>Rasagiline mesylate</t>
         </is>
       </c>
       <c r="E20" s="43" t="inlineStr">
         <is>
-          <t>15 mg/1</t>
+          <t>.5 mg/1</t>
         </is>
       </c>
       <c r="F20" s="43" t="inlineStr">
@@ -2502,17 +2502,17 @@
       </c>
       <c r="G20" s="43" t="inlineStr">
         <is>
-          <t>22140477</t>
+          <t>RCY01AD6</t>
         </is>
       </c>
       <c r="H20" s="43" t="inlineStr">
         <is>
-          <t>01/24/31</t>
+          <t>12/23/31</t>
         </is>
       </c>
       <c r="I20" s="43" t="inlineStr">
         <is>
-          <t>500 CT</t>
+          <t>30 CT</t>
         </is>
       </c>
       <c r="J20" s="43" t="n">
@@ -2531,22 +2531,22 @@
       <c r="A21" s="51" t="n"/>
       <c r="B21" s="44" t="inlineStr">
         <is>
-          <t>6787743305</t>
+          <t>2315574603</t>
         </is>
       </c>
       <c r="C21" s="45" t="inlineStr">
         <is>
-          <t>Ascend Laboratories, LLC</t>
+          <t>Avet Pharmaceuticals Inc.</t>
         </is>
       </c>
       <c r="D21" s="45" t="inlineStr">
         <is>
-          <t>Aripiprazole</t>
+          <t>Rasagiline mesylate</t>
         </is>
       </c>
       <c r="E21" s="46" t="inlineStr">
         <is>
-          <t>15 mg/1</t>
+          <t>.5 mg/1</t>
         </is>
       </c>
       <c r="F21" s="46" t="inlineStr">
@@ -2556,17 +2556,17 @@
       </c>
       <c r="G21" s="46" t="inlineStr">
         <is>
-          <t>22140477</t>
+          <t>RCY01AD6</t>
         </is>
       </c>
       <c r="H21" s="46" t="inlineStr">
         <is>
-          <t>01/24/31</t>
+          <t>12/23/31</t>
         </is>
       </c>
       <c r="I21" s="46" t="inlineStr">
         <is>
-          <t>500 CT</t>
+          <t>30 CT</t>
         </is>
       </c>
       <c r="J21" s="46" t="n">
@@ -2583,17 +2583,53 @@
     </row>
     <row r="22" ht="18" customHeight="1" s="78">
       <c r="A22" s="51" t="n"/>
-      <c r="B22" s="41" t="n"/>
-      <c r="C22" s="42" t="n"/>
-      <c r="D22" s="42" t="n"/>
-      <c r="E22" s="43" t="n"/>
-      <c r="F22" s="43" t="n"/>
-      <c r="G22" s="43" t="n"/>
-      <c r="H22" s="43" t="n"/>
-      <c r="I22" s="43" t="n"/>
-      <c r="J22" s="43" t="n"/>
+      <c r="B22" s="41" t="inlineStr">
+        <is>
+          <t>2315574603</t>
+        </is>
+      </c>
+      <c r="C22" s="42" t="inlineStr">
+        <is>
+          <t>Avet Pharmaceuticals Inc.</t>
+        </is>
+      </c>
+      <c r="D22" s="42" t="inlineStr">
+        <is>
+          <t>Rasagiline mesylate</t>
+        </is>
+      </c>
+      <c r="E22" s="43" t="inlineStr">
+        <is>
+          <t>.5 mg/1</t>
+        </is>
+      </c>
+      <c r="F22" s="43" t="inlineStr">
+        <is>
+          <t>TABLET</t>
+        </is>
+      </c>
+      <c r="G22" s="43" t="inlineStr">
+        <is>
+          <t>RCY01AD6</t>
+        </is>
+      </c>
+      <c r="H22" s="43" t="inlineStr">
+        <is>
+          <t>12/23/31</t>
+        </is>
+      </c>
+      <c r="I22" s="43" t="inlineStr">
+        <is>
+          <t>30 CT</t>
+        </is>
+      </c>
+      <c r="J22" s="43" t="n">
+        <v>1</v>
+      </c>
       <c r="K22" s="43" t="n"/>
-      <c r="L22" s="46" t="n"/>
+      <c r="L22" s="46" t="n">
+        <v>1</v>
+      </c>
       <c r="M22" s="43" t="n">
         <v>1</v>
       </c>
@@ -2601,18 +2637,56 @@
     </row>
     <row r="23" ht="18" customHeight="1" s="78">
       <c r="A23" s="51" t="n"/>
-      <c r="B23" s="44" t="n"/>
-      <c r="C23" s="45" t="n"/>
-      <c r="D23" s="45" t="n"/>
-      <c r="E23" s="46" t="n"/>
-      <c r="F23" s="46" t="n"/>
-      <c r="G23" s="46" t="n"/>
-      <c r="H23" s="46" t="n"/>
-      <c r="I23" s="46" t="n"/>
-      <c r="J23" s="46" t="n"/>
+      <c r="B23" s="44" t="inlineStr">
+        <is>
+          <t>6330490190</t>
+        </is>
+      </c>
+      <c r="C23" s="45" t="inlineStr">
+        <is>
+          <t>Sun Pharmaceutical Industries, Inc.</t>
+        </is>
+      </c>
+      <c r="D23" s="45" t="inlineStr">
+        <is>
+          <t>Fenofibrate</t>
+        </is>
+      </c>
+      <c r="E23" s="46" t="inlineStr">
+        <is>
+          <t>160 mg/1</t>
+        </is>
+      </c>
+      <c r="F23" s="46" t="inlineStr">
+        <is>
+          <t>TABLET, FILM COATED</t>
+        </is>
+      </c>
+      <c r="G23" s="46" t="inlineStr">
+        <is>
+          <t>MHC1672A</t>
+        </is>
+      </c>
+      <c r="H23" s="46" t="inlineStr">
+        <is>
+          <t>11/23/30</t>
+        </is>
+      </c>
+      <c r="I23" s="46" t="inlineStr">
+        <is>
+          <t>90 CT</t>
+        </is>
+      </c>
+      <c r="J23" s="46" t="n">
+        <v>24</v>
+      </c>
       <c r="K23" s="46" t="n"/>
-      <c r="L23" s="46" t="n"/>
-      <c r="M23" s="46" t="n"/>
+      <c r="L23" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" s="46" t="n">
+        <v>24</v>
+      </c>
       <c r="N23" s="21" t="n"/>
     </row>
     <row r="24" ht="18" customHeight="1" s="78">
@@ -2793,7 +2867,7 @@
         </is>
       </c>
       <c r="L34" s="109" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="N34" s="62" t="n"/>
       <c r="O34" s="91" t="n"/>

</xml_diff>

<commit_message>
fixed bugs in inventory and bugs in NDC lookup, Product tested by employees and extra bugs found
</commit_message>
<xml_diff>
--- a/docs/invoice.xlsx
+++ b/docs/invoice.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot;-&quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="31">
     <font>
       <name val="Arial"/>
       <color indexed="8"/>
@@ -193,12 +193,6 @@
     <font>
       <name val="Roboto"/>
       <b val="1"/>
-      <color indexed="8"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Roboto"/>
-      <b val="1"/>
       <color rgb="FF000000"/>
       <sz val="12"/>
     </font>
@@ -654,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -834,81 +828,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="32"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -918,31 +853,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="19" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="29" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="27" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="32"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2072,7 +2055,7 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:K10"/>
+      <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -2127,18 +2110,18 @@
     </row>
     <row r="3" ht="73" customHeight="1" s="78" thickBot="1">
       <c r="A3" s="7" t="n"/>
-      <c r="B3" s="77" t="inlineStr">
+      <c r="B3" s="114" t="inlineStr">
         <is>
           <t>Manufacturer Packaging Slip</t>
         </is>
       </c>
       <c r="K3" s="9" t="n"/>
-      <c r="L3" s="75" t="inlineStr">
+      <c r="L3" s="96" t="inlineStr">
         <is>
           <t>Quick Returns</t>
         </is>
       </c>
-      <c r="M3" s="81" t="n"/>
+      <c r="M3" s="97" t="n"/>
       <c r="N3" s="10" t="n"/>
     </row>
     <row r="4" ht="18" customHeight="1" s="78" thickBot="1">
@@ -2148,241 +2131,241 @@
           <t>DATE</t>
         </is>
       </c>
-      <c r="D4" s="103" t="n"/>
-      <c r="E4" s="104" t="n"/>
-      <c r="F4" s="104" t="n"/>
-      <c r="G4" s="104" t="n"/>
-      <c r="H4" s="105" t="n"/>
-      <c r="I4" s="97" t="n"/>
-      <c r="J4" s="97" t="n"/>
-      <c r="K4" s="97" t="n"/>
-      <c r="L4" s="112" t="inlineStr">
+      <c r="D4" s="82" t="n"/>
+      <c r="E4" s="83" t="n"/>
+      <c r="F4" s="83" t="n"/>
+      <c r="G4" s="83" t="n"/>
+      <c r="H4" s="84" t="n"/>
+      <c r="I4" s="91" t="n"/>
+      <c r="J4" s="91" t="n"/>
+      <c r="K4" s="91" t="n"/>
+      <c r="L4" s="108" t="inlineStr">
         <is>
           <t>INVOICE NO:</t>
         </is>
       </c>
-      <c r="M4" s="113" t="n"/>
+      <c r="M4" s="109" t="n"/>
       <c r="N4" s="11" t="n"/>
     </row>
     <row r="5" ht="18" customHeight="1" s="78" thickBot="1">
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="69" t="inlineStr">
         <is>
-          <t>02/20/2024</t>
-        </is>
-      </c>
-      <c r="D5" s="106" t="n"/>
-      <c r="E5" s="107" t="n"/>
-      <c r="F5" s="107" t="n"/>
-      <c r="G5" s="107" t="n"/>
-      <c r="H5" s="108" t="n"/>
-      <c r="I5" s="97" t="n"/>
-      <c r="J5" s="97" t="n"/>
-      <c r="K5" s="97" t="n"/>
-      <c r="L5" s="110" t="inlineStr">
-        <is>
-          <t>QR02202024AP101</t>
-        </is>
-      </c>
-      <c r="M5" s="111" t="n"/>
+          <t>02/23/2024</t>
+        </is>
+      </c>
+      <c r="D5" s="85" t="n"/>
+      <c r="E5" s="86" t="n"/>
+      <c r="F5" s="86" t="n"/>
+      <c r="G5" s="86" t="n"/>
+      <c r="H5" s="87" t="n"/>
+      <c r="I5" s="91" t="n"/>
+      <c r="J5" s="91" t="n"/>
+      <c r="K5" s="91" t="n"/>
+      <c r="L5" s="101" t="inlineStr">
+        <is>
+          <t>QR02232024AP301</t>
+        </is>
+      </c>
+      <c r="M5" s="102" t="n"/>
       <c r="N5" s="13" t="n"/>
     </row>
     <row r="6" ht="18" customHeight="1" s="78">
       <c r="A6" s="7" t="n"/>
       <c r="D6" s="12" t="n"/>
-      <c r="E6" s="98" t="n"/>
+      <c r="E6" s="94" t="n"/>
       <c r="N6" s="14" t="n"/>
     </row>
     <row r="7" ht="22.5" customHeight="1" s="78">
       <c r="A7" s="7" t="n"/>
       <c r="D7" s="12" t="n"/>
-      <c r="E7" s="102" t="n"/>
+      <c r="E7" s="105" t="n"/>
       <c r="N7" s="15" t="n"/>
     </row>
     <row r="8" ht="26.25" customHeight="1" s="78">
       <c r="A8" s="7" t="n"/>
-      <c r="B8" s="100" t="inlineStr">
+      <c r="B8" s="103" t="inlineStr">
         <is>
           <t>Account:</t>
         </is>
       </c>
-      <c r="C8" s="81" t="n"/>
-      <c r="D8" s="100" t="inlineStr">
-        <is>
-          <t>Wholesaler:</t>
-        </is>
-      </c>
-      <c r="E8" s="80" t="inlineStr">
-        <is>
-          <t>Issue Credit to:</t>
-        </is>
-      </c>
-      <c r="F8" s="81" t="n"/>
-      <c r="G8" s="81" t="n"/>
-      <c r="H8" s="99" t="n"/>
+      <c r="C8" s="97" t="n"/>
+      <c r="D8" s="103" t="inlineStr">
+        <is>
+          <t>Ship To:</t>
+        </is>
+      </c>
+      <c r="E8" s="115" t="inlineStr">
+        <is>
+          <t>Bill To:</t>
+        </is>
+      </c>
+      <c r="F8" s="97" t="n"/>
+      <c r="G8" s="97" t="n"/>
+      <c r="H8" s="98" t="n"/>
       <c r="L8" s="64" t="n"/>
       <c r="M8" s="64" t="n"/>
       <c r="N8" s="16" t="n"/>
     </row>
     <row r="9" ht="8" customHeight="1" s="78">
       <c r="A9" s="7" t="n"/>
-      <c r="B9" s="97" t="n"/>
-      <c r="D9" s="37" t="n"/>
-      <c r="E9" s="97" t="n"/>
-      <c r="H9" s="37" t="n"/>
-      <c r="I9" s="37" t="n"/>
-      <c r="J9" s="37" t="n"/>
-      <c r="K9" s="37" t="n"/>
-      <c r="L9" s="97" t="n"/>
-      <c r="M9" s="97" t="n"/>
+      <c r="B9" s="91" t="n"/>
+      <c r="D9" s="80" t="n"/>
+      <c r="E9" s="91" t="n"/>
+      <c r="H9" s="80" t="n"/>
+      <c r="I9" s="80" t="n"/>
+      <c r="J9" s="80" t="n"/>
+      <c r="K9" s="80" t="n"/>
+      <c r="L9" s="91" t="n"/>
+      <c r="M9" s="91" t="n"/>
       <c r="N9" s="17" t="n"/>
     </row>
     <row r="10" ht="35" customHeight="1" s="78">
       <c r="A10" s="50" t="n"/>
-      <c r="B10" s="114" t="inlineStr">
-        <is>
-          <t>AUTREY PHARMACY 1</t>
-        </is>
-      </c>
-      <c r="D10" s="115" t="inlineStr">
-        <is>
-          <t>KINARY</t>
-        </is>
-      </c>
-      <c r="E10" s="118" t="inlineStr">
-        <is>
-          <t>AUTREY PHARMACY 1</t>
-        </is>
-      </c>
-      <c r="H10" s="101" t="n"/>
+      <c r="B10" s="79" t="inlineStr">
+        <is>
+          <t>AUTREY PHARMACY 3</t>
+        </is>
+      </c>
+      <c r="D10" s="75" t="inlineStr">
+        <is>
+          <t>Lake Carmel PhaRxmacy</t>
+        </is>
+      </c>
+      <c r="E10" s="77" t="inlineStr">
+        <is>
+          <t>AUTREY PHARMACY 3</t>
+        </is>
+      </c>
+      <c r="H10" s="104" t="n"/>
       <c r="L10" s="12" t="n"/>
       <c r="M10" s="12" t="n"/>
       <c r="N10" s="18" t="n"/>
     </row>
     <row r="11" ht="18" customHeight="1" s="78">
       <c r="A11" s="50" t="n"/>
-      <c r="B11" s="114" t="inlineStr">
-        <is>
-          <t>1205 CENTRAL BLVD</t>
-        </is>
-      </c>
-      <c r="D11" s="115" t="inlineStr">
-        <is>
-          <t>152.35 TENTH AVE</t>
-        </is>
-      </c>
-      <c r="E11" s="118" t="inlineStr">
-        <is>
-          <t>1205 CENTRAL BLVD</t>
-        </is>
-      </c>
-      <c r="H11" s="79" t="n"/>
+      <c r="B11" s="79" t="inlineStr">
+        <is>
+          <t>800 E. ALTON GLOR BLVD, UNIT B</t>
+        </is>
+      </c>
+      <c r="D11" s="75" t="inlineStr">
+        <is>
+          <t>1205 Central Blvd,</t>
+        </is>
+      </c>
+      <c r="E11" s="77" t="inlineStr">
+        <is>
+          <t>800 E. ALTON GLOR BLVD, UNIT B</t>
+        </is>
+      </c>
+      <c r="H11" s="81" t="n"/>
       <c r="L11" s="12" t="n"/>
       <c r="M11" s="12" t="n"/>
       <c r="N11" s="18" t="n"/>
     </row>
     <row r="12" ht="18" customHeight="1" s="78">
       <c r="A12" s="50" t="n"/>
-      <c r="B12" s="114" t="inlineStr">
-        <is>
-          <t>BROWNSVILLE, TX, 78520</t>
-        </is>
-      </c>
-      <c r="D12" s="115" t="inlineStr">
-        <is>
-          <t>WHITESTONE, NY,11357</t>
-        </is>
-      </c>
-      <c r="E12" s="118" t="inlineStr">
-        <is>
-          <t>BROWNSVILLE, TX, 78520</t>
-        </is>
-      </c>
-      <c r="H12" s="79" t="n"/>
+      <c r="B12" s="79" t="inlineStr">
+        <is>
+          <t>BROWNSVILLE, TX, 78526</t>
+        </is>
+      </c>
+      <c r="D12" s="75" t="inlineStr">
+        <is>
+          <t>Brownsville, TX 78520</t>
+        </is>
+      </c>
+      <c r="E12" s="77" t="inlineStr">
+        <is>
+          <t>BROWNSVILLE, TX, 78526</t>
+        </is>
+      </c>
+      <c r="H12" s="81" t="n"/>
       <c r="L12" s="12" t="n"/>
       <c r="M12" s="12" t="n"/>
       <c r="N12" s="18" t="n"/>
     </row>
     <row r="13" ht="18" customHeight="1" s="78">
       <c r="A13" s="50" t="n"/>
-      <c r="B13" s="114" t="inlineStr">
+      <c r="B13" s="79" t="inlineStr">
         <is>
           <t>contact name</t>
         </is>
       </c>
-      <c r="D13" s="115" t="inlineStr">
+      <c r="D13" s="75" t="inlineStr">
         <is>
           <t xml:space="preserve">Account#: </t>
         </is>
       </c>
-      <c r="E13" s="118" t="inlineStr">
+      <c r="E13" s="77" t="inlineStr">
         <is>
           <t>contact name</t>
         </is>
       </c>
-      <c r="H13" s="79" t="n"/>
+      <c r="H13" s="81" t="n"/>
       <c r="L13" s="12" t="n"/>
       <c r="M13" s="12" t="n"/>
       <c r="N13" s="18" t="n"/>
     </row>
     <row r="14" ht="18" customHeight="1" s="78">
       <c r="A14" s="50" t="n"/>
-      <c r="B14" s="114" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Phone: 956-548-0801, fax: </t>
-        </is>
-      </c>
-      <c r="D14" s="118" t="inlineStr">
-        <is>
-          <t>Phone: 718-767-1234/ 888-527-6806</t>
-        </is>
-      </c>
-      <c r="E14" s="118" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Phone: 956-548-0801, fax: </t>
-        </is>
-      </c>
-      <c r="H14" s="83" t="n"/>
+      <c r="B14" s="79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phone: 956-525-7759, fax: </t>
+        </is>
+      </c>
+      <c r="D14" s="77" t="inlineStr">
+        <is>
+          <t>Phone: (956) 548-0801</t>
+        </is>
+      </c>
+      <c r="E14" s="77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phone: 956-525-7759, fax: </t>
+        </is>
+      </c>
+      <c r="H14" s="92" t="n"/>
       <c r="L14" s="12" t="n"/>
       <c r="M14" s="12" t="n"/>
       <c r="N14" s="18" t="n"/>
     </row>
     <row r="15" ht="18" customHeight="1" s="78">
       <c r="A15" s="50" t="n"/>
-      <c r="B15" s="114" t="inlineStr">
-        <is>
-          <t>DEA: FA3704358, Exp: 06/30/2023</t>
-        </is>
-      </c>
-      <c r="D15" s="118" t="inlineStr">
-        <is>
-          <t>DEA: RK0416900</t>
-        </is>
-      </c>
-      <c r="E15" s="118" t="inlineStr">
-        <is>
-          <t>DEA: FA3704358, Exp: 06/30/2023</t>
-        </is>
-      </c>
-      <c r="H15" s="83" t="n"/>
+      <c r="B15" s="79" t="inlineStr">
+        <is>
+          <t>DEA: FA5030010, Exp: 06/30/2023</t>
+        </is>
+      </c>
+      <c r="D15" s="77" t="inlineStr">
+        <is>
+          <t>DEA: 1233934230</t>
+        </is>
+      </c>
+      <c r="E15" s="77" t="inlineStr">
+        <is>
+          <t>DEA: FA5030010, Exp: 06/30/2023</t>
+        </is>
+      </c>
+      <c r="H15" s="92" t="n"/>
       <c r="L15" s="12" t="n"/>
       <c r="M15" s="12" t="n"/>
       <c r="N15" s="18" t="n"/>
     </row>
-    <row r="16" ht="18" customFormat="1" customHeight="1" s="37">
+    <row r="16" ht="18" customFormat="1" customHeight="1" s="80">
       <c r="A16" s="50" t="n"/>
-      <c r="B16" s="114" t="inlineStr">
+      <c r="B16" s="79" t="inlineStr">
         <is>
           <t>Authorized Classes: 2, 2N, 3, 3N, 4. 5</t>
         </is>
       </c>
-      <c r="D16" s="118" t="n"/>
-      <c r="E16" s="118" t="inlineStr">
+      <c r="D16" s="77" t="n"/>
+      <c r="E16" s="77" t="inlineStr">
         <is>
           <t>Authorized Classes: 2, 2N, 3, 3N, 4. 5</t>
         </is>
       </c>
-      <c r="H16" s="83" t="n"/>
+      <c r="H16" s="92" t="n"/>
       <c r="L16" s="12" t="n"/>
       <c r="M16" s="12" t="n"/>
       <c r="N16" s="18" t="n"/>
@@ -2390,23 +2373,23 @@
     <row r="17" ht="18" customHeight="1" s="78">
       <c r="A17" s="50" t="n"/>
       <c r="B17" s="12" t="n"/>
-      <c r="C17" s="96" t="n"/>
+      <c r="C17" s="112" t="n"/>
       <c r="N17" s="13" t="n"/>
     </row>
     <row r="18" ht="8" customHeight="1" s="78">
       <c r="A18" s="50" t="n"/>
-      <c r="B18" s="97" t="n"/>
-      <c r="C18" s="97" t="n"/>
-      <c r="D18" s="97" t="n"/>
-      <c r="E18" s="97" t="n"/>
-      <c r="F18" s="97" t="n"/>
-      <c r="G18" s="97" t="n"/>
-      <c r="H18" s="97" t="n"/>
-      <c r="I18" s="97" t="n"/>
-      <c r="J18" s="97" t="n"/>
-      <c r="K18" s="97" t="n"/>
-      <c r="L18" s="97" t="n"/>
-      <c r="M18" s="97" t="n"/>
+      <c r="B18" s="91" t="n"/>
+      <c r="C18" s="91" t="n"/>
+      <c r="D18" s="91" t="n"/>
+      <c r="E18" s="91" t="n"/>
+      <c r="F18" s="91" t="n"/>
+      <c r="G18" s="91" t="n"/>
+      <c r="H18" s="91" t="n"/>
+      <c r="I18" s="91" t="n"/>
+      <c r="J18" s="91" t="n"/>
+      <c r="K18" s="91" t="n"/>
+      <c r="L18" s="91" t="n"/>
+      <c r="M18" s="91" t="n"/>
       <c r="N18" s="17" t="n"/>
     </row>
     <row r="19" ht="25" customHeight="1" s="78">
@@ -2502,12 +2485,12 @@
       </c>
       <c r="G20" s="43" t="inlineStr">
         <is>
-          <t>RCY01AD6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H20" s="43" t="inlineStr">
         <is>
-          <t>12/23/31</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I20" s="43" t="inlineStr">
@@ -2515,12 +2498,16 @@
           <t>30 CT</t>
         </is>
       </c>
-      <c r="J20" s="43" t="n">
-        <v>1</v>
+      <c r="J20" s="43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="K20" s="43" t="n"/>
-      <c r="L20" s="43" t="n">
-        <v>1</v>
+      <c r="L20" s="43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="M20" s="43" t="n">
         <v>1</v>
@@ -2529,107 +2516,34 @@
     </row>
     <row r="21" ht="18" customHeight="1" s="78">
       <c r="A21" s="51" t="n"/>
-      <c r="B21" s="44" t="inlineStr">
-        <is>
-          <t>2315574603</t>
-        </is>
-      </c>
-      <c r="C21" s="45" t="inlineStr">
-        <is>
-          <t>Avet Pharmaceuticals Inc.</t>
-        </is>
-      </c>
-      <c r="D21" s="45" t="inlineStr">
-        <is>
-          <t>Rasagiline mesylate</t>
-        </is>
-      </c>
-      <c r="E21" s="46" t="inlineStr">
-        <is>
-          <t>.5 mg/1</t>
-        </is>
-      </c>
-      <c r="F21" s="46" t="inlineStr">
-        <is>
-          <t>TABLET</t>
-        </is>
-      </c>
-      <c r="G21" s="46" t="inlineStr">
-        <is>
-          <t>RCY01AD6</t>
-        </is>
-      </c>
-      <c r="H21" s="46" t="inlineStr">
-        <is>
-          <t>12/23/31</t>
-        </is>
-      </c>
-      <c r="I21" s="46" t="inlineStr">
-        <is>
-          <t>30 CT</t>
-        </is>
-      </c>
-      <c r="J21" s="46" t="n">
-        <v>1</v>
-      </c>
+      <c r="B21" s="44" t="n"/>
+      <c r="C21" s="45" t="n"/>
+      <c r="D21" s="45" t="n"/>
+      <c r="E21" s="46" t="n"/>
+      <c r="F21" s="46" t="n"/>
+      <c r="G21" s="46" t="n"/>
+      <c r="H21" s="46" t="n"/>
+      <c r="I21" s="46" t="n"/>
+      <c r="J21" s="46" t="n"/>
       <c r="K21" s="46" t="n"/>
-      <c r="L21" t="n">
-        <v>1</v>
-      </c>
       <c r="M21" s="46" t="n">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="N21" s="21" t="n"/>
     </row>
     <row r="22" ht="18" customHeight="1" s="78">
       <c r="A22" s="51" t="n"/>
-      <c r="B22" s="41" t="inlineStr">
-        <is>
-          <t>2315574603</t>
-        </is>
-      </c>
-      <c r="C22" s="42" t="inlineStr">
-        <is>
-          <t>Avet Pharmaceuticals Inc.</t>
-        </is>
-      </c>
-      <c r="D22" s="42" t="inlineStr">
-        <is>
-          <t>Rasagiline mesylate</t>
-        </is>
-      </c>
-      <c r="E22" s="43" t="inlineStr">
-        <is>
-          <t>.5 mg/1</t>
-        </is>
-      </c>
-      <c r="F22" s="43" t="inlineStr">
-        <is>
-          <t>TABLET</t>
-        </is>
-      </c>
-      <c r="G22" s="43" t="inlineStr">
-        <is>
-          <t>RCY01AD6</t>
-        </is>
-      </c>
-      <c r="H22" s="43" t="inlineStr">
-        <is>
-          <t>12/23/31</t>
-        </is>
-      </c>
-      <c r="I22" s="43" t="inlineStr">
-        <is>
-          <t>30 CT</t>
-        </is>
-      </c>
-      <c r="J22" s="43" t="n">
-        <v>1</v>
-      </c>
+      <c r="B22" s="41" t="n"/>
+      <c r="C22" s="42" t="n"/>
+      <c r="D22" s="42" t="n"/>
+      <c r="E22" s="43" t="n"/>
+      <c r="F22" s="43" t="n"/>
+      <c r="G22" s="43" t="n"/>
+      <c r="H22" s="43" t="n"/>
+      <c r="I22" s="43" t="n"/>
+      <c r="J22" s="43" t="n"/>
       <c r="K22" s="43" t="n"/>
-      <c r="L22" s="46" t="n">
-        <v>1</v>
-      </c>
+      <c r="L22" s="46" t="n"/>
       <c r="M22" s="43" t="n">
         <v>1</v>
       </c>
@@ -2637,55 +2551,19 @@
     </row>
     <row r="23" ht="18" customHeight="1" s="78">
       <c r="A23" s="51" t="n"/>
-      <c r="B23" s="44" t="inlineStr">
-        <is>
-          <t>6330490190</t>
-        </is>
-      </c>
-      <c r="C23" s="45" t="inlineStr">
-        <is>
-          <t>Sun Pharmaceutical Industries, Inc.</t>
-        </is>
-      </c>
-      <c r="D23" s="45" t="inlineStr">
-        <is>
-          <t>Fenofibrate</t>
-        </is>
-      </c>
-      <c r="E23" s="46" t="inlineStr">
-        <is>
-          <t>160 mg/1</t>
-        </is>
-      </c>
-      <c r="F23" s="46" t="inlineStr">
-        <is>
-          <t>TABLET, FILM COATED</t>
-        </is>
-      </c>
-      <c r="G23" s="46" t="inlineStr">
-        <is>
-          <t>MHC1672A</t>
-        </is>
-      </c>
-      <c r="H23" s="46" t="inlineStr">
-        <is>
-          <t>11/23/30</t>
-        </is>
-      </c>
-      <c r="I23" s="46" t="inlineStr">
-        <is>
-          <t>90 CT</t>
-        </is>
-      </c>
-      <c r="J23" s="46" t="n">
-        <v>24</v>
-      </c>
+      <c r="B23" s="44" t="n"/>
+      <c r="C23" s="45" t="n"/>
+      <c r="D23" s="45" t="n"/>
+      <c r="E23" s="46" t="n"/>
+      <c r="F23" s="46" t="n"/>
+      <c r="G23" s="46" t="n"/>
+      <c r="H23" s="46" t="n"/>
+      <c r="I23" s="46" t="n"/>
+      <c r="J23" s="46" t="n"/>
       <c r="K23" s="46" t="n"/>
-      <c r="L23" s="46" t="n">
-        <v>1</v>
-      </c>
+      <c r="L23" s="46" t="n"/>
       <c r="M23" s="46" t="n">
-        <v>24</v>
+        <v>175</v>
       </c>
       <c r="N23" s="21" t="n"/>
     </row>
@@ -2702,7 +2580,9 @@
       <c r="J24" s="43" t="n"/>
       <c r="K24" s="43" t="n"/>
       <c r="L24" s="43" t="n"/>
-      <c r="M24" s="43" t="n"/>
+      <c r="M24" s="43" t="n">
+        <v>225</v>
+      </c>
       <c r="N24" s="21" t="n"/>
     </row>
     <row r="25" ht="18" customHeight="1" s="78">
@@ -2785,7 +2665,7 @@
       <c r="M29" s="46" t="n"/>
       <c r="N29" s="21" t="n"/>
     </row>
-    <row r="30" ht="18" customFormat="1" customHeight="1" s="37">
+    <row r="30" ht="18" customFormat="1" customHeight="1" s="80">
       <c r="A30" s="51" t="n"/>
       <c r="B30" s="41" t="n"/>
       <c r="C30" s="42" t="n"/>
@@ -2801,7 +2681,7 @@
       <c r="M30" s="43" t="n"/>
       <c r="N30" s="21" t="n"/>
     </row>
-    <row r="31" ht="18" customFormat="1" customHeight="1" s="37">
+    <row r="31" ht="18" customFormat="1" customHeight="1" s="80">
       <c r="A31" s="51" t="n"/>
       <c r="B31" s="44" t="n"/>
       <c r="C31" s="45" t="n"/>
@@ -2848,7 +2728,7 @@
       <c r="L33" s="24" t="n"/>
       <c r="M33" s="38" t="n"/>
       <c r="N33" s="63" t="n"/>
-      <c r="O33" s="91" t="n"/>
+      <c r="O33" s="90" t="n"/>
     </row>
     <row r="34" ht="33.75" customHeight="1" s="78">
       <c r="A34" s="50" t="n"/>
@@ -2866,11 +2746,11 @@
           <t>Total:</t>
         </is>
       </c>
-      <c r="L34" s="109" t="n">
-        <v>27</v>
+      <c r="L34" s="113" t="n">
+        <v>1</v>
       </c>
       <c r="N34" s="62" t="n"/>
-      <c r="O34" s="91" t="n"/>
+      <c r="O34" s="90" t="n"/>
     </row>
     <row r="35" ht="9.75" customHeight="1" s="78">
       <c r="A35" s="50" t="n"/>
@@ -2887,21 +2767,21 @@
       <c r="L35" s="26" t="n"/>
       <c r="M35" s="26" t="n"/>
       <c r="N35" s="26" t="n"/>
-      <c r="O35" s="91" t="n"/>
+      <c r="O35" s="90" t="n"/>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="78">
       <c r="A36" s="50" t="n"/>
-      <c r="B36" s="88" t="n"/>
+      <c r="B36" s="110" t="n"/>
       <c r="N36" s="27" t="n"/>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="78">
       <c r="A37" s="50" t="n"/>
-      <c r="B37" s="95" t="n"/>
+      <c r="B37" s="99" t="n"/>
       <c r="N37" s="28" t="n"/>
     </row>
     <row r="38" ht="21" customHeight="1" s="78">
       <c r="A38" s="52" t="n"/>
-      <c r="B38" s="94" t="n"/>
+      <c r="B38" s="95" t="n"/>
       <c r="N38" s="29" t="n"/>
     </row>
     <row r="39" ht="8" customHeight="1" s="78">
@@ -2921,9 +2801,9 @@
       <c r="N39" s="47" t="n"/>
     </row>
     <row r="40" ht="24" customHeight="1" s="78">
-      <c r="A40" s="91" t="n"/>
+      <c r="A40" s="90" t="n"/>
       <c r="C40" s="58" t="n"/>
-      <c r="D40" s="82" t="inlineStr">
+      <c r="D40" s="93" t="inlineStr">
         <is>
           <t>Return instructions:</t>
         </is>
@@ -2932,10 +2812,10 @@
       <c r="J40" s="59" t="n"/>
       <c r="K40" s="59" t="n"/>
       <c r="L40" s="60" t="n"/>
-      <c r="N40" s="90" t="n"/>
+      <c r="N40" s="89" t="n"/>
     </row>
     <row r="41" ht="15" customHeight="1" s="78">
-      <c r="A41" s="91" t="n"/>
+      <c r="A41" s="90" t="n"/>
       <c r="C41" s="58" t="n"/>
       <c r="D41" s="59" t="n"/>
       <c r="E41" s="59" t="n"/>
@@ -2946,59 +2826,59 @@
       <c r="J41" s="59" t="n"/>
       <c r="K41" s="59" t="n"/>
       <c r="L41" s="60" t="n"/>
-      <c r="N41" s="90" t="n"/>
+      <c r="N41" s="89" t="n"/>
     </row>
     <row r="42" ht="17" customHeight="1" s="78">
-      <c r="A42" s="91" t="n"/>
-      <c r="C42" s="89" t="inlineStr">
+      <c r="A42" s="90" t="n"/>
+      <c r="C42" s="88" t="inlineStr">
         <is>
           <t>1. Email the Packing Slip to Customer Service via email to https://returns.healthcare.inmar.com request a Return Authorization (RGA).</t>
         </is>
       </c>
-      <c r="L42" s="90" t="n"/>
-      <c r="N42" s="90" t="n"/>
+      <c r="L42" s="89" t="n"/>
+      <c r="N42" s="89" t="n"/>
     </row>
     <row r="43" ht="3" customHeight="1" s="78">
-      <c r="A43" s="91" t="n"/>
-      <c r="C43" s="91" t="n"/>
-      <c r="L43" s="90" t="n"/>
-      <c r="N43" s="90" t="n"/>
+      <c r="A43" s="90" t="n"/>
+      <c r="C43" s="90" t="n"/>
+      <c r="L43" s="89" t="n"/>
+      <c r="N43" s="89" t="n"/>
     </row>
     <row r="44" ht="15" customHeight="1" s="78">
-      <c r="A44" s="91" t="n"/>
-      <c r="C44" s="89" t="inlineStr">
+      <c r="A44" s="90" t="n"/>
+      <c r="C44" s="88" t="inlineStr">
         <is>
           <t>2. Alternatively, you can create an RGA by logging in to https://clsnetlink.com</t>
         </is>
       </c>
-      <c r="L44" s="90" t="n"/>
-      <c r="N44" s="90" t="n"/>
+      <c r="L44" s="89" t="n"/>
+      <c r="N44" s="89" t="n"/>
     </row>
     <row r="45" ht="5" customHeight="1" s="78">
-      <c r="A45" s="91" t="n"/>
-      <c r="C45" s="91" t="n"/>
-      <c r="L45" s="90" t="n"/>
-      <c r="N45" s="90" t="n"/>
+      <c r="A45" s="90" t="n"/>
+      <c r="C45" s="90" t="n"/>
+      <c r="L45" s="89" t="n"/>
+      <c r="N45" s="89" t="n"/>
     </row>
     <row r="46" ht="31" customHeight="1" s="78">
-      <c r="A46" s="91" t="n"/>
-      <c r="C46" s="89" t="inlineStr">
+      <c r="A46" s="90" t="n"/>
+      <c r="C46" s="88" t="inlineStr">
         <is>
           <t>3. Upon receiving the Returned Goods Authorization Form (RGA), include the RGA along with the Packing Slip and ship the outdated products to the following address:</t>
         </is>
       </c>
-      <c r="L46" s="90" t="n"/>
-      <c r="N46" s="90" t="n"/>
+      <c r="L46" s="89" t="n"/>
+      <c r="N46" s="89" t="n"/>
     </row>
     <row r="47" ht="4" customHeight="1" s="78">
-      <c r="A47" s="91" t="n"/>
-      <c r="C47" s="91" t="n"/>
-      <c r="L47" s="90" t="n"/>
-      <c r="N47" s="90" t="n"/>
+      <c r="A47" s="90" t="n"/>
+      <c r="C47" s="90" t="n"/>
+      <c r="L47" s="89" t="n"/>
+      <c r="N47" s="89" t="n"/>
     </row>
     <row r="48" ht="18" customHeight="1" s="78">
-      <c r="A48" s="91" t="n"/>
-      <c r="C48" s="93" t="inlineStr">
+      <c r="A48" s="90" t="n"/>
+      <c r="C48" s="111" t="inlineStr">
         <is>
           <t>INMAR Pharmaceutical Services</t>
         </is>
@@ -3011,11 +2891,11 @@
       <c r="J48" s="59" t="n"/>
       <c r="K48" s="59" t="n"/>
       <c r="L48" s="60" t="n"/>
-      <c r="N48" s="90" t="n"/>
+      <c r="N48" s="89" t="n"/>
     </row>
     <row r="49" ht="17" customHeight="1" s="78">
-      <c r="A49" s="91" t="n"/>
-      <c r="C49" s="92" t="inlineStr">
+      <c r="A49" s="90" t="n"/>
+      <c r="C49" s="100" t="inlineStr">
         <is>
           <t>4332 Empire Road</t>
         </is>
@@ -3028,11 +2908,11 @@
       <c r="J49" s="59" t="n"/>
       <c r="K49" s="59" t="n"/>
       <c r="L49" s="60" t="n"/>
-      <c r="N49" s="90" t="n"/>
+      <c r="N49" s="89" t="n"/>
     </row>
     <row r="50" ht="18" customHeight="1" s="78">
-      <c r="A50" s="91" t="n"/>
-      <c r="C50" s="92" t="inlineStr">
+      <c r="A50" s="90" t="n"/>
+      <c r="C50" s="100" t="inlineStr">
         <is>
           <t>Fort Worth, TX 76155</t>
         </is>
@@ -3045,10 +2925,10 @@
       <c r="J50" s="59" t="n"/>
       <c r="K50" s="59" t="n"/>
       <c r="L50" s="60" t="n"/>
-      <c r="N50" s="90" t="n"/>
+      <c r="N50" s="89" t="n"/>
     </row>
     <row r="51" hidden="1" ht="18" customHeight="1" s="78">
-      <c r="A51" s="91" t="n"/>
+      <c r="A51" s="90" t="n"/>
       <c r="C51" s="58" t="n"/>
       <c r="D51" s="59" t="n"/>
       <c r="E51" s="59" t="n"/>
@@ -3059,26 +2939,26 @@
       <c r="J51" s="59" t="n"/>
       <c r="K51" s="59" t="n"/>
       <c r="L51" s="60" t="n"/>
-      <c r="N51" s="90" t="n"/>
+      <c r="N51" s="89" t="n"/>
     </row>
     <row r="52" ht="15" customHeight="1" s="78">
-      <c r="A52" s="91" t="n"/>
-      <c r="C52" s="84" t="inlineStr">
+      <c r="A52" s="90" t="n"/>
+      <c r="C52" s="106" t="inlineStr">
         <is>
           <t>Please DO NOT mix products from multiple debit memos/packing slips in one shipment. In case of any questions, please contact INMAR customer service at 1-800-967-5952</t>
         </is>
       </c>
-      <c r="L52" s="90" t="n"/>
-      <c r="N52" s="90" t="n"/>
-    </row>
-    <row r="53" ht="25" customFormat="1" customHeight="1" s="117">
+      <c r="L52" s="89" t="n"/>
+      <c r="N52" s="89" t="n"/>
+    </row>
+    <row r="53" ht="25" customFormat="1" customHeight="1" s="107">
       <c r="A53" s="72" t="n"/>
-      <c r="C53" s="91" t="n"/>
-      <c r="L53" s="90" t="n"/>
+      <c r="C53" s="90" t="n"/>
+      <c r="L53" s="89" t="n"/>
       <c r="N53" s="74" t="n"/>
     </row>
     <row r="54" ht="15" customHeight="1" s="78">
-      <c r="A54" s="91" t="n"/>
+      <c r="A54" s="90" t="n"/>
       <c r="C54" s="65" t="n"/>
       <c r="D54" s="66" t="n"/>
       <c r="E54" s="66" t="n"/>
@@ -3089,15 +2969,15 @@
       <c r="J54" s="66" t="n"/>
       <c r="K54" s="66" t="n"/>
       <c r="L54" s="67" t="n"/>
-      <c r="N54" s="90" t="n"/>
+      <c r="N54" s="89" t="n"/>
     </row>
     <row r="55" ht="15" customHeight="1" s="78">
-      <c r="A55" s="91" t="n"/>
-      <c r="N55" s="90" t="n"/>
+      <c r="A55" s="90" t="n"/>
+      <c r="N55" s="89" t="n"/>
     </row>
     <row r="56" ht="15" customHeight="1" s="78">
-      <c r="A56" s="91" t="n"/>
-      <c r="N56" s="90" t="n"/>
+      <c r="A56" s="90" t="n"/>
+      <c r="N56" s="89" t="n"/>
     </row>
     <row r="57" ht="15.75" customHeight="1" s="78">
       <c r="A57" s="53" t="n"/>
@@ -3130,10 +3010,10 @@
     <mergeCell ref="D40:H40"/>
     <mergeCell ref="E6:M6"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="C44:L45"/>
     <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B38:M38"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="H8:K8"/>
@@ -3141,8 +3021,8 @@
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="C46:L47"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="B13:C13"/>

</xml_diff>